<commit_message>
add to control vocab lookup
</commit_message>
<xml_diff>
--- a/data-raw/control_vocab_mapping.xlsx
+++ b/data-raw/control_vocab_mapping.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wb499754\OneDrive - WBG\my_packages\mdlibtoddh\data-raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wb523589\Programs\mdlibtoddh\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1367" uniqueCount="868">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1369" uniqueCount="869">
   <si>
     <t>microdata_category</t>
   </si>
@@ -2641,6 +2641,9 @@
   </si>
   <si>
     <t>malaria indicator survey</t>
+  </si>
+  <si>
+    <t>Sample survey data[ssd]</t>
   </si>
 </sst>
 </file>
@@ -6683,11 +6686,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C171"/>
+  <dimension ref="A1:C172"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A153" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B180" sqref="B180"/>
+      <pane ySplit="1" topLeftCell="A144" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B174" sqref="B174"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8465,6 +8468,14 @@
       </c>
       <c r="B171" s="2" t="s">
         <v>768</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A172" t="s">
+        <v>868</v>
+      </c>
+      <c r="B172" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update controlled vocab lookup
</commit_message>
<xml_diff>
--- a/data-raw/control_vocab_mapping.xlsx
+++ b/data-raw/control_vocab_mapping.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="9870" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="9870" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="dataClassification" sheetId="1" r:id="rId1"/>
@@ -3338,10 +3338,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C43"/>
+  <dimension ref="A1:C44"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3797,6 +3797,14 @@
         <v>806</v>
       </c>
       <c r="B43" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>868</v>
+      </c>
+      <c r="B44" t="s">
         <v>14</v>
       </c>
     </row>
@@ -6686,11 +6694,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C172"/>
+  <dimension ref="A1:C171"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A144" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B174" sqref="B174"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A150" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A172" sqref="A172:C172"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8468,14 +8476,6 @@
       </c>
       <c r="B171" s="2" t="s">
         <v>768</v>
-      </c>
-    </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A172" t="s">
-        <v>868</v>
-      </c>
-      <c r="B172" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed lookup with data collection and Eswatini
</commit_message>
<xml_diff>
--- a/data-raw/control_vocab_mapping.xlsx
+++ b/data-raw/control_vocab_mapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WB525812\cmder\Git Repos\mdlibtoddh\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{F37F90E9-5273-436F-8A34-4C8BB65A8E19}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{9667F295-8439-44D7-91B6-B7DCA654A025}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="10770" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="10770" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dataClassification" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1400" uniqueCount="882">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1404" uniqueCount="883">
   <si>
     <t>microdata_category</t>
   </si>
@@ -2683,7 +2683,10 @@
     <t>Multiple Indicator Cluster Survey - Round 6 [hh/mics-6]</t>
   </si>
   <si>
-    <t>Other Household Survey [hh/oth]</t>
+    <t>Other[oth]</t>
+  </si>
+  <si>
+    <t>Kingdom of Eswatini</t>
   </si>
 </sst>
 </file>
@@ -3875,10 +3878,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:C93"/>
+  <dimension ref="A1:C94"/>
   <sheetViews>
-    <sheetView topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="B94" sqref="B94"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F73" sqref="F73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4868,6 +4871,17 @@
         <v>877</v>
       </c>
       <c r="B93" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>881</v>
+      </c>
+      <c r="B94" t="s">
+        <v>25</v>
+      </c>
+      <c r="C94" t="s">
         <v>25</v>
       </c>
     </row>
@@ -4914,11 +4928,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:B232"/>
+  <dimension ref="A1:B233"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A182" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B207" sqref="B207"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A91" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J95" sqref="J95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5793,223 +5807,223 @@
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>395</v>
+        <v>882</v>
       </c>
       <c r="B109" t="s">
-        <v>575</v>
+        <v>878</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>349</v>
+        <v>395</v>
       </c>
       <c r="B110" t="s">
-        <v>536</v>
+        <v>575</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>265</v>
+        <v>349</v>
       </c>
       <c r="B111" t="s">
-        <v>454</v>
+        <v>536</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>350</v>
+        <v>265</v>
       </c>
       <c r="B112" t="s">
-        <v>537</v>
+        <v>454</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>264</v>
+        <v>350</v>
       </c>
       <c r="B113" t="s">
-        <v>453</v>
+        <v>537</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>201</v>
+        <v>264</v>
       </c>
       <c r="B114" t="s">
-        <v>47</v>
+        <v>453</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>374</v>
+        <v>201</v>
       </c>
       <c r="B115" t="s">
-        <v>559</v>
+        <v>47</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>284</v>
+        <v>374</v>
       </c>
       <c r="B116" t="s">
-        <v>472</v>
+        <v>559</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>351</v>
+        <v>284</v>
       </c>
       <c r="B117" t="s">
-        <v>538</v>
+        <v>472</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>283</v>
+        <v>351</v>
       </c>
       <c r="B118" t="s">
-        <v>471</v>
+        <v>538</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>227</v>
+        <v>283</v>
       </c>
       <c r="B119" t="s">
-        <v>416</v>
+        <v>471</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>382</v>
+        <v>227</v>
       </c>
       <c r="B120" t="s">
-        <v>567</v>
+        <v>416</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>378</v>
+        <v>382</v>
       </c>
       <c r="B121" t="s">
-        <v>563</v>
+        <v>567</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>282</v>
+        <v>378</v>
       </c>
       <c r="B122" t="s">
-        <v>470</v>
+        <v>563</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>352</v>
+        <v>282</v>
       </c>
       <c r="B123" t="s">
-        <v>539</v>
+        <v>470</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>285</v>
+        <v>352</v>
       </c>
       <c r="B124" t="s">
-        <v>473</v>
+        <v>539</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>202</v>
+        <v>285</v>
       </c>
       <c r="B125" t="s">
-        <v>48</v>
+        <v>473</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>297</v>
+        <v>202</v>
       </c>
       <c r="B126" t="s">
-        <v>484</v>
+        <v>48</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>316</v>
+        <v>297</v>
       </c>
       <c r="B127" t="s">
-        <v>503</v>
+        <v>484</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>299</v>
+        <v>316</v>
       </c>
       <c r="B128" t="s">
-        <v>486</v>
+        <v>503</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>203</v>
+        <v>299</v>
       </c>
       <c r="B129" t="s">
-        <v>49</v>
+        <v>486</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>353</v>
+        <v>203</v>
       </c>
       <c r="B130" t="s">
-        <v>540</v>
+        <v>49</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>309</v>
+        <v>353</v>
       </c>
       <c r="B131" t="s">
-        <v>496</v>
+        <v>540</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="B132" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="B133" t="s">
-        <v>500</v>
+        <v>495</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>246</v>
+        <v>313</v>
       </c>
       <c r="B134" t="s">
-        <v>435</v>
+        <v>500</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>384</v>
+        <v>246</v>
       </c>
       <c r="B135" t="s">
-        <v>568</v>
+        <v>435</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>798</v>
+        <v>384</v>
       </c>
       <c r="B136" t="s">
         <v>568</v>
@@ -6017,303 +6031,303 @@
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>269</v>
+        <v>798</v>
       </c>
       <c r="B137" t="s">
-        <v>458</v>
+        <v>568</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>399</v>
+        <v>269</v>
       </c>
       <c r="B138" t="s">
-        <v>576</v>
+        <v>458</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>204</v>
+        <v>399</v>
       </c>
       <c r="B139" t="s">
-        <v>50</v>
+        <v>576</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="B140" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>393</v>
+        <v>210</v>
       </c>
       <c r="B141" t="s">
-        <v>836</v>
+        <v>55</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>310</v>
+        <v>393</v>
       </c>
       <c r="B142" t="s">
-        <v>497</v>
+        <v>836</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>205</v>
+        <v>310</v>
       </c>
       <c r="B143" t="s">
-        <v>51</v>
+        <v>497</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>314</v>
+        <v>205</v>
       </c>
       <c r="B144" t="s">
-        <v>501</v>
+        <v>51</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>206</v>
+        <v>314</v>
       </c>
       <c r="B145" t="s">
-        <v>52</v>
+        <v>501</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>386</v>
+        <v>206</v>
       </c>
       <c r="B146" t="s">
-        <v>569</v>
+        <v>52</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>230</v>
+        <v>386</v>
       </c>
       <c r="B147" t="s">
-        <v>419</v>
+        <v>569</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>354</v>
+        <v>230</v>
       </c>
       <c r="B148" t="s">
-        <v>541</v>
+        <v>419</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B149" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>247</v>
+        <v>355</v>
       </c>
       <c r="B150" t="s">
-        <v>436</v>
+        <v>542</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>188</v>
+        <v>247</v>
       </c>
       <c r="B151" t="s">
-        <v>36</v>
+        <v>436</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>298</v>
+        <v>188</v>
       </c>
       <c r="B152" t="s">
-        <v>485</v>
+        <v>36</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>385</v>
+        <v>298</v>
       </c>
       <c r="B153" t="s">
-        <v>859</v>
+        <v>485</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>379</v>
+        <v>385</v>
       </c>
       <c r="B154" t="s">
-        <v>564</v>
+        <v>859</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>356</v>
+        <v>379</v>
       </c>
       <c r="B155" t="s">
-        <v>543</v>
+        <v>564</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>229</v>
+        <v>356</v>
       </c>
       <c r="B156" t="s">
-        <v>418</v>
+        <v>543</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>387</v>
+        <v>229</v>
       </c>
       <c r="B157" t="s">
-        <v>570</v>
+        <v>418</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>248</v>
+        <v>387</v>
       </c>
       <c r="B158" t="s">
-        <v>437</v>
+        <v>570</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>197</v>
+        <v>248</v>
       </c>
       <c r="B159" t="s">
-        <v>43</v>
+        <v>437</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>249</v>
+        <v>197</v>
       </c>
       <c r="B160" t="s">
-        <v>438</v>
+        <v>43</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>196</v>
+        <v>249</v>
       </c>
       <c r="B161" t="s">
-        <v>42</v>
+        <v>438</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>287</v>
+        <v>196</v>
       </c>
       <c r="B162" t="s">
-        <v>475</v>
+        <v>42</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>266</v>
+        <v>287</v>
       </c>
       <c r="B163" t="s">
-        <v>455</v>
+        <v>475</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>357</v>
+        <v>266</v>
       </c>
       <c r="B164" t="s">
-        <v>544</v>
+        <v>455</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>401</v>
+        <v>357</v>
       </c>
       <c r="B165" t="s">
-        <v>577</v>
+        <v>544</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>358</v>
+        <v>401</v>
       </c>
       <c r="B166" t="s">
-        <v>545</v>
+        <v>577</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>191</v>
+        <v>358</v>
       </c>
       <c r="B167" t="s">
-        <v>63</v>
+        <v>545</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>273</v>
+        <v>191</v>
       </c>
       <c r="B168" t="s">
-        <v>462</v>
+        <v>63</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>294</v>
+        <v>273</v>
       </c>
       <c r="B169" t="s">
-        <v>481</v>
+        <v>462</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>193</v>
+        <v>294</v>
       </c>
       <c r="B170" t="s">
-        <v>40</v>
+        <v>481</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>295</v>
+        <v>193</v>
       </c>
       <c r="B171" t="s">
-        <v>482</v>
+        <v>40</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>380</v>
+        <v>295</v>
       </c>
       <c r="B172" t="s">
-        <v>565</v>
+        <v>482</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>396</v>
+        <v>380</v>
       </c>
       <c r="B173" t="s">
-        <v>492</v>
+        <v>565</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>305</v>
+        <v>396</v>
       </c>
       <c r="B174" t="s">
         <v>492</v>
@@ -6321,7 +6335,7 @@
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>404</v>
+        <v>305</v>
       </c>
       <c r="B175" t="s">
         <v>492</v>
@@ -6329,23 +6343,23 @@
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>359</v>
+        <v>404</v>
       </c>
       <c r="B176" t="s">
-        <v>546</v>
+        <v>492</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>194</v>
+        <v>359</v>
       </c>
       <c r="B177" t="s">
-        <v>41</v>
+        <v>546</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>870</v>
+        <v>194</v>
       </c>
       <c r="B178" t="s">
         <v>41</v>
@@ -6353,7 +6367,7 @@
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="B179" t="s">
         <v>41</v>
@@ -6361,135 +6375,135 @@
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>209</v>
+        <v>871</v>
       </c>
       <c r="B180" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B181" t="s">
-        <v>579</v>
+        <v>54</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>296</v>
+        <v>208</v>
       </c>
       <c r="B182" t="s">
-        <v>483</v>
+        <v>579</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>190</v>
+        <v>296</v>
       </c>
       <c r="B183" t="s">
-        <v>38</v>
+        <v>483</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>360</v>
+        <v>190</v>
       </c>
       <c r="B184" t="s">
-        <v>547</v>
+        <v>38</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="B185" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B186" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>306</v>
+        <v>363</v>
       </c>
       <c r="B187" t="s">
-        <v>493</v>
+        <v>550</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>361</v>
+        <v>306</v>
       </c>
       <c r="B188" t="s">
-        <v>548</v>
+        <v>493</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>200</v>
+        <v>361</v>
       </c>
       <c r="B189" t="s">
-        <v>46</v>
+        <v>548</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>304</v>
+        <v>200</v>
       </c>
       <c r="B190" t="s">
-        <v>491</v>
+        <v>46</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>338</v>
+        <v>304</v>
       </c>
       <c r="B191" t="s">
-        <v>525</v>
+        <v>491</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>293</v>
+        <v>338</v>
       </c>
       <c r="B192" t="s">
-        <v>480</v>
+        <v>525</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>259</v>
+        <v>293</v>
       </c>
       <c r="B193" t="s">
-        <v>448</v>
+        <v>480</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="B194" t="s">
-        <v>444</v>
+        <v>448</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>398</v>
+        <v>255</v>
       </c>
       <c r="B195" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>258</v>
+        <v>398</v>
       </c>
       <c r="B196" t="s">
         <v>447</v>
@@ -6497,63 +6511,63 @@
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>292</v>
+        <v>258</v>
       </c>
       <c r="B197" t="s">
-        <v>479</v>
+        <v>447</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>251</v>
+        <v>292</v>
       </c>
       <c r="B198" t="s">
-        <v>440</v>
+        <v>479</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>291</v>
+        <v>251</v>
       </c>
       <c r="B199" t="s">
-        <v>878</v>
+        <v>440</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>364</v>
+        <v>291</v>
       </c>
       <c r="B200" t="s">
-        <v>551</v>
+        <v>878</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>381</v>
+        <v>364</v>
       </c>
       <c r="B201" t="s">
-        <v>566</v>
+        <v>551</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>365</v>
+        <v>381</v>
       </c>
       <c r="B202" t="s">
-        <v>552</v>
+        <v>566</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>879</v>
+        <v>365</v>
       </c>
       <c r="B203" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>366</v>
+        <v>879</v>
       </c>
       <c r="B204" t="s">
         <v>553</v>
@@ -6561,167 +6575,167 @@
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>198</v>
+        <v>366</v>
       </c>
       <c r="B205" t="s">
-        <v>44</v>
+        <v>553</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>187</v>
+        <v>198</v>
       </c>
       <c r="B206" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>222</v>
+        <v>187</v>
       </c>
       <c r="B207" t="s">
-        <v>411</v>
+        <v>35</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>326</v>
+        <v>222</v>
       </c>
       <c r="B208" t="s">
-        <v>513</v>
+        <v>411</v>
       </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>302</v>
+        <v>326</v>
       </c>
       <c r="B209" t="s">
-        <v>489</v>
+        <v>513</v>
       </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>290</v>
+        <v>302</v>
       </c>
       <c r="B210" t="s">
-        <v>478</v>
+        <v>489</v>
       </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>254</v>
+        <v>290</v>
       </c>
       <c r="B211" t="s">
-        <v>443</v>
+        <v>478</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>317</v>
+        <v>254</v>
       </c>
       <c r="B212" t="s">
-        <v>504</v>
+        <v>443</v>
       </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>307</v>
+        <v>317</v>
       </c>
       <c r="B213" t="s">
-        <v>494</v>
+        <v>504</v>
       </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>301</v>
+        <v>307</v>
       </c>
       <c r="B214" t="s">
-        <v>488</v>
+        <v>494</v>
       </c>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>388</v>
+        <v>301</v>
       </c>
       <c r="B215" t="s">
-        <v>571</v>
+        <v>488</v>
       </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>189</v>
+        <v>388</v>
       </c>
       <c r="B216" t="s">
-        <v>37</v>
+        <v>571</v>
       </c>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>270</v>
+        <v>189</v>
       </c>
       <c r="B217" t="s">
-        <v>459</v>
+        <v>37</v>
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>328</v>
+        <v>270</v>
       </c>
       <c r="B218" t="s">
-        <v>515</v>
+        <v>459</v>
       </c>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>342</v>
+        <v>328</v>
       </c>
       <c r="B219" t="s">
-        <v>529</v>
+        <v>515</v>
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>367</v>
+        <v>342</v>
       </c>
       <c r="B220" t="s">
-        <v>554</v>
+        <v>529</v>
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
-        <v>252</v>
+        <v>367</v>
       </c>
       <c r="B221" t="s">
-        <v>441</v>
+        <v>554</v>
       </c>
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>327</v>
+        <v>252</v>
       </c>
       <c r="B222" t="s">
-        <v>514</v>
+        <v>441</v>
       </c>
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>192</v>
+        <v>327</v>
       </c>
       <c r="B223" t="s">
-        <v>39</v>
+        <v>514</v>
       </c>
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>394</v>
+        <v>192</v>
       </c>
       <c r="B224" t="s">
-        <v>832</v>
+        <v>39</v>
       </c>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>195</v>
+        <v>394</v>
       </c>
       <c r="B225" t="s">
         <v>832</v>
@@ -6729,15 +6743,15 @@
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>811</v>
+        <v>195</v>
       </c>
       <c r="B226" t="s">
-        <v>45</v>
+        <v>832</v>
       </c>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>199</v>
+        <v>811</v>
       </c>
       <c r="B227" t="s">
         <v>45</v>
@@ -6745,72 +6759,80 @@
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
-        <v>289</v>
+        <v>199</v>
       </c>
       <c r="B228" t="s">
-        <v>477</v>
+        <v>45</v>
       </c>
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
-        <v>214</v>
+        <v>289</v>
       </c>
       <c r="B229" t="s">
-        <v>58</v>
+        <v>477</v>
       </c>
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="B230" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
-        <v>207</v>
+        <v>212</v>
       </c>
       <c r="B231" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
+        <v>207</v>
+      </c>
+      <c r="B232" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="233" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A233" t="s">
         <v>303</v>
       </c>
-      <c r="B232" t="s">
+      <c r="B233" t="s">
         <v>490</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:B1" xr:uid="{00000000-0009-0000-0000-000004000000}">
-    <sortState ref="A2:B229">
+    <sortState ref="A2:B230">
       <sortCondition ref="A1"/>
     </sortState>
   </autoFilter>
   <sortState ref="A2:B35">
     <sortCondition ref="A2:A35"/>
   </sortState>
-  <conditionalFormatting sqref="A233:A1048576 A1:A53 A137:A178 A227:A231 A55:A135 A180:A225">
+  <conditionalFormatting sqref="A234:A1048576 A1:A53 A138:A179 A228:A232 A55:A136 A181:A226">
     <cfRule type="duplicateValues" dxfId="7" priority="8"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B232">
+  <conditionalFormatting sqref="B233">
     <cfRule type="duplicateValues" dxfId="6" priority="7"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A232">
+  <conditionalFormatting sqref="A233">
     <cfRule type="duplicateValues" dxfId="5" priority="6"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A136">
+  <conditionalFormatting sqref="A137">
     <cfRule type="duplicateValues" dxfId="4" priority="5"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A226">
+  <conditionalFormatting sqref="A227">
     <cfRule type="duplicateValues" dxfId="3" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A54">
     <cfRule type="duplicateValues" dxfId="2" priority="13"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A179">
+  <conditionalFormatting sqref="A180">
     <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6822,9 +6844,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:C176"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A92" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F105" sqref="F105"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A98" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H109" sqref="H109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8013,9 +8035,7 @@
       <c r="B109" s="2" t="s">
         <v>585</v>
       </c>
-      <c r="C109" s="2" t="s">
-        <v>881</v>
-      </c>
+      <c r="C109" s="2"/>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" t="s">

</xml_diff>

<commit_message>
added lisence for data_enclave case
</commit_message>
<xml_diff>
--- a/data-raw/control_vocab_mapping.xlsx
+++ b/data-raw/control_vocab_mapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WB525812\cmder\Git Repos\mdlibtoddh\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D698C397-171C-42C6-9D47-106B9ECE7582}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B972C01-014D-4168-8CEC-9515EC831356}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="10770" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1135" uniqueCount="774">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1136" uniqueCount="774">
   <si>
     <t>microdata_category</t>
   </si>
@@ -7331,7 +7331,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7400,6 +7400,9 @@
       <c r="A8" s="1" t="s">
         <v>666</v>
       </c>
+      <c r="B8" s="1" t="s">
+        <v>754</v>
+      </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>

</xml_diff>

<commit_message>
study_type fix for lookup vector
</commit_message>
<xml_diff>
--- a/data-raw/control_vocab_mapping.xlsx
+++ b/data-raw/control_vocab_mapping.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WB525812\cmder\Git Repos\mdlibtoddh\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{9667F295-8439-44D7-91B6-B7DCA654A025}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B50C3C26-AF22-4A15-BA20-DD415EBA968A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="10770" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="10770" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dataClassification" sheetId="1" r:id="rId1"/>
@@ -18,15 +18,13 @@
     <sheet name="kindData" sheetId="3" r:id="rId3"/>
     <sheet name="modeDataColl" sheetId="4" r:id="rId4"/>
     <sheet name="geographicalCoverage" sheetId="5" r:id="rId5"/>
-    <sheet name="studyType" sheetId="6" r:id="rId6"/>
-    <sheet name="source" sheetId="7" r:id="rId7"/>
-    <sheet name="license" sheetId="8" r:id="rId8"/>
+    <sheet name="source" sheetId="7" r:id="rId6"/>
+    <sheet name="license" sheetId="8" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">geographicalCoverage!$A$1:$B$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">kindData!$A$1:$B$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">modeDataColl!$A$1:$C$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">studyType!$A$1:$C$1</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -38,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1404" uniqueCount="883">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="919" uniqueCount="648">
   <si>
     <t>microdata_category</t>
   </si>
@@ -1780,474 +1778,6 @@
     <t>Serbia;Montenegro</t>
   </si>
   <si>
-    <t>1-2-3 Survey, phase 1</t>
-  </si>
-  <si>
-    <t>1-2-3 Survey, phase 3</t>
-  </si>
-  <si>
-    <t>Enterprise Survey</t>
-  </si>
-  <si>
-    <t>Income/Expenditure/Household Survey</t>
-  </si>
-  <si>
-    <t>Labor Force Survey</t>
-  </si>
-  <si>
-    <t>Other Household Survey</t>
-  </si>
-  <si>
-    <t>labor force survey [hh/lfs]</t>
-  </si>
-  <si>
-    <t>living standards measurement study [hh/lsms]</t>
-  </si>
-  <si>
-    <t>public expenditure tracking survey (pets)</t>
-  </si>
-  <si>
-    <t>enterprise survey [en/oth]</t>
-  </si>
-  <si>
-    <t>multiple indicator cluster survey - round 3 [hh/mics-3]</t>
-  </si>
-  <si>
-    <t>core welfare indicators questionnaire [hh/cwiq]</t>
-  </si>
-  <si>
-    <t>multiple indicator cluster survey - round 2 [hh/mics-2]</t>
-  </si>
-  <si>
-    <t>public expenditure tracking survey (pets)/quantitative service delivery survey (qsds)</t>
-  </si>
-  <si>
-    <t>public expenditure tracking survey</t>
-  </si>
-  <si>
-    <t>multiple indicator cluster survey - round 1 [hh/mics-1]</t>
-  </si>
-  <si>
-    <t>income/expenditure/household survey [hh/ies]</t>
-  </si>
-  <si>
-    <t>public expenditure tracking survey (pets)/quantitative service delivery surveys (qsds)</t>
-  </si>
-  <si>
-    <t>macroeconomics - indicators</t>
-  </si>
-  <si>
-    <t>other household survey [hh/oth]</t>
-  </si>
-  <si>
-    <t>agricultural survey [ag/oth]</t>
-  </si>
-  <si>
-    <t>demographic and health survey [hh/dhs]</t>
-  </si>
-  <si>
-    <t>agricultural census [ag/census]</t>
-  </si>
-  <si>
-    <t>aids indicators survey (ais)</t>
-  </si>
-  <si>
-    <t>population and housing census [hh/popcen]</t>
-  </si>
-  <si>
-    <t>demographic and health survey (standard) - dhs v</t>
-  </si>
-  <si>
-    <t>demographic and health survey (standard) - dhs iii</t>
-  </si>
-  <si>
-    <t>enterprise/establishment survey [en/oth]</t>
-  </si>
-  <si>
-    <t>demographic and health survey (standard) - dhs iv</t>
-  </si>
-  <si>
-    <t>other household health survey [hh/hea]</t>
-  </si>
-  <si>
-    <t>child labor survey [hh/cls]</t>
-  </si>
-  <si>
-    <t>health facility survey</t>
-  </si>
-  <si>
-    <t>africa client feedback surveys</t>
-  </si>
-  <si>
-    <t>socio-economic/monitoring survey [hh/sems]</t>
-  </si>
-  <si>
-    <t>enquête budget-consommation des ménages [hh/ies]</t>
-  </si>
-  <si>
-    <t>multiple indicator cluster survey - round 4 [hh/mics-4]</t>
-  </si>
-  <si>
-    <t>sample frame, enterprises [sf/en]</t>
-  </si>
-  <si>
-    <t>integrated survey (non-lsms) [hh/is]</t>
-  </si>
-  <si>
-    <t>demographic and health survey (standard) - dhs vi</t>
-  </si>
-  <si>
-    <t>administrative records, other (ad/oth]</t>
-  </si>
-  <si>
-    <t>world fertility survey [hh/wfs]</t>
-  </si>
-  <si>
-    <t>other survey</t>
-  </si>
-  <si>
-    <t>enterprise census [en/census]</t>
-  </si>
-  <si>
-    <t>administrative records, education (ad/edu]</t>
-  </si>
-  <si>
-    <t>demographic and health survey, special [hh/dhs-sp]</t>
-  </si>
-  <si>
-    <t>demographic and health survey (standard) - dhs i</t>
-  </si>
-  <si>
-    <t>service provision assessments [hh/spa]</t>
-  </si>
-  <si>
-    <t>encuesta de fuerza laboral [hh/lfs]</t>
-  </si>
-  <si>
-    <t>priority survey (hh/ps]</t>
-  </si>
-  <si>
-    <t>demographic and health survey (standard) - dhs ii</t>
-  </si>
-  <si>
-    <t>public opinion survey [ind/pos]</t>
-  </si>
-  <si>
-    <t>informal sector survey [hh/iss]</t>
-  </si>
-  <si>
-    <t>administrative records, construction statistics (ad/oth]</t>
-  </si>
-  <si>
-    <t>administrative records, other (ad/oth]- import and export documents</t>
-  </si>
-  <si>
-    <t>client feedback surveys</t>
-  </si>
-  <si>
-    <t>household survey &amp; census</t>
-  </si>
-  <si>
-    <t>encuesta de monitoreo socio - económico [hh/sems]</t>
-  </si>
-  <si>
-    <t>malaria indicators survey (mis)</t>
-  </si>
-  <si>
-    <t>world health survey [hh/whs]</t>
-  </si>
-  <si>
-    <t>enquête sur les conditions de vie des ménages [hh/lsms]</t>
-  </si>
-  <si>
-    <t>impact evaluation</t>
-  </si>
-  <si>
-    <t>impact evaluation study [ie/ies]</t>
-  </si>
-  <si>
-    <t>administrative, trade</t>
-  </si>
-  <si>
-    <t>turism survey</t>
-  </si>
-  <si>
-    <t>statistical info. &amp; monitoring prog. [hh/simpoc]</t>
-  </si>
-  <si>
-    <t>demographic and health survey (standard) - other</t>
-  </si>
-  <si>
-    <t>demographic and health survey, round 3  [hh/dhs-3]</t>
-  </si>
-  <si>
-    <t>people security surveys</t>
-  </si>
-  <si>
-    <t>health facility survey [fac/hfs]</t>
-  </si>
-  <si>
-    <t>labor force survey</t>
-  </si>
-  <si>
-    <t>price survey [hh/prc]</t>
-  </si>
-  <si>
-    <t>administrative records, health (ad/hea]</t>
-  </si>
-  <si>
-    <t>public opinion survey</t>
-  </si>
-  <si>
-    <t>demographic and health survey (special) - dhs iii</t>
-  </si>
-  <si>
-    <t>administrative records, other [ad/oth]</t>
-  </si>
-  <si>
-    <t>financial survey</t>
-  </si>
-  <si>
-    <t>housing construction survey</t>
-  </si>
-  <si>
-    <t>enterprise/establishment census [en/census]</t>
-  </si>
-  <si>
-    <t>demographic survey [hh/ds]</t>
-  </si>
-  <si>
-    <t>sample frame, households [sf/hh]</t>
-  </si>
-  <si>
-    <t>non-profit institution survey</t>
-  </si>
-  <si>
-    <t>service delivery indicators survey (sdi)</t>
-  </si>
-  <si>
-    <t>service availability mapping</t>
-  </si>
-  <si>
-    <t>demographic and health survey, ais</t>
-  </si>
-  <si>
-    <t>demographic and health survey, aids indicator</t>
-  </si>
-  <si>
-    <t>enquête socio-economique / monitoring [hh/sems]</t>
-  </si>
-  <si>
-    <t>demographic and health survey, interim [hh/dhs-int]</t>
-  </si>
-  <si>
-    <t>comprehensive food security &amp; vulnerability analysis [hh/cfsva]</t>
-  </si>
-  <si>
-    <t>other household survey</t>
-  </si>
-  <si>
-    <t>encuesta a hogares - otro [hh/oth]</t>
-  </si>
-  <si>
-    <t>encuesta de gastos e ingresos a hogares[hh/ies]</t>
-  </si>
-  <si>
-    <t>quantitative service delivery survey (qsds)</t>
-  </si>
-  <si>
-    <t>country opinion survey</t>
-  </si>
-  <si>
-    <t>1-2-3 survey, phase 1 [hh/123-1]</t>
-  </si>
-  <si>
-    <t>rural, agriculture and fisheries census</t>
-  </si>
-  <si>
-    <t>1-2-3 survey, phase 2 [hh/123-2]</t>
-  </si>
-  <si>
-    <t>autres enquêtes ménages [hh/oth]</t>
-  </si>
-  <si>
-    <t>enquête sur le secteur informel [hh/iss]</t>
-  </si>
-  <si>
-    <t>opinion survey</t>
-  </si>
-  <si>
-    <t>encuesta a hogares</t>
-  </si>
-  <si>
-    <t>enquête agricole [ag/oth]</t>
-  </si>
-  <si>
-    <t>income/expenditure/household survey</t>
-  </si>
-  <si>
-    <t>censo de población y habitación [hh/popcen]</t>
-  </si>
-  <si>
-    <t>encuesta de hogares</t>
-  </si>
-  <si>
-    <t>encuesta de hogares de propósitos múltiples</t>
-  </si>
-  <si>
-    <t>encuesta de hogares de propósitos múltiples (ehpm)</t>
-  </si>
-  <si>
-    <t>encuesta fuerza laboral</t>
-  </si>
-  <si>
-    <t>enquête sur le travail des enfants [hh/cls]</t>
-  </si>
-  <si>
-    <t>censo de población y vivienda</t>
-  </si>
-  <si>
-    <t>encuesta nacional (censo continuo)</t>
-  </si>
-  <si>
-    <t>encuesta de monitoreo socio-económico [hh/sems]</t>
-  </si>
-  <si>
-    <t>registros administrativos, otros (ad/oth]</t>
-  </si>
-  <si>
-    <t>impact evaluation survey</t>
-  </si>
-  <si>
-    <t>enterprise survey</t>
-  </si>
-  <si>
-    <t>education/school survey [ed/sch]</t>
-  </si>
-  <si>
-    <t>encuesta de empresas [en/oth]</t>
-  </si>
-  <si>
-    <t>otras encuestas a hogares [hh/oth]</t>
-  </si>
-  <si>
-    <t>demographic surveillance</t>
-  </si>
-  <si>
-    <t>cross-sectional</t>
-  </si>
-  <si>
-    <t>estudio de medición de las condiciones de vida [hh/lsms]</t>
-  </si>
-  <si>
-    <t>pay for performance (p4p) - tanzania</t>
-  </si>
-  <si>
-    <t>censo</t>
-  </si>
-  <si>
-    <t>encuesta de empleo [hh/lfs]</t>
-  </si>
-  <si>
-    <t>censo de la gestión, gasto e inversión en protección ambiental en municipios y consejos provinciales</t>
-  </si>
-  <si>
-    <t>1-2-3 survey, phase 3</t>
-  </si>
-  <si>
-    <t>encuesta de buenas prácticas ambientales</t>
-  </si>
-  <si>
-    <t>encuesta ambiental</t>
-  </si>
-  <si>
-    <t>demographic and health survey, round 2 [hh/dhs-2]</t>
-  </si>
-  <si>
-    <t>demographic and health survey (special) - dhs vi</t>
-  </si>
-  <si>
-    <t>demographic and health survey (standard) - dhs vii</t>
-  </si>
-  <si>
-    <t>independent impact evaluation</t>
-  </si>
-  <si>
-    <t>independent evaluation</t>
-  </si>
-  <si>
-    <t>school survey (baseline)</t>
-  </si>
-  <si>
-    <t>independent performance evaluation</t>
-  </si>
-  <si>
-    <t>independent impact evaluation, independent performance evaluation</t>
-  </si>
-  <si>
-    <t>1-2-3 survey, phase 1</t>
-  </si>
-  <si>
-    <t>agricultural survey &amp; census</t>
-  </si>
-  <si>
-    <t>multiple indicator cluster survey - round 5 [hh/mics-5]</t>
-  </si>
-  <si>
-    <t>encuesta</t>
-  </si>
-  <si>
-    <t>registros administrativos</t>
-  </si>
-  <si>
-    <t>estadística de precios</t>
-  </si>
-  <si>
-    <t>estadística del sector eléctrico</t>
-  </si>
-  <si>
-    <t>impact evaluation study</t>
-  </si>
-  <si>
-    <t>other enterprise survey</t>
-  </si>
-  <si>
-    <t>public expenditure tracking survey (pets/qsds)</t>
-  </si>
-  <si>
-    <t>public expenditure tracking survey / quantitative service delivery suurvey (pets/qsds)</t>
-  </si>
-  <si>
-    <t>public expenditure tracking survey / quantitative service delivery survey (pets/qsds)</t>
-  </si>
-  <si>
-    <t>Agricultural Census;Agricultural Survey</t>
-  </si>
-  <si>
-    <t>Opinion survey</t>
-  </si>
-  <si>
-    <t>Comprehensive Food Security and Vulnerability Analysis</t>
-  </si>
-  <si>
-    <t>Independent Performance Evaluation</t>
-  </si>
-  <si>
-    <t>Macroeconomic indicators</t>
-  </si>
-  <si>
-    <t>Independent Performance Evaluation;Impact evaluation</t>
-  </si>
-  <si>
-    <t>Public Expenditure Tracking Survey (PETS)</t>
-  </si>
-  <si>
-    <t>Quantitative Service Delivery Survey/Service Delivery Indicators</t>
-  </si>
-  <si>
-    <t>Public Expenditure Tracking Survey (PETS);Quantitative Service Delivery Survey/Service Delivery Indicators</t>
-  </si>
-  <si>
     <t>Official Use Only</t>
   </si>
   <si>
@@ -2311,162 +1841,24 @@
     <t>remote</t>
   </si>
   <si>
-    <t>Living Standards Measurement Study [hh/lsms]</t>
-  </si>
-  <si>
-    <t>1-2-3 Survey, phase 1 [hh/123-1]</t>
-  </si>
-  <si>
-    <t>1-2-3 Survey, phase 2 [hh/123-2]</t>
-  </si>
-  <si>
-    <t>Administrative Records, Education (ad/edu]</t>
-  </si>
-  <si>
-    <t>Administrative Records, Health (ad/hea]</t>
-  </si>
-  <si>
-    <t>Administrative Records, Other [ad/oth]</t>
-  </si>
-  <si>
-    <t>Agricultural Census [ag/census]</t>
-  </si>
-  <si>
-    <t>Agricultural Survey [ag/oth]</t>
-  </si>
-  <si>
-    <t>Child Labor Survey [hh/cls]</t>
-  </si>
-  <si>
-    <t>Core Welfare Indicators Questionnaire [hh/cwiq]</t>
-  </si>
-  <si>
-    <t>Demographic and Health Survey [hh/dhs]</t>
-  </si>
-  <si>
-    <t>Enterprise Census [en/census]</t>
-  </si>
-  <si>
-    <t>Impact Evaluation</t>
-  </si>
-  <si>
-    <t>Informal Sector Survey [hh/iss]</t>
-  </si>
-  <si>
-    <t>Integrated Survey (non-LSMS) [hh/is]</t>
-  </si>
-  <si>
-    <t>Multiple Indicator Cluster Survey - Round 1 [hh/mics-1]</t>
-  </si>
-  <si>
-    <t>Multiple Indicator Cluster Survey - Round 2 [hh/mics-2]</t>
-  </si>
-  <si>
-    <t>Multiple Indicator Cluster Survey - Round 3 [hh/mics-3]</t>
-  </si>
-  <si>
-    <t>Multiple Indicator Cluster Survey - Round 4 [hh/mics-4]</t>
-  </si>
-  <si>
-    <t>Multiple Indicator Cluster Survey - Round 5 [hh/mics-5]</t>
-  </si>
-  <si>
-    <t>Other Household Health Survey [hh/hea]</t>
-  </si>
-  <si>
-    <t>Population and Housing Census [hh/popcen]</t>
-  </si>
-  <si>
-    <t>Price Survey [hh/prc]</t>
-  </si>
-  <si>
-    <t>Sample Frame, Enterprises [sf/en]</t>
-  </si>
-  <si>
-    <t>Sample Frame, Households [sf/hh]</t>
-  </si>
-  <si>
-    <t>Service Provision Assessments [hh/spa]</t>
-  </si>
-  <si>
-    <t>Socio-Economic/Monitoring Survey [hh/sems]</t>
-  </si>
-  <si>
-    <t>Statistical Info. &amp; Monitoring Prog. [hh/simpoc]</t>
-  </si>
-  <si>
-    <t>World Fertility Survey [hh/wfs]</t>
-  </si>
-  <si>
-    <t>World Health Survey [hh/whs]</t>
-  </si>
-  <si>
-    <t>Enterprise/Establishment Census [en/census]</t>
-  </si>
-  <si>
-    <t>establishment census [en/census]</t>
-  </si>
-  <si>
-    <t>world health survey [step survey]</t>
-  </si>
-  <si>
     <t>Sub-Saharan Africa</t>
   </si>
   <si>
     <t>Brunei Darussalam</t>
   </si>
   <si>
-    <t>Other Household Health Survey</t>
-  </si>
-  <si>
-    <t>country opnion survey</t>
-  </si>
-  <si>
-    <t>socio-economic/monitoring survey</t>
-  </si>
-  <si>
-    <t>young people in egypt survey</t>
-  </si>
-  <si>
-    <t>Education/School Survey [ed/sch]</t>
-  </si>
-  <si>
-    <t>higher education graduates survey [ind/hegs]</t>
-  </si>
-  <si>
     <t>federated states of micronesia</t>
   </si>
   <si>
-    <t>Living Standards Measurement Study</t>
-  </si>
-  <si>
     <t>Cote d’Ivoire</t>
   </si>
   <si>
-    <t>demographic and health survey, special (mis)</t>
-  </si>
-  <si>
-    <t>Encuesta Continua de Empleo</t>
-  </si>
-  <si>
     <t>statutory return submitted by factories as well as face to face</t>
   </si>
   <si>
-    <t>industrial statistics</t>
-  </si>
-  <si>
     <t>encuesta probabilística en establecimientos</t>
   </si>
   <si>
-    <t>school survey (midline)</t>
-  </si>
-  <si>
-    <t>service provision assessments</t>
-  </si>
-  <si>
-    <t>aids indicator survey [hh/ais]</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Face-to-face;internet [int]</t>
   </si>
   <si>
@@ -2476,66 +1868,6 @@
     <t>viet nam</t>
   </si>
   <si>
-    <t>labour force survey [hh/lfs]</t>
-  </si>
-  <si>
-    <t>household survey [hh]</t>
-  </si>
-  <si>
-    <t>People Security Surveys</t>
-  </si>
-  <si>
-    <t>AIDS Indicators Survey (AIS)</t>
-  </si>
-  <si>
-    <t>Censo de la GestiÃ³n, Gasto e InversiÃ³n en ProtecciÃ³n Ambiental en Municipios y Consejos Provinciales</t>
-  </si>
-  <si>
-    <t>Cross-sectional</t>
-  </si>
-  <si>
-    <t>Encuesta Ambiental</t>
-  </si>
-  <si>
-    <t>Encuesta de Buenas PrÃ¡cticas Ambientales</t>
-  </si>
-  <si>
-    <t>Financial Survey</t>
-  </si>
-  <si>
-    <t>Housing Construction Survey</t>
-  </si>
-  <si>
-    <t>Malaria Indicators Survey (MIS)</t>
-  </si>
-  <si>
-    <t>Other Survey</t>
-  </si>
-  <si>
-    <t>Pay For Performance (P4P) - Tanzania</t>
-  </si>
-  <si>
-    <t>Service Availability Mapping</t>
-  </si>
-  <si>
-    <t>Priority Survey (hh/ps]</t>
-  </si>
-  <si>
-    <t>School survey (baseline)</t>
-  </si>
-  <si>
-    <t>Service Delivery Indicators Survey (SDI)</t>
-  </si>
-  <si>
-    <t>Turism survey</t>
-  </si>
-  <si>
-    <t>Non-profit Institution Survey</t>
-  </si>
-  <si>
-    <t>Encuesta</t>
-  </si>
-  <si>
     <t>Venezuela, RB</t>
   </si>
   <si>
@@ -2566,9 +1898,6 @@
     <t>Source not specified</t>
   </si>
   <si>
-    <t>informal sector survey</t>
-  </si>
-  <si>
     <t>face-to-face[f2f]</t>
   </si>
   <si>
@@ -2578,24 +1907,9 @@
     <t>questionnaire envoyé [mail]</t>
   </si>
   <si>
-    <t>community survey</t>
-  </si>
-  <si>
-    <t>crime survey [hh/cr]</t>
-  </si>
-  <si>
     <t>this series of savvy mortality surveillance system manuals, guides, and other documents is available at the measure evaluation\\nweb site at: http://www.cpc.unc.edu/measure/leadership/savvy.html</t>
   </si>
   <si>
-    <t>Estadã­stica del Sector Elã©ctrico</t>
-  </si>
-  <si>
-    <t>demographic and health survey, mis</t>
-  </si>
-  <si>
-    <t>enquête sur les entreprises [en/oth]</t>
-  </si>
-  <si>
     <t>paper and pencil</t>
   </si>
   <si>
@@ -2623,9 +1937,6 @@
     <t>gambia</t>
   </si>
   <si>
-    <t>Public Opinion Survey [po]]</t>
-  </si>
-  <si>
     <t xml:space="preserve">Other </t>
   </si>
   <si>
@@ -2638,18 +1949,9 @@
     <t>please see: http://www.europeansocialsurvey.org/essdoc/doc.html?year=2012&amp;ddi=2.3.1.6</t>
   </si>
   <si>
-    <t>malaria indicator survey</t>
-  </si>
-  <si>
     <t>Sample survey data[ssd]</t>
   </si>
   <si>
-    <t>Demographic and Health Survey, Special - AIS</t>
-  </si>
-  <si>
-    <t>Health Survey [hh/hs]</t>
-  </si>
-  <si>
     <t>Sénégal</t>
   </si>
   <si>
@@ -2659,12 +1961,6 @@
     <t>Face_to_Face</t>
   </si>
   <si>
-    <t>Données administrative, santé [ad/hea]</t>
-  </si>
-  <si>
-    <t>Echantillon de référence, ménages [sf/hh]</t>
-  </si>
-  <si>
     <t>Par téléphone [cati]</t>
   </si>
   <si>
@@ -2678,9 +1974,6 @@
   </si>
   <si>
     <t>Taiwan China</t>
-  </si>
-  <si>
-    <t>Multiple Indicator Cluster Survey - Round 6 [hh/mics-6]</t>
   </si>
   <si>
     <t>Other[oth]</t>
@@ -2693,7 +1986,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2708,36 +2001,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="8"/>
-      <color rgb="FF000000"/>
-      <name val="Lucida Sans"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Courier New"/>
-      <family val="3"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFDFDFD"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -2752,34 +2022,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="18">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="17">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -3285,7 +2535,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>736</v>
+        <v>580</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -3325,7 +2575,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>752</v>
+        <v>596</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>5</v>
@@ -3333,7 +2583,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>753</v>
+        <v>597</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>6</v>
@@ -3349,7 +2599,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>754</v>
+        <v>598</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>8</v>
@@ -3357,7 +2607,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>756</v>
+        <v>600</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>9</v>
@@ -3365,7 +2615,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>751</v>
+        <v>595</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>10</v>
@@ -3373,7 +2623,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>755</v>
+        <v>599</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>11</v>
@@ -3420,7 +2670,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>737</v>
+        <v>581</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -3507,7 +2757,7 @@
         <v>72</v>
       </c>
       <c r="B10" t="s">
-        <v>833</v>
+        <v>611</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -3515,7 +2765,7 @@
         <v>64</v>
       </c>
       <c r="B11" t="s">
-        <v>833</v>
+        <v>611</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -3765,7 +3015,7 @@
         <v>94</v>
       </c>
       <c r="B34" t="s">
-        <v>833</v>
+        <v>611</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -3855,7 +3105,7 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>805</v>
+        <v>606</v>
       </c>
       <c r="B43" t="s">
         <v>14</v>
@@ -3863,7 +3113,7 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>867</v>
+        <v>637</v>
       </c>
       <c r="B44" t="s">
         <v>14</v>
@@ -3898,7 +3148,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>737</v>
+        <v>581</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -3950,7 +3200,7 @@
         <v>154</v>
       </c>
       <c r="B6" t="s">
-        <v>839</v>
+        <v>617</v>
       </c>
       <c r="C6" t="s">
         <v>28</v>
@@ -3961,7 +3211,7 @@
         <v>157</v>
       </c>
       <c r="B7" t="s">
-        <v>839</v>
+        <v>617</v>
       </c>
       <c r="C7" t="s">
         <v>28</v>
@@ -3972,7 +3222,7 @@
         <v>136</v>
       </c>
       <c r="B8" t="s">
-        <v>863</v>
+        <v>634</v>
       </c>
       <c r="C8" t="s">
         <v>27</v>
@@ -3983,7 +3233,7 @@
         <v>135</v>
       </c>
       <c r="B9" t="s">
-        <v>863</v>
+        <v>634</v>
       </c>
       <c r="C9" t="s">
         <v>27</v>
@@ -3994,7 +3244,7 @@
         <v>150</v>
       </c>
       <c r="B10" t="s">
-        <v>863</v>
+        <v>634</v>
       </c>
       <c r="C10" t="s">
         <v>27</v>
@@ -4005,7 +3255,7 @@
         <v>145</v>
       </c>
       <c r="B11" t="s">
-        <v>863</v>
+        <v>634</v>
       </c>
       <c r="C11" t="s">
         <v>27</v>
@@ -4016,7 +3266,7 @@
         <v>152</v>
       </c>
       <c r="B12" t="s">
-        <v>863</v>
+        <v>634</v>
       </c>
       <c r="C12" t="s">
         <v>27</v>
@@ -4057,7 +3307,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>875</v>
+        <v>641</v>
       </c>
       <c r="B16" t="s">
         <v>32</v>
@@ -4093,7 +3343,7 @@
         <v>139</v>
       </c>
       <c r="B19" t="s">
-        <v>863</v>
+        <v>634</v>
       </c>
       <c r="C19" t="s">
         <v>27</v>
@@ -4104,7 +3354,7 @@
         <v>151</v>
       </c>
       <c r="B20" t="s">
-        <v>863</v>
+        <v>634</v>
       </c>
       <c r="C20" t="s">
         <v>27</v>
@@ -4126,7 +3376,7 @@
         <v>146</v>
       </c>
       <c r="B22" t="s">
-        <v>863</v>
+        <v>634</v>
       </c>
       <c r="C22" t="s">
         <v>27</v>
@@ -4137,7 +3387,7 @@
         <v>148</v>
       </c>
       <c r="B23" t="s">
-        <v>863</v>
+        <v>634</v>
       </c>
       <c r="C23" t="s">
         <v>27</v>
@@ -4170,7 +3420,7 @@
         <v>153</v>
       </c>
       <c r="B26" t="s">
-        <v>863</v>
+        <v>634</v>
       </c>
       <c r="C26" t="s">
         <v>27</v>
@@ -4181,7 +3431,7 @@
         <v>149</v>
       </c>
       <c r="B27" t="s">
-        <v>863</v>
+        <v>634</v>
       </c>
       <c r="C27" t="s">
         <v>27</v>
@@ -4203,7 +3453,7 @@
         <v>172</v>
       </c>
       <c r="B29" t="s">
-        <v>863</v>
+        <v>634</v>
       </c>
       <c r="C29" t="s">
         <v>27</v>
@@ -4214,7 +3464,7 @@
         <v>104</v>
       </c>
       <c r="B30" t="s">
-        <v>863</v>
+        <v>634</v>
       </c>
       <c r="C30" t="s">
         <v>27</v>
@@ -4225,7 +3475,7 @@
         <v>130</v>
       </c>
       <c r="B31" t="s">
-        <v>863</v>
+        <v>634</v>
       </c>
       <c r="C31" t="s">
         <v>27</v>
@@ -4233,10 +3483,10 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>843</v>
+        <v>620</v>
       </c>
       <c r="B32" t="s">
-        <v>863</v>
+        <v>634</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -4244,7 +3494,7 @@
         <v>103</v>
       </c>
       <c r="B33" t="s">
-        <v>863</v>
+        <v>634</v>
       </c>
       <c r="C33" t="s">
         <v>27</v>
@@ -4255,7 +3505,7 @@
         <v>107</v>
       </c>
       <c r="B34" t="s">
-        <v>863</v>
+        <v>634</v>
       </c>
       <c r="C34" t="s">
         <v>27</v>
@@ -4277,7 +3527,7 @@
         <v>137</v>
       </c>
       <c r="B36" t="s">
-        <v>863</v>
+        <v>634</v>
       </c>
       <c r="C36" t="s">
         <v>27</v>
@@ -4288,7 +3538,7 @@
         <v>131</v>
       </c>
       <c r="B37" t="s">
-        <v>863</v>
+        <v>634</v>
       </c>
       <c r="C37" t="s">
         <v>181</v>
@@ -4299,7 +3549,7 @@
         <v>122</v>
       </c>
       <c r="B38" t="s">
-        <v>863</v>
+        <v>634</v>
       </c>
       <c r="C38" t="s">
         <v>27</v>
@@ -4310,7 +3560,7 @@
         <v>132</v>
       </c>
       <c r="B39" t="s">
-        <v>863</v>
+        <v>634</v>
       </c>
       <c r="C39" t="s">
         <v>182</v>
@@ -4329,13 +3579,13 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>810</v>
+        <v>608</v>
       </c>
       <c r="B41" t="s">
-        <v>863</v>
+        <v>634</v>
       </c>
       <c r="C41" t="s">
-        <v>809</v>
+        <v>607</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -4343,7 +3593,7 @@
         <v>123</v>
       </c>
       <c r="B42" t="s">
-        <v>863</v>
+        <v>634</v>
       </c>
       <c r="C42" t="s">
         <v>27</v>
@@ -4354,7 +3604,7 @@
         <v>134</v>
       </c>
       <c r="B43" t="s">
-        <v>863</v>
+        <v>634</v>
       </c>
       <c r="C43" t="s">
         <v>27</v>
@@ -4362,10 +3612,10 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>844</v>
+        <v>621</v>
       </c>
       <c r="B44" t="s">
-        <v>863</v>
+        <v>634</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -4384,7 +3634,7 @@
         <v>158</v>
       </c>
       <c r="B46" t="s">
-        <v>863</v>
+        <v>634</v>
       </c>
       <c r="C46" t="s">
         <v>27</v>
@@ -4395,7 +3645,7 @@
         <v>159</v>
       </c>
       <c r="B47" t="s">
-        <v>863</v>
+        <v>634</v>
       </c>
       <c r="C47" t="s">
         <v>27</v>
@@ -4406,7 +3656,7 @@
         <v>160</v>
       </c>
       <c r="B48" t="s">
-        <v>863</v>
+        <v>634</v>
       </c>
       <c r="C48" t="s">
         <v>183</v>
@@ -4417,7 +3667,7 @@
         <v>170</v>
       </c>
       <c r="B49" t="s">
-        <v>863</v>
+        <v>634</v>
       </c>
       <c r="C49" t="s">
         <v>27</v>
@@ -4428,7 +3678,7 @@
         <v>175</v>
       </c>
       <c r="B50" t="s">
-        <v>863</v>
+        <v>634</v>
       </c>
       <c r="C50" t="s">
         <v>27</v>
@@ -4436,10 +3686,10 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>872</v>
+        <v>640</v>
       </c>
       <c r="B51" t="s">
-        <v>863</v>
+        <v>634</v>
       </c>
       <c r="C51" t="s">
         <v>104</v>
@@ -4450,7 +3700,7 @@
         <v>147</v>
       </c>
       <c r="B52" t="s">
-        <v>864</v>
+        <v>635</v>
       </c>
       <c r="C52" t="s">
         <v>29</v>
@@ -4458,13 +3708,13 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>876</v>
+        <v>642</v>
       </c>
       <c r="B53" t="s">
-        <v>864</v>
+        <v>635</v>
       </c>
       <c r="C53" t="s">
-        <v>864</v>
+        <v>635</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
@@ -4472,7 +3722,7 @@
         <v>115</v>
       </c>
       <c r="B54" t="s">
-        <v>864</v>
+        <v>635</v>
       </c>
       <c r="C54" t="s">
         <v>178</v>
@@ -4505,7 +3755,7 @@
         <v>109</v>
       </c>
       <c r="B57" t="s">
-        <v>863</v>
+        <v>634</v>
       </c>
       <c r="C57" t="s">
         <v>27</v>
@@ -4538,7 +3788,7 @@
         <v>108</v>
       </c>
       <c r="B60" t="s">
-        <v>839</v>
+        <v>617</v>
       </c>
       <c r="C60" t="s">
         <v>28</v>
@@ -4549,7 +3799,7 @@
         <v>120</v>
       </c>
       <c r="B61" t="s">
-        <v>839</v>
+        <v>617</v>
       </c>
       <c r="C61" t="s">
         <v>28</v>
@@ -4571,7 +3821,7 @@
         <v>94</v>
       </c>
       <c r="B63" t="s">
-        <v>835</v>
+        <v>613</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
@@ -4579,7 +3829,7 @@
         <v>142</v>
       </c>
       <c r="B64" t="s">
-        <v>835</v>
+        <v>613</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
@@ -4587,7 +3837,7 @@
         <v>72</v>
       </c>
       <c r="B65" t="s">
-        <v>862</v>
+        <v>633</v>
       </c>
       <c r="C65" t="s">
         <v>31</v>
@@ -4598,7 +3848,7 @@
         <v>105</v>
       </c>
       <c r="B66" t="s">
-        <v>862</v>
+        <v>633</v>
       </c>
       <c r="C66" t="s">
         <v>31</v>
@@ -4697,7 +3947,7 @@
         <v>155</v>
       </c>
       <c r="B75" t="s">
-        <v>862</v>
+        <v>633</v>
       </c>
       <c r="C75" t="s">
         <v>31</v>
@@ -4719,7 +3969,7 @@
         <v>167</v>
       </c>
       <c r="B77" t="s">
-        <v>863</v>
+        <v>634</v>
       </c>
       <c r="C77" t="s">
         <v>182</v>
@@ -4730,7 +3980,7 @@
         <v>133</v>
       </c>
       <c r="B78" t="s">
-        <v>863</v>
+        <v>634</v>
       </c>
       <c r="C78" t="s">
         <v>27</v>
@@ -4749,10 +3999,10 @@
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>838</v>
+        <v>616</v>
       </c>
       <c r="B80" t="s">
-        <v>839</v>
+        <v>617</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
@@ -4760,7 +4010,7 @@
         <v>138</v>
       </c>
       <c r="B81" t="s">
-        <v>863</v>
+        <v>634</v>
       </c>
       <c r="C81" t="s">
         <v>182</v>
@@ -4768,10 +4018,10 @@
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>803</v>
+        <v>605</v>
       </c>
       <c r="B82" t="s">
-        <v>863</v>
+        <v>634</v>
       </c>
       <c r="C82" t="s">
         <v>27</v>
@@ -4801,7 +4051,7 @@
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>840</v>
+        <v>618</v>
       </c>
       <c r="B85" t="s">
         <v>25</v>
@@ -4836,7 +4086,7 @@
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B89" t="s">
-        <v>864</v>
+        <v>635</v>
       </c>
       <c r="C89" t="s">
         <v>29</v>
@@ -4844,23 +4094,23 @@
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>845</v>
+        <v>622</v>
       </c>
       <c r="B90" t="s">
-        <v>839</v>
+        <v>617</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>852</v>
+        <v>624</v>
       </c>
       <c r="B91" t="s">
-        <v>863</v>
+        <v>634</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>865</v>
+        <v>636</v>
       </c>
       <c r="B92" t="s">
         <v>25</v>
@@ -4868,7 +4118,7 @@
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>877</v>
+        <v>643</v>
       </c>
       <c r="B93" t="s">
         <v>25</v>
@@ -4876,7 +4126,7 @@
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>881</v>
+        <v>646</v>
       </c>
       <c r="B94" t="s">
         <v>25</v>
@@ -4892,34 +4142,34 @@
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="A93:A1048576 A1:A8 A10:A12 A14:A43 A45:A86">
-    <cfRule type="duplicateValues" dxfId="17" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="16" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A9">
-    <cfRule type="duplicateValues" dxfId="16" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="15" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A13">
-    <cfRule type="duplicateValues" dxfId="15" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="14" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A87">
-    <cfRule type="duplicateValues" dxfId="14" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A88">
-    <cfRule type="duplicateValues" dxfId="13" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A89">
-    <cfRule type="duplicateValues" dxfId="12" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A44">
-    <cfRule type="duplicateValues" dxfId="11" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A90">
-    <cfRule type="duplicateValues" dxfId="10" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A91">
-    <cfRule type="duplicateValues" dxfId="9" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A92">
-    <cfRule type="duplicateValues" dxfId="8" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4930,7 +4180,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B233"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A91" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="J95" sqref="J95"/>
     </sheetView>
@@ -4962,7 +4212,7 @@
         <v>275</v>
       </c>
       <c r="B3" t="s">
-        <v>790</v>
+        <v>601</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -4970,7 +4220,7 @@
         <v>368</v>
       </c>
       <c r="B4" t="s">
-        <v>790</v>
+        <v>601</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -5010,7 +4260,7 @@
         <v>389</v>
       </c>
       <c r="B9" t="s">
-        <v>857</v>
+        <v>629</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -5191,10 +4441,10 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>791</v>
+        <v>602</v>
       </c>
       <c r="B32" t="s">
-        <v>791</v>
+        <v>602</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -5330,7 +4580,7 @@
         <v>383</v>
       </c>
       <c r="B49" t="s">
-        <v>858</v>
+        <v>630</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
@@ -5367,7 +4617,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>800</v>
+        <v>604</v>
       </c>
       <c r="B54" t="s">
         <v>487</v>
@@ -5471,7 +4721,7 @@
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>834</v>
+        <v>612</v>
       </c>
       <c r="B67" t="s">
         <v>507</v>
@@ -5575,7 +4825,7 @@
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>860</v>
+        <v>632</v>
       </c>
       <c r="B80" t="s">
         <v>61</v>
@@ -5807,10 +5057,10 @@
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>882</v>
+        <v>647</v>
       </c>
       <c r="B109" t="s">
-        <v>878</v>
+        <v>644</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
@@ -6031,7 +5281,7 @@
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>798</v>
+        <v>603</v>
       </c>
       <c r="B137" t="s">
         <v>568</v>
@@ -6074,7 +5324,7 @@
         <v>393</v>
       </c>
       <c r="B142" t="s">
-        <v>836</v>
+        <v>614</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
@@ -6170,7 +5420,7 @@
         <v>385</v>
       </c>
       <c r="B154" t="s">
-        <v>859</v>
+        <v>631</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
@@ -6367,7 +5617,7 @@
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>870</v>
+        <v>638</v>
       </c>
       <c r="B179" t="s">
         <v>41</v>
@@ -6375,7 +5625,7 @@
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>871</v>
+        <v>639</v>
       </c>
       <c r="B180" t="s">
         <v>41</v>
@@ -6538,7 +5788,7 @@
         <v>291</v>
       </c>
       <c r="B200" t="s">
-        <v>878</v>
+        <v>644</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.25">
@@ -6567,7 +5817,7 @@
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>879</v>
+        <v>645</v>
       </c>
       <c r="B204" t="s">
         <v>553</v>
@@ -6738,7 +5988,7 @@
         <v>394</v>
       </c>
       <c r="B225" t="s">
-        <v>832</v>
+        <v>610</v>
       </c>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.25">
@@ -6746,12 +5996,12 @@
         <v>195</v>
       </c>
       <c r="B226" t="s">
-        <v>832</v>
+        <v>610</v>
       </c>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>811</v>
+        <v>609</v>
       </c>
       <c r="B227" t="s">
         <v>45</v>
@@ -6815,25 +6065,25 @@
     <sortCondition ref="A2:A35"/>
   </sortState>
   <conditionalFormatting sqref="A234:A1048576 A1:A53 A138:A179 A228:A232 A55:A136 A181:A226">
-    <cfRule type="duplicateValues" dxfId="7" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B233">
-    <cfRule type="duplicateValues" dxfId="6" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A233">
-    <cfRule type="duplicateValues" dxfId="5" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A137">
-    <cfRule type="duplicateValues" dxfId="4" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A227">
-    <cfRule type="duplicateValues" dxfId="3" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A54">
-    <cfRule type="duplicateValues" dxfId="2" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="13"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A180">
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -6841,1859 +6091,10 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:C176"/>
-  <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A98" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H109" sqref="H109"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="90.5703125" customWidth="1"/>
-    <col min="2" max="2" width="51.5703125" customWidth="1"/>
-    <col min="3" max="3" width="53.28515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>737</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>715</v>
-      </c>
-      <c r="B2" t="s">
-        <v>580</v>
-      </c>
-      <c r="C2" t="s">
-        <v>580</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>673</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>758</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>758</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>675</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>759</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>759</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>704</v>
-      </c>
-      <c r="B5" t="s">
-        <v>581</v>
-      </c>
-      <c r="C5" t="s">
-        <v>581</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>623</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>760</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>760</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>651</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>761</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>761</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>632</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>762</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>762</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>619</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>762</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>762</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>633</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>762</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>762</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>654</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>762</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>762</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>642</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>762</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>762</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>719</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>762</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>762</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>691</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>762</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>762</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>602</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>763</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>763</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>716</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>763</v>
-      </c>
-      <c r="C16" t="s">
-        <v>727</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>674</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>763</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>763</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>600</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>764</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>764</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>680</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>764</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>764</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>610</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>765</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>765</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>687</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>765</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>765</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>667</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>729</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>729</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>591</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>766</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>766</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>625</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>767</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>767</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>629</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>767</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>767</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>606</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>767</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>767</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>608</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>767</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>767</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>605</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>767</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>767</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>618</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>767</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>767</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>709</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>767</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>767</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>645</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>767</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>767</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>601</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>767</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>767</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>664</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>767</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>767</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>808</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>767</v>
-      </c>
-      <c r="C34" s="2"/>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>850</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>767</v>
-      </c>
-      <c r="C35" s="2"/>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>663</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>767</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>767</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>666</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>767</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>767</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>697</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>767</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>767</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>658</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>767</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>767</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>707</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>767</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>767</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>646</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>767</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>767</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>717</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>767</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>767</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>653</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>767</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>767</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>708</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>767</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>767</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>624</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>767</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>767</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>801</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>767</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>767</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>679</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>767</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>767</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>669</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>767</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>767</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>622</v>
-      </c>
-      <c r="B49" s="3" t="s">
-        <v>768</v>
-      </c>
-      <c r="C49" s="3" t="s">
-        <v>768</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>657</v>
-      </c>
-      <c r="B50" s="3" t="s">
-        <v>787</v>
-      </c>
-      <c r="C50" s="3" t="s">
-        <v>768</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>788</v>
-      </c>
-      <c r="B51" s="3" t="s">
-        <v>787</v>
-      </c>
-      <c r="C51" s="3"/>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>695</v>
-      </c>
-      <c r="B52" s="3" t="s">
-        <v>582</v>
-      </c>
-      <c r="C52" s="3" t="s">
-        <v>582</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>804</v>
-      </c>
-      <c r="B53" s="3" t="s">
-        <v>582</v>
-      </c>
-      <c r="C53" s="3" t="s">
-        <v>582</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>693</v>
-      </c>
-      <c r="B54" s="3" t="s">
-        <v>582</v>
-      </c>
-      <c r="C54" s="3" t="s">
-        <v>582</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>589</v>
-      </c>
-      <c r="B55" s="3" t="s">
-        <v>582</v>
-      </c>
-      <c r="C55" s="3" t="s">
-        <v>582</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>607</v>
-      </c>
-      <c r="B56" s="3" t="s">
-        <v>582</v>
-      </c>
-      <c r="C56" s="3" t="s">
-        <v>582</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>723</v>
-      </c>
-      <c r="B57" s="3" t="s">
-        <v>582</v>
-      </c>
-      <c r="C57" s="3" t="s">
-        <v>582</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>640</v>
-      </c>
-      <c r="B58" s="3" t="s">
-        <v>769</v>
-      </c>
-      <c r="C58" s="3" t="s">
-        <v>769</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>722</v>
-      </c>
-      <c r="B59" s="3" t="s">
-        <v>769</v>
-      </c>
-      <c r="C59" s="3" t="s">
-        <v>769</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>641</v>
-      </c>
-      <c r="B60" s="3" t="s">
-        <v>769</v>
-      </c>
-      <c r="C60" s="3" t="s">
-        <v>769</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>692</v>
-      </c>
-      <c r="B61" s="3" t="s">
-        <v>769</v>
-      </c>
-      <c r="C61" s="3" t="s">
-        <v>769</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>710</v>
-      </c>
-      <c r="B62" s="3" t="s">
-        <v>769</v>
-      </c>
-      <c r="C62" s="3" t="s">
-        <v>769</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>670</v>
-      </c>
-      <c r="B63" s="2" t="s">
-        <v>583</v>
-      </c>
-      <c r="C63" s="2" t="s">
-        <v>583</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>636</v>
-      </c>
-      <c r="B64" s="2" t="s">
-        <v>583</v>
-      </c>
-      <c r="C64" s="2" t="s">
-        <v>583</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>690</v>
-      </c>
-      <c r="B65" s="2" t="s">
-        <v>583</v>
-      </c>
-      <c r="C65" s="2" t="s">
-        <v>583</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>614</v>
-      </c>
-      <c r="B66" s="2" t="s">
-        <v>583</v>
-      </c>
-      <c r="C66" s="2" t="s">
-        <v>583</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>665</v>
-      </c>
-      <c r="B67" s="2" t="s">
-        <v>583</v>
-      </c>
-      <c r="C67" s="2" t="s">
-        <v>583</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>681</v>
-      </c>
-      <c r="B68" s="2" t="s">
-        <v>583</v>
-      </c>
-      <c r="C68" s="2" t="s">
-        <v>583</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>596</v>
-      </c>
-      <c r="B69" s="2" t="s">
-        <v>583</v>
-      </c>
-      <c r="C69" s="2" t="s">
-        <v>583</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>711</v>
-      </c>
-      <c r="B70" s="3" t="s">
-        <v>730</v>
-      </c>
-      <c r="C70" t="s">
-        <v>732</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>714</v>
-      </c>
-      <c r="B71" s="3" t="s">
-        <v>730</v>
-      </c>
-      <c r="C71" t="s">
-        <v>732</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A72" s="4" t="s">
-        <v>713</v>
-      </c>
-      <c r="B72" s="3" t="s">
-        <v>730</v>
-      </c>
-      <c r="C72" t="s">
-        <v>730</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>677</v>
-      </c>
-      <c r="B73" s="2" t="s">
-        <v>770</v>
-      </c>
-      <c r="C73" s="2" t="s">
-        <v>770</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>842</v>
-      </c>
-      <c r="B74" s="2" t="s">
-        <v>770</v>
-      </c>
-      <c r="C74" s="2" t="s">
-        <v>770</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
-        <v>631</v>
-      </c>
-      <c r="B75" s="2" t="s">
-        <v>770</v>
-      </c>
-      <c r="C75" s="2" t="s">
-        <v>770</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
-        <v>617</v>
-      </c>
-      <c r="B76" s="3" t="s">
-        <v>771</v>
-      </c>
-      <c r="C76" s="3" t="s">
-        <v>771</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
-        <v>702</v>
-      </c>
-      <c r="B77" s="3" t="s">
-        <v>584</v>
-      </c>
-      <c r="C77" s="3" t="s">
-        <v>584</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
-        <v>802</v>
-      </c>
-      <c r="B78" s="3" t="s">
-        <v>584</v>
-      </c>
-      <c r="C78" s="3" t="s">
-        <v>584</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
-        <v>812</v>
-      </c>
-      <c r="B79" s="3" t="s">
-        <v>584</v>
-      </c>
-      <c r="C79" s="3"/>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
-        <v>627</v>
-      </c>
-      <c r="B80" s="3" t="s">
-        <v>584</v>
-      </c>
-      <c r="C80" s="3" t="s">
-        <v>584</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
-        <v>686</v>
-      </c>
-      <c r="B81" s="3" t="s">
-        <v>584</v>
-      </c>
-      <c r="C81" s="3" t="s">
-        <v>584</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
-        <v>649</v>
-      </c>
-      <c r="B82" s="3" t="s">
-        <v>584</v>
-      </c>
-      <c r="C82" s="3" t="s">
-        <v>584</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
-        <v>586</v>
-      </c>
-      <c r="B83" s="3" t="s">
-        <v>584</v>
-      </c>
-      <c r="C83" s="3" t="s">
-        <v>584</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
-        <v>639</v>
-      </c>
-      <c r="B84" s="2" t="s">
-        <v>757</v>
-      </c>
-      <c r="C84" s="2" t="s">
-        <v>757</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
-        <v>699</v>
-      </c>
-      <c r="B85" s="2" t="s">
-        <v>757</v>
-      </c>
-      <c r="C85" s="2" t="s">
-        <v>757</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
-        <v>587</v>
-      </c>
-      <c r="B86" s="2" t="s">
-        <v>757</v>
-      </c>
-      <c r="C86" s="2" t="s">
-        <v>757</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
-        <v>799</v>
-      </c>
-      <c r="B87" s="2" t="s">
-        <v>757</v>
-      </c>
-      <c r="C87" s="2" t="s">
-        <v>757</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
-        <v>598</v>
-      </c>
-      <c r="B88" s="3" t="s">
-        <v>731</v>
-      </c>
-      <c r="C88" s="3" t="s">
-        <v>731</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
-        <v>595</v>
-      </c>
-      <c r="B89" s="2" t="s">
-        <v>772</v>
-      </c>
-      <c r="C89" s="2" t="s">
-        <v>772</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
-        <v>592</v>
-      </c>
-      <c r="B90" s="3" t="s">
-        <v>773</v>
-      </c>
-      <c r="C90" s="3" t="s">
-        <v>773</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
-        <v>590</v>
-      </c>
-      <c r="B91" s="2" t="s">
-        <v>774</v>
-      </c>
-      <c r="C91" s="2" t="s">
-        <v>774</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
-        <v>615</v>
-      </c>
-      <c r="B92" s="3" t="s">
-        <v>775</v>
-      </c>
-      <c r="C92" s="3" t="s">
-        <v>775</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
-        <v>717</v>
-      </c>
-      <c r="B93" s="2" t="s">
-        <v>776</v>
-      </c>
-      <c r="C93" s="2" t="s">
-        <v>776</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
-        <v>880</v>
-      </c>
-      <c r="B94" t="s">
-        <v>880</v>
-      </c>
-      <c r="C94" t="s">
-        <v>880</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
-        <v>612</v>
-      </c>
-      <c r="B95" s="2" t="s">
-        <v>728</v>
-      </c>
-      <c r="C95" s="2" t="s">
-        <v>728</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
-        <v>634</v>
-      </c>
-      <c r="B96" s="2" t="s">
-        <v>728</v>
-      </c>
-      <c r="C96" s="2" t="s">
-        <v>728</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
-        <v>718</v>
-      </c>
-      <c r="B97" s="2" t="s">
-        <v>728</v>
-      </c>
-      <c r="C97" s="2"/>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
-        <v>672</v>
-      </c>
-      <c r="B98" s="2" t="s">
-        <v>728</v>
-      </c>
-      <c r="C98" s="2" t="s">
-        <v>728</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
-        <v>861</v>
-      </c>
-      <c r="B99" s="2" t="s">
-        <v>728</v>
-      </c>
-      <c r="C99" s="2"/>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A100" t="s">
-        <v>793</v>
-      </c>
-      <c r="B100" s="2" t="s">
-        <v>728</v>
-      </c>
-      <c r="C100" s="2" t="s">
-        <v>728</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A101" t="s">
-        <v>795</v>
-      </c>
-      <c r="B101" s="2" t="s">
-        <v>728</v>
-      </c>
-      <c r="C101" s="2"/>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A102" t="s">
-        <v>678</v>
-      </c>
-      <c r="B102" s="2" t="s">
-        <v>728</v>
-      </c>
-      <c r="C102" s="2" t="s">
-        <v>728</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A103" t="s">
-        <v>652</v>
-      </c>
-      <c r="B103" s="2" t="s">
-        <v>728</v>
-      </c>
-      <c r="C103" s="2" t="s">
-        <v>728</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A104" t="s">
-        <v>630</v>
-      </c>
-      <c r="B104" s="2" t="s">
-        <v>728</v>
-      </c>
-      <c r="C104" s="2" t="s">
-        <v>728</v>
-      </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A105" t="s">
-        <v>609</v>
-      </c>
-      <c r="B105" s="2" t="s">
-        <v>777</v>
-      </c>
-      <c r="C105" s="2" t="s">
-        <v>777</v>
-      </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A106" t="s">
-        <v>873</v>
-      </c>
-      <c r="B106" s="2" t="s">
-        <v>777</v>
-      </c>
-      <c r="C106" s="2" t="s">
-        <v>777</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A107" t="s">
-        <v>792</v>
-      </c>
-      <c r="B107" s="2" t="s">
-        <v>777</v>
-      </c>
-      <c r="C107" s="2"/>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A108" t="s">
-        <v>676</v>
-      </c>
-      <c r="B108" s="2" t="s">
-        <v>585</v>
-      </c>
-      <c r="C108" s="2" t="s">
-        <v>585</v>
-      </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A109" t="s">
-        <v>813</v>
-      </c>
-      <c r="B109" s="2" t="s">
-        <v>585</v>
-      </c>
-      <c r="C109" s="2"/>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A110" t="s">
-        <v>683</v>
-      </c>
-      <c r="B110" s="2" t="s">
-        <v>585</v>
-      </c>
-      <c r="C110" s="2" t="s">
-        <v>585</v>
-      </c>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A111" t="s">
-        <v>85</v>
-      </c>
-      <c r="B111" s="2" t="s">
-        <v>585</v>
-      </c>
-      <c r="C111" s="2"/>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A112" t="s">
-        <v>684</v>
-      </c>
-      <c r="B112" s="2" t="s">
-        <v>585</v>
-      </c>
-      <c r="C112" s="2" t="s">
-        <v>585</v>
-      </c>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A113" t="s">
-        <v>685</v>
-      </c>
-      <c r="B113" s="2" t="s">
-        <v>585</v>
-      </c>
-      <c r="C113" s="2" t="s">
-        <v>585</v>
-      </c>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A114" t="s">
-        <v>635</v>
-      </c>
-      <c r="B114" s="2" t="s">
-        <v>585</v>
-      </c>
-      <c r="C114" s="2" t="s">
-        <v>585</v>
-      </c>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A115" t="s">
-        <v>668</v>
-      </c>
-      <c r="B115" s="2" t="s">
-        <v>585</v>
-      </c>
-      <c r="C115" s="2" t="s">
-        <v>585</v>
-      </c>
-    </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A116" t="s">
-        <v>599</v>
-      </c>
-      <c r="B116" s="2" t="s">
-        <v>585</v>
-      </c>
-      <c r="C116" s="2" t="s">
-        <v>585</v>
-      </c>
-    </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A117" t="s">
-        <v>696</v>
-      </c>
-      <c r="B117" s="2" t="s">
-        <v>585</v>
-      </c>
-      <c r="C117" s="2" t="s">
-        <v>585</v>
-      </c>
-    </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A118" t="s">
-        <v>701</v>
-      </c>
-      <c r="B118" s="2" t="s">
-        <v>778</v>
-      </c>
-      <c r="C118" s="2" t="s">
-        <v>778</v>
-      </c>
-    </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A119" t="s">
-        <v>682</v>
-      </c>
-      <c r="B119" s="2" t="s">
-        <v>778</v>
-      </c>
-      <c r="C119" s="2" t="s">
-        <v>778</v>
-      </c>
-    </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A120" t="s">
-        <v>688</v>
-      </c>
-      <c r="B120" s="2" t="s">
-        <v>778</v>
-      </c>
-      <c r="C120" s="2" t="s">
-        <v>778</v>
-      </c>
-    </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A121" t="s">
-        <v>689</v>
-      </c>
-      <c r="B121" s="2" t="s">
-        <v>778</v>
-      </c>
-      <c r="C121" s="2" t="s">
-        <v>778</v>
-      </c>
-    </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A122" t="s">
-        <v>604</v>
-      </c>
-      <c r="B122" s="2" t="s">
-        <v>778</v>
-      </c>
-      <c r="C122" s="2" t="s">
-        <v>778</v>
-      </c>
-    </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A123" t="s">
-        <v>720</v>
-      </c>
-      <c r="B123" s="3" t="s">
-        <v>779</v>
-      </c>
-      <c r="C123" s="3" t="s">
-        <v>779</v>
-      </c>
-    </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A124" t="s">
-        <v>650</v>
-      </c>
-      <c r="B124" s="3" t="s">
-        <v>779</v>
-      </c>
-      <c r="C124" s="3" t="s">
-        <v>779</v>
-      </c>
-    </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A125" t="s">
-        <v>594</v>
-      </c>
-      <c r="B125" s="3" t="s">
-        <v>733</v>
-      </c>
-      <c r="C125" s="3" t="s">
-        <v>733</v>
-      </c>
-    </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A126" t="s">
-        <v>588</v>
-      </c>
-      <c r="B126" s="3" t="s">
-        <v>733</v>
-      </c>
-      <c r="C126" s="3" t="s">
-        <v>733</v>
-      </c>
-    </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A127" t="s">
-        <v>593</v>
-      </c>
-      <c r="B127" s="3" t="s">
-        <v>733</v>
-      </c>
-      <c r="C127" t="s">
-        <v>735</v>
-      </c>
-    </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A128" t="s">
-        <v>597</v>
-      </c>
-      <c r="B128" s="3" t="s">
-        <v>733</v>
-      </c>
-      <c r="C128" t="s">
-        <v>735</v>
-      </c>
-    </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A129" t="s">
-        <v>724</v>
-      </c>
-      <c r="B129" s="3" t="s">
-        <v>733</v>
-      </c>
-      <c r="C129" t="s">
-        <v>735</v>
-      </c>
-    </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A130" t="s">
-        <v>726</v>
-      </c>
-      <c r="B130" s="3" t="s">
-        <v>733</v>
-      </c>
-      <c r="C130" t="s">
-        <v>735</v>
-      </c>
-    </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A131" t="s">
-        <v>725</v>
-      </c>
-      <c r="B131" s="3" t="s">
-        <v>733</v>
-      </c>
-      <c r="C131" t="s">
-        <v>735</v>
-      </c>
-    </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A132" t="s">
-        <v>671</v>
-      </c>
-      <c r="B132" s="3" t="s">
-        <v>734</v>
-      </c>
-      <c r="C132" s="3" t="s">
-        <v>734</v>
-      </c>
-    </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A133" t="s">
-        <v>616</v>
-      </c>
-      <c r="B133" s="3" t="s">
-        <v>780</v>
-      </c>
-      <c r="C133" s="3" t="s">
-        <v>780</v>
-      </c>
-    </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A134" t="s">
-        <v>659</v>
-      </c>
-      <c r="B134" s="2" t="s">
-        <v>781</v>
-      </c>
-      <c r="C134" s="2" t="s">
-        <v>781</v>
-      </c>
-    </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A135" t="s">
-        <v>874</v>
-      </c>
-      <c r="B135" s="2" t="s">
-        <v>781</v>
-      </c>
-      <c r="C135" s="2" t="s">
-        <v>781</v>
-      </c>
-    </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A136" t="s">
-        <v>611</v>
-      </c>
-      <c r="B136" s="2" t="s">
-        <v>782</v>
-      </c>
-      <c r="C136" s="2" t="s">
-        <v>782</v>
-      </c>
-    </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A137" t="s">
-        <v>648</v>
-      </c>
-      <c r="B137" s="2" t="s">
-        <v>782</v>
-      </c>
-      <c r="C137" s="2" t="s">
-        <v>782</v>
-      </c>
-    </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A138" t="s">
-        <v>626</v>
-      </c>
-      <c r="B138" s="2" t="s">
-        <v>782</v>
-      </c>
-      <c r="C138" s="2" t="s">
-        <v>782</v>
-      </c>
-    </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A139" t="s">
-        <v>807</v>
-      </c>
-      <c r="B139" s="2" t="s">
-        <v>782</v>
-      </c>
-      <c r="C139" s="2"/>
-    </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A140" t="s">
-        <v>613</v>
-      </c>
-      <c r="B140" s="3" t="s">
-        <v>783</v>
-      </c>
-      <c r="C140" s="3" t="s">
-        <v>783</v>
-      </c>
-    </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A141" t="s">
-        <v>794</v>
-      </c>
-      <c r="B141" s="3" t="s">
-        <v>783</v>
-      </c>
-      <c r="C141" s="3"/>
-    </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A142" t="s">
-        <v>644</v>
-      </c>
-      <c r="B142" s="2" t="s">
-        <v>784</v>
-      </c>
-      <c r="C142" s="2" t="s">
-        <v>784</v>
-      </c>
-    </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A143" t="s">
-        <v>620</v>
-      </c>
-      <c r="B143" s="2" t="s">
-        <v>785</v>
-      </c>
-      <c r="C143" s="2" t="s">
-        <v>785</v>
-      </c>
-    </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A144" t="s">
-        <v>638</v>
-      </c>
-      <c r="B144" s="3" t="s">
-        <v>786</v>
-      </c>
-      <c r="C144" s="3" t="s">
-        <v>786</v>
-      </c>
-    </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A145" t="s">
-        <v>789</v>
-      </c>
-      <c r="B145" s="3" t="s">
-        <v>786</v>
-      </c>
-      <c r="C145" s="3" t="s">
-        <v>786</v>
-      </c>
-    </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A146" t="s">
-        <v>64</v>
-      </c>
-      <c r="B146" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A147" t="s">
-        <v>603</v>
-      </c>
-      <c r="B147" t="s">
-        <v>815</v>
-      </c>
-    </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A148" t="s">
-        <v>703</v>
-      </c>
-      <c r="B148" t="s">
-        <v>816</v>
-      </c>
-    </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A149" t="s">
-        <v>698</v>
-      </c>
-      <c r="B149" t="s">
-        <v>817</v>
-      </c>
-    </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A150" t="s">
-        <v>694</v>
-      </c>
-      <c r="B150" t="s">
-        <v>796</v>
-      </c>
-    </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A151" t="s">
-        <v>797</v>
-      </c>
-      <c r="B151" t="s">
-        <v>796</v>
-      </c>
-    </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A152" t="s">
-        <v>806</v>
-      </c>
-      <c r="B152" t="s">
-        <v>796</v>
-      </c>
-    </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A153" t="s">
-        <v>718</v>
-      </c>
-      <c r="B153" t="s">
-        <v>831</v>
-      </c>
-    </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A154" t="s">
-        <v>706</v>
-      </c>
-      <c r="B154" t="s">
-        <v>818</v>
-      </c>
-    </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A155" t="s">
-        <v>705</v>
-      </c>
-      <c r="B155" t="s">
-        <v>819</v>
-      </c>
-    </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A156" t="s">
-        <v>721</v>
-      </c>
-      <c r="B156" t="s">
-        <v>849</v>
-      </c>
-    </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A157" t="s">
-        <v>655</v>
-      </c>
-      <c r="B157" t="s">
-        <v>820</v>
-      </c>
-    </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A158" t="s">
-        <v>656</v>
-      </c>
-      <c r="B158" t="s">
-        <v>821</v>
-      </c>
-    </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A159" t="s">
-        <v>637</v>
-      </c>
-      <c r="B159" t="s">
-        <v>822</v>
-      </c>
-    </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A160" t="s">
-        <v>94</v>
-      </c>
-      <c r="B160" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A161" t="s">
-        <v>660</v>
-      </c>
-      <c r="B161" t="s">
-        <v>830</v>
-      </c>
-    </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A162" t="s">
-        <v>72</v>
-      </c>
-      <c r="B162" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A163" t="s">
-        <v>621</v>
-      </c>
-      <c r="B163" t="s">
-        <v>823</v>
-      </c>
-    </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A164" t="s">
-        <v>700</v>
-      </c>
-      <c r="B164" t="s">
-        <v>824</v>
-      </c>
-    </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A165" t="s">
-        <v>647</v>
-      </c>
-      <c r="B165" t="s">
-        <v>814</v>
-      </c>
-    </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A166" t="s">
-        <v>628</v>
-      </c>
-      <c r="B166" t="s">
-        <v>826</v>
-      </c>
-    </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A167" t="s">
-        <v>712</v>
-      </c>
-      <c r="B167" t="s">
-        <v>827</v>
-      </c>
-    </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A168" t="s">
-        <v>662</v>
-      </c>
-      <c r="B168" t="s">
-        <v>825</v>
-      </c>
-    </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A169" t="s">
-        <v>661</v>
-      </c>
-      <c r="B169" t="s">
-        <v>828</v>
-      </c>
-    </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A170" t="s">
-        <v>643</v>
-      </c>
-      <c r="B170" t="s">
-        <v>829</v>
-      </c>
-    </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A171" t="s">
-        <v>846</v>
-      </c>
-      <c r="B171" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A172" t="s">
-        <v>847</v>
-      </c>
-      <c r="B172" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A173" t="s">
-        <v>851</v>
-      </c>
-      <c r="B173" t="s">
-        <v>582</v>
-      </c>
-    </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A174" t="s">
-        <v>866</v>
-      </c>
-      <c r="B174" s="2" t="s">
-        <v>767</v>
-      </c>
-    </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A175" s="5" t="s">
-        <v>868</v>
-      </c>
-      <c r="B175" s="2" t="s">
-        <v>767</v>
-      </c>
-    </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A176" s="5" t="s">
-        <v>869</v>
-      </c>
-      <c r="B176" t="s">
-        <v>25</v>
-      </c>
-    </row>
-  </sheetData>
-  <autoFilter ref="A1:C1" xr:uid="{00000000-0009-0000-0000-000005000000}">
-    <sortState ref="A2:C151">
-      <sortCondition ref="B1"/>
-    </sortState>
-  </autoFilter>
-  <conditionalFormatting sqref="A1">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
@@ -8713,90 +6114,90 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>848</v>
+        <v>623</v>
       </c>
       <c r="B2" t="s">
-        <v>841</v>
+        <v>619</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>747</v>
+        <v>591</v>
       </c>
       <c r="B3" t="s">
-        <v>738</v>
+        <v>582</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>748</v>
+        <v>592</v>
       </c>
       <c r="B4" t="s">
-        <v>738</v>
+        <v>582</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>739</v>
+        <v>583</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>740</v>
+        <v>584</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>741</v>
+        <v>585</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>742</v>
+        <v>586</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>743</v>
+        <v>587</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>744</v>
+        <v>588</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>745</v>
+        <v>589</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>746</v>
+        <v>590</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>750</v>
+        <v>594</v>
       </c>
       <c r="B13" t="s">
-        <v>841</v>
+        <v>619</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>837</v>
+        <v>615</v>
       </c>
       <c r="B14" t="s">
-        <v>841</v>
+        <v>619</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>749</v>
+        <v>593</v>
       </c>
       <c r="B15" t="s">
-        <v>841</v>
+        <v>619</v>
       </c>
     </row>
   </sheetData>
@@ -8805,7 +6206,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:B10"/>
   <sheetViews>
@@ -8829,18 +6230,18 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>752</v>
+        <v>596</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>853</v>
+        <v>625</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>753</v>
+        <v>597</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>854</v>
+        <v>626</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -8848,36 +6249,36 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>854</v>
+        <v>626</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>754</v>
+        <v>598</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>854</v>
+        <v>626</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>756</v>
+        <v>600</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>856</v>
+        <v>628</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>751</v>
+        <v>595</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>855</v>
+        <v>627</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>755</v>
+        <v>599</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
fixed lookup table for mode 0f data collection
</commit_message>
<xml_diff>
--- a/data-raw/control_vocab_mapping.xlsx
+++ b/data-raw/control_vocab_mapping.xlsx
@@ -8,23 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WB525812\cmder\Git Repos\mdlibtoddh\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B50C3C26-AF22-4A15-BA20-DD415EBA968A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{590854F0-2327-499D-AAAC-0BE2BF1FD823}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="10770" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="10770" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dataClassification" sheetId="1" r:id="rId1"/>
     <sheet name="termsofUse" sheetId="2" r:id="rId2"/>
     <sheet name="kindData" sheetId="3" r:id="rId3"/>
-    <sheet name="modeDataColl" sheetId="4" r:id="rId4"/>
-    <sheet name="geographicalCoverage" sheetId="5" r:id="rId5"/>
-    <sheet name="source" sheetId="7" r:id="rId6"/>
-    <sheet name="license" sheetId="8" r:id="rId7"/>
+    <sheet name="geographicalCoverage" sheetId="5" r:id="rId4"/>
+    <sheet name="source" sheetId="7" r:id="rId5"/>
+    <sheet name="license" sheetId="8" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">geographicalCoverage!$A$1:$B$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">geographicalCoverage!$A$1:$B$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">kindData!$A$1:$B$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">modeDataColl!$A$1:$C$1</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -36,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="919" uniqueCount="648">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="650" uniqueCount="538">
   <si>
     <t>microdata_category</t>
   </si>
@@ -113,30 +111,6 @@
     <t>Geo-Spatial data</t>
   </si>
   <si>
-    <t>Other</t>
-  </si>
-  <si>
-    <t>Computer Assisted Personal Interview</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Face-to-face</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Mail Questionnaire</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Focus Group</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Internet</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Other </t>
-  </si>
-  <si>
-    <t>Computer Assisted Telephone Interview</t>
-  </si>
-  <si>
     <t>Bhutan</t>
   </si>
   <si>
@@ -347,252 +321,6 @@
     <t>Sample survey data;Administrative records data</t>
   </si>
   <si>
-    <t>face-to-face [f2f]</t>
-  </si>
-  <si>
-    <t>face-to-face</t>
-  </si>
-  <si>
-    <t>other [oth]</t>
-  </si>
-  <si>
-    <t>internet [int]</t>
-  </si>
-  <si>
-    <t>face-to-face [f2f] and interviewer observation</t>
-  </si>
-  <si>
-    <t>mail questionnaire</t>
-  </si>
-  <si>
-    <t>interview face à face [f2f]</t>
-  </si>
-  <si>
-    <t>other [oth] mixed method: self accomplished, mailed, face to face</t>
-  </si>
-  <si>
-    <t>other [oth] mixed method self-accomplished, mailed and face to face</t>
-  </si>
-  <si>
-    <t>other [oth] mixed method:  self-accomplished, mailed, face-to-face</t>
-  </si>
-  <si>
-    <t>other [oth], mixed method: self-accomplished, mailed and face-to-face</t>
-  </si>
-  <si>
-    <t>other [oth] mixed method: self-accomplished, mailed, face-to-face</t>
-  </si>
-  <si>
-    <t>focus group [foc] / face-to-face, key informants</t>
-  </si>
-  <si>
-    <t>other [oth] - self administered administrative form</t>
-  </si>
-  <si>
-    <t>other [oth] - self-administered administrative form</t>
-  </si>
-  <si>
-    <t>self administered questionnaire and/or face-to-face interview</t>
-  </si>
-  <si>
-    <t>other [oth]- self administered administrative form</t>
-  </si>
-  <si>
-    <t>mail questionnaire [mail]</t>
-  </si>
-  <si>
-    <t>computer assisted personal interview [capi]</t>
-  </si>
-  <si>
-    <t>face-to-face [f2f] papi</t>
-  </si>
-  <si>
-    <t>face-to-face [f2f], papi</t>
-  </si>
-  <si>
-    <t>face-to-face [f2f], capi</t>
-  </si>
-  <si>
-    <t>face-to-face [f2f]f</t>
-  </si>
-  <si>
-    <t>landline and cellular telephone</t>
-  </si>
-  <si>
-    <t>landline telephone</t>
-  </si>
-  <si>
-    <t>face-to-face [f2f] and landline telephone</t>
-  </si>
-  <si>
-    <t>cellular telephone</t>
-  </si>
-  <si>
-    <t>face-to-face [f2f</t>
-  </si>
-  <si>
-    <t>face-to-face [f2f] or landline telephone or landline and cellular telephone</t>
-  </si>
-  <si>
-    <t>face-to-face [f2f], and self enumerated</t>
-  </si>
-  <si>
-    <t>self administered and face to face</t>
-  </si>
-  <si>
-    <t>face-to-face [f2f]; self-administered</t>
-  </si>
-  <si>
-    <t>both self-administered and face-to-face</t>
-  </si>
-  <si>
-    <t>both self-administered and face to face</t>
-  </si>
-  <si>
-    <t>face-to-face [f2f] for questionnaires, self-enumeration for the diaries</t>
-  </si>
-  <si>
-    <t>statutory return submitted by factories as well  as face to face</t>
-  </si>
-  <si>
-    <t>entrevista con encuestadores (cara a cara [f2f])</t>
-  </si>
-  <si>
-    <t>entrevista con asistencia de computador personal [capi]</t>
-  </si>
-  <si>
-    <t>telephone interview</t>
-  </si>
-  <si>
-    <t>not specified</t>
-  </si>
-  <si>
-    <t>computer assisted telephone interview [cati]</t>
-  </si>
-  <si>
-    <t>mixed</t>
-  </si>
-  <si>
-    <t>cara a cara [f2f]</t>
-  </si>
-  <si>
-    <t>entrevista directa con formato de captación a papel</t>
-  </si>
-  <si>
-    <t>focus group</t>
-  </si>
-  <si>
-    <t>entrevista personal [f2f]</t>
-  </si>
-  <si>
-    <t>entrevista presencial con documento impreso</t>
-  </si>
-  <si>
-    <t>cara a cara</t>
-  </si>
-  <si>
-    <t>entrevista directa [f2f]</t>
-  </si>
-  <si>
-    <t>cara à cara [f2f]</t>
-  </si>
-  <si>
-    <t>entrevista personal con formulario de papel</t>
-  </si>
-  <si>
-    <t>autodiligenciamiento por correo</t>
-  </si>
-  <si>
-    <t>otro método</t>
-  </si>
-  <si>
-    <t>autodiligenciamiento asistido con dmc</t>
-  </si>
-  <si>
-    <t>autodiligenciamiento por correo [mail]</t>
-  </si>
-  <si>
-    <t>face-to-face interview</t>
-  </si>
-  <si>
-    <t>face-to-face interview; self-completion</t>
-  </si>
-  <si>
-    <t>face-to-face interview; self-completion; educational measurements; observation</t>
-  </si>
-  <si>
-    <t>autodiligenciamiento libre con formulario electrónico vía página web</t>
-  </si>
-  <si>
-    <t>entrevista personal asistida con dmc (dispositivo móvil de captura)</t>
-  </si>
-  <si>
-    <t>autodiligenciamiento asistido con formulario electrónico vía página web</t>
-  </si>
-  <si>
-    <t>entrevista telefónica</t>
-  </si>
-  <si>
-    <t>entrevista personal asistida por computador</t>
-  </si>
-  <si>
-    <t>autodiligenciamiento de formulario electrónico vía página web (por selección; por ejemplo en encuestas por muestreo o censos)</t>
-  </si>
-  <si>
-    <t>proxy respondent [proxy] &amp; face-to-face [ftf]</t>
-  </si>
-  <si>
-    <t>proxy respondent [proxy]</t>
-  </si>
-  <si>
-    <t>entrevista directa asistida por dispositivo de cómputo móvil</t>
-  </si>
-  <si>
-    <t>face-to-face interviews were used to collect data.</t>
-  </si>
-  <si>
-    <t>household-, community-, and health center-level surveys</t>
-  </si>
-  <si>
-    <t>face to face personal interview using paper and pencil questionnaire (papi).</t>
-  </si>
-  <si>
-    <t>the data collection method used is household survey conducted in two selected urban areas in nampula province, northern mozambique. the data were collected by interviewing the head of the households using a structured questionnaire. the questionnaire included more than 25 sections encompassing modules on: household characteristics (demographic information by each member of the hh); employment and sources of any other cash transfers; identification and list of all the parcels; land conflicts; rights to the land and perceptions of the risk; parcels rented out, rented in; characteristics of parcels; investments on land; perceptions about the duat, renting land and the land law; relative space occupied by crops in the plot; production and sales of basic food crops, cash crops, vegetables, fruits, nuts, etc.; agricultural practices; ownership of assets; monthly expenditures; credit in the last 12 months; livestock and sub-products produced and sold in the last 12 months; and consumption   each of the survey households were geo-referenced for ease of locating them for the panel survey. in households that were male-headed with a spouse present, the spouse was the respondent for the livestock and food consumption modules. the survey was designed to take between 1 and 1 ½ hours to complete.</t>
-  </si>
-  <si>
-    <t>data collection methods include: semi-structured interviews with staff, educators, government officials, and other key informants; a survey of rsrc patrons; panels of secondary students and business people who have used an rsrc; the most significant change technique;  focus groups;  observations;  document analysis, including system-generated data, administrative records, and online media sources</t>
-  </si>
-  <si>
-    <t>face-to-face paper-and-pencil interviews (papi)</t>
-  </si>
-  <si>
-    <t>the data were collected using paper questionnaires with concurrent data entry in the field using computer assisted field entry (cafe)</t>
-  </si>
-  <si>
-    <t>Other;Mail Questionnaire; Face-to-face</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Focus Group; Face-to-face</t>
-  </si>
-  <si>
-    <t>Other;Face-to-face</t>
-  </si>
-  <si>
-    <t>Computer Assisted Telephone Interview;</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Face-to-face;Computer Assisted Telephone Interview</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Face-to-face;Other</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Face-to-face;Other </t>
-  </si>
-  <si>
-    <t>Internet</t>
-  </si>
-  <si>
     <t>bhutan</t>
   </si>
   <si>
@@ -1853,18 +1581,9 @@
     <t>Cote d’Ivoire</t>
   </si>
   <si>
-    <t>statutory return submitted by factories as well as face to face</t>
-  </si>
-  <si>
     <t>encuesta probabilística en establecimientos</t>
   </si>
   <si>
-    <t xml:space="preserve"> Face-to-face;internet [int]</t>
-  </si>
-  <si>
-    <t>face-to-face [f2f], internet [int]</t>
-  </si>
-  <si>
     <t>viet nam</t>
   </si>
   <si>
@@ -1877,42 +1596,18 @@
     <t>egypt</t>
   </si>
   <si>
-    <t>Mode of Data Collection not specified</t>
-  </si>
-  <si>
     <t>Montserrat</t>
   </si>
   <si>
     <t>this series of savvy mortality surveillance system manuals, guides, and other documents is available at the measure evaluation\nweb site at: http://www.cpc.unc.edu/measure/leadership/savvy.html</t>
   </si>
   <si>
-    <t>self-administered</t>
-  </si>
-  <si>
-    <t>Mail Questionnaire</t>
-  </si>
-  <si>
-    <t>the data collection method used is household survey conducted in two selected urban areas in nampula province, northern mozambique. the data were collected by interviewing the head of the households using a structured questionnaire. the questionnaire included more than 25 sections encompassing modules on: household characteristics (demographic information by each member of the hh); employment and sources of any other cash transfers; identification and list of all the parcels; land conflicts; rights to the land and perceptions of the risk; parcels rented out, rented in; characteristics of parcels; investments on land; perceptions about the duat, renting land and the land law; relative space occupied by crops in the plot; production and sales of basic food crops, cash crops, vegetables, fruits, nuts, etc.; agricultural practices; ownership of assets; monthly expenditures; credit in the last 12 months; livestock and sub-products produced and sold in the last 12 months; and consumption \n\neach of the survey households were geo-referenced for ease of locating them for the panel survey. in households that were male-headed with a spouse present, the spouse was the respondent for the livestock and food consumption modules. the survey was designed to take between 1 and 1 ½ hours to complete.</t>
-  </si>
-  <si>
     <t>Source not specified</t>
   </si>
   <si>
-    <t>face-to-face[f2f]</t>
-  </si>
-  <si>
-    <t>face-to-face interview [f2f] and self-administered</t>
-  </si>
-  <si>
-    <t>questionnaire envoyé [mail]</t>
-  </si>
-  <si>
     <t>this series of savvy mortality surveillance system manuals, guides, and other documents is available at the measure evaluation\\nweb site at: http://www.cpc.unc.edu/measure/leadership/savvy.html</t>
   </si>
   <si>
-    <t>paper and pencil</t>
-  </si>
-  <si>
     <t>Creative Commons Attribution 4.0</t>
   </si>
   <si>
@@ -1937,18 +1632,6 @@
     <t>gambia</t>
   </si>
   <si>
-    <t xml:space="preserve">Other </t>
-  </si>
-  <si>
-    <t>Face-to-face</t>
-  </si>
-  <si>
-    <t>Focus Group</t>
-  </si>
-  <si>
-    <t>please see: http://www.europeansocialsurvey.org/essdoc/doc.html?year=2012&amp;ddi=2.3.1.6</t>
-  </si>
-  <si>
     <t>Sample survey data[ssd]</t>
   </si>
   <si>
@@ -1958,25 +1641,10 @@
     <t>sénégal</t>
   </si>
   <si>
-    <t>Face_to_Face</t>
-  </si>
-  <si>
-    <t>Par téléphone [cati]</t>
-  </si>
-  <si>
-    <t>Interview de groupe [foc]</t>
-  </si>
-  <si>
-    <t>Visita personal, vía correo o llamada telefónica</t>
-  </si>
-  <si>
     <t>Eswatini</t>
   </si>
   <si>
     <t>Taiwan China</t>
-  </si>
-  <si>
-    <t>Other[oth]</t>
   </si>
   <si>
     <t>Kingdom of Eswatini</t>
@@ -2029,107 +1697,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="17">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="7">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -2535,7 +2103,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>580</v>
+        <v>490</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -2575,7 +2143,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>596</v>
+        <v>506</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>5</v>
@@ -2583,7 +2151,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>597</v>
+        <v>507</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>6</v>
@@ -2599,7 +2167,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>598</v>
+        <v>508</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>8</v>
@@ -2607,7 +2175,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>600</v>
+        <v>510</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>9</v>
@@ -2615,7 +2183,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>595</v>
+        <v>505</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>10</v>
@@ -2623,7 +2191,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>599</v>
+        <v>509</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>11</v>
@@ -2670,12 +2238,12 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>581</v>
+        <v>491</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="B2" t="s">
         <v>14</v>
@@ -2686,7 +2254,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="B3" t="s">
         <v>14</v>
@@ -2697,7 +2265,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="B4" t="s">
         <v>15</v>
@@ -2708,7 +2276,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="B5" t="s">
         <v>17</v>
@@ -2719,7 +2287,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="B6" t="s">
         <v>20</v>
@@ -2754,23 +2322,23 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="B10" t="s">
-        <v>611</v>
+        <v>518</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="B11" t="s">
-        <v>611</v>
+        <v>518</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="B12" t="s">
         <v>16</v>
@@ -2781,7 +2349,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="B13" t="s">
         <v>16</v>
@@ -2792,7 +2360,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="B14" t="s">
         <v>15</v>
@@ -2803,7 +2371,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="B15" t="s">
         <v>15</v>
@@ -2814,7 +2382,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="B16" t="s">
         <v>18</v>
@@ -2825,7 +2393,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="B17" t="s">
         <v>14</v>
@@ -2836,7 +2404,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="B18" t="s">
         <v>21</v>
@@ -2847,7 +2415,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="B19" t="s">
         <v>14</v>
@@ -2858,7 +2426,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="B20" t="s">
         <v>14</v>
@@ -2869,7 +2437,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="B21" t="s">
         <v>14</v>
@@ -2880,7 +2448,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="B22" t="s">
         <v>14</v>
@@ -2891,7 +2459,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="B23" t="s">
         <v>14</v>
@@ -2902,7 +2470,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="B24" t="s">
         <v>14</v>
@@ -2913,7 +2481,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="B25" t="s">
         <v>14</v>
@@ -2924,7 +2492,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="B26" t="s">
         <v>14</v>
@@ -2935,7 +2503,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="B27" t="s">
         <v>14</v>
@@ -2946,7 +2514,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="B28" t="s">
         <v>14</v>
@@ -2957,7 +2525,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="B29" t="s">
         <v>16</v>
@@ -2968,7 +2536,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="B30" t="s">
         <v>19</v>
@@ -2979,7 +2547,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="B31" t="s">
         <v>19</v>
@@ -2990,7 +2558,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="B32" t="s">
         <v>14</v>
@@ -3001,7 +2569,7 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="B33" t="s">
         <v>14</v>
@@ -3012,15 +2580,15 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="B34" t="s">
-        <v>611</v>
+        <v>518</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="B35" t="s">
         <v>14</v>
@@ -3031,7 +2599,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="B36" t="s">
         <v>16</v>
@@ -3042,7 +2610,7 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="B37" t="s">
         <v>21</v>
@@ -3053,7 +2621,7 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="B38" t="s">
         <v>16</v>
@@ -3064,18 +2632,18 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="B39" t="s">
         <v>14</v>
       </c>
       <c r="C39" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="B40" t="s">
         <v>14</v>
@@ -3086,7 +2654,7 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="B41" t="s">
         <v>14</v>
@@ -3097,7 +2665,7 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="B42" t="s">
         <v>16</v>
@@ -3105,7 +2673,7 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>606</v>
+        <v>515</v>
       </c>
       <c r="B43" t="s">
         <v>14</v>
@@ -3113,7 +2681,7 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>637</v>
+        <v>532</v>
       </c>
       <c r="B44" t="s">
         <v>14</v>
@@ -3127,1060 +2695,10 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:C94"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F73" sqref="F73"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="69.42578125" customWidth="1"/>
-    <col min="2" max="3" width="38" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>581</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>156</v>
-      </c>
-      <c r="B2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>163</v>
-      </c>
-      <c r="B3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>166</v>
-      </c>
-      <c r="B4" t="s">
-        <v>184</v>
-      </c>
-      <c r="C4" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>161</v>
-      </c>
-      <c r="B5" t="s">
-        <v>184</v>
-      </c>
-      <c r="C5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>154</v>
-      </c>
-      <c r="B6" t="s">
-        <v>617</v>
-      </c>
-      <c r="C6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>157</v>
-      </c>
-      <c r="B7" t="s">
-        <v>617</v>
-      </c>
-      <c r="C7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>136</v>
-      </c>
-      <c r="B8" t="s">
-        <v>634</v>
-      </c>
-      <c r="C8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>135</v>
-      </c>
-      <c r="B9" t="s">
-        <v>634</v>
-      </c>
-      <c r="C9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>150</v>
-      </c>
-      <c r="B10" t="s">
-        <v>634</v>
-      </c>
-      <c r="C10" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>145</v>
-      </c>
-      <c r="B11" t="s">
-        <v>634</v>
-      </c>
-      <c r="C11" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>152</v>
-      </c>
-      <c r="B12" t="s">
-        <v>634</v>
-      </c>
-      <c r="C12" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>129</v>
-      </c>
-      <c r="B13" t="s">
-        <v>32</v>
-      </c>
-      <c r="C13" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>121</v>
-      </c>
-      <c r="B14" t="s">
-        <v>26</v>
-      </c>
-      <c r="C14" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>143</v>
-      </c>
-      <c r="B15" t="s">
-        <v>32</v>
-      </c>
-      <c r="C15" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>641</v>
-      </c>
-      <c r="B16" t="s">
-        <v>32</v>
-      </c>
-      <c r="C16" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>174</v>
-      </c>
-      <c r="B17" t="s">
-        <v>25</v>
-      </c>
-      <c r="C17" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>140</v>
-      </c>
-      <c r="B18" t="s">
-        <v>26</v>
-      </c>
-      <c r="C18" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>139</v>
-      </c>
-      <c r="B19" t="s">
-        <v>634</v>
-      </c>
-      <c r="C19" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>151</v>
-      </c>
-      <c r="B20" t="s">
-        <v>634</v>
-      </c>
-      <c r="C20" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>169</v>
-      </c>
-      <c r="B21" t="s">
-        <v>26</v>
-      </c>
-      <c r="C21" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>146</v>
-      </c>
-      <c r="B22" t="s">
-        <v>634</v>
-      </c>
-      <c r="C22" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>148</v>
-      </c>
-      <c r="B23" t="s">
-        <v>634</v>
-      </c>
-      <c r="C23" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>162</v>
-      </c>
-      <c r="B24" t="s">
-        <v>26</v>
-      </c>
-      <c r="C24" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>165</v>
-      </c>
-      <c r="B25" t="s">
-        <v>26</v>
-      </c>
-      <c r="C25" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>153</v>
-      </c>
-      <c r="B26" t="s">
-        <v>634</v>
-      </c>
-      <c r="C26" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>149</v>
-      </c>
-      <c r="B27" t="s">
-        <v>634</v>
-      </c>
-      <c r="C27" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>164</v>
-      </c>
-      <c r="B28" t="s">
-        <v>32</v>
-      </c>
-      <c r="C28" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>172</v>
-      </c>
-      <c r="B29" t="s">
-        <v>634</v>
-      </c>
-      <c r="C29" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>104</v>
-      </c>
-      <c r="B30" t="s">
-        <v>634</v>
-      </c>
-      <c r="C30" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>130</v>
-      </c>
-      <c r="B31" t="s">
-        <v>634</v>
-      </c>
-      <c r="C31" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>620</v>
-      </c>
-      <c r="B32" t="s">
-        <v>634</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>103</v>
-      </c>
-      <c r="B33" t="s">
-        <v>634</v>
-      </c>
-      <c r="C33" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>107</v>
-      </c>
-      <c r="B34" t="s">
-        <v>634</v>
-      </c>
-      <c r="C34" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>128</v>
-      </c>
-      <c r="B35" t="s">
-        <v>32</v>
-      </c>
-      <c r="C35" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>137</v>
-      </c>
-      <c r="B36" t="s">
-        <v>634</v>
-      </c>
-      <c r="C36" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>131</v>
-      </c>
-      <c r="B37" t="s">
-        <v>634</v>
-      </c>
-      <c r="C37" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>122</v>
-      </c>
-      <c r="B38" t="s">
-        <v>634</v>
-      </c>
-      <c r="C38" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>132</v>
-      </c>
-      <c r="B39" t="s">
-        <v>634</v>
-      </c>
-      <c r="C39" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>124</v>
-      </c>
-      <c r="B40" t="s">
-        <v>26</v>
-      </c>
-      <c r="C40" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>608</v>
-      </c>
-      <c r="B41" t="s">
-        <v>634</v>
-      </c>
-      <c r="C41" t="s">
-        <v>607</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>123</v>
-      </c>
-      <c r="B42" t="s">
-        <v>634</v>
-      </c>
-      <c r="C42" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>134</v>
-      </c>
-      <c r="B43" t="s">
-        <v>634</v>
-      </c>
-      <c r="C43" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>621</v>
-      </c>
-      <c r="B44" t="s">
-        <v>634</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>125</v>
-      </c>
-      <c r="B45" t="s">
-        <v>26</v>
-      </c>
-      <c r="C45" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>158</v>
-      </c>
-      <c r="B46" t="s">
-        <v>634</v>
-      </c>
-      <c r="C46" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>159</v>
-      </c>
-      <c r="B47" t="s">
-        <v>634</v>
-      </c>
-      <c r="C47" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>160</v>
-      </c>
-      <c r="B48" t="s">
-        <v>634</v>
-      </c>
-      <c r="C48" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>170</v>
-      </c>
-      <c r="B49" t="s">
-        <v>634</v>
-      </c>
-      <c r="C49" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>175</v>
-      </c>
-      <c r="B50" t="s">
-        <v>634</v>
-      </c>
-      <c r="C50" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>640</v>
-      </c>
-      <c r="B51" t="s">
-        <v>634</v>
-      </c>
-      <c r="C51" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>147</v>
-      </c>
-      <c r="B52" t="s">
-        <v>635</v>
-      </c>
-      <c r="C52" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>642</v>
-      </c>
-      <c r="B53" t="s">
-        <v>635</v>
-      </c>
-      <c r="C53" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>115</v>
-      </c>
-      <c r="B54" t="s">
-        <v>635</v>
-      </c>
-      <c r="C54" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>171</v>
-      </c>
-      <c r="B55" t="s">
-        <v>25</v>
-      </c>
-      <c r="C55" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>106</v>
-      </c>
-      <c r="B56" t="s">
-        <v>184</v>
-      </c>
-      <c r="C56" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>109</v>
-      </c>
-      <c r="B57" t="s">
-        <v>634</v>
-      </c>
-      <c r="C57" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>126</v>
-      </c>
-      <c r="B58" t="s">
-        <v>32</v>
-      </c>
-      <c r="C58" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>127</v>
-      </c>
-      <c r="B59" t="s">
-        <v>32</v>
-      </c>
-      <c r="C59" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>108</v>
-      </c>
-      <c r="B60" t="s">
-        <v>617</v>
-      </c>
-      <c r="C60" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>120</v>
-      </c>
-      <c r="B61" t="s">
-        <v>617</v>
-      </c>
-      <c r="C61" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>144</v>
-      </c>
-      <c r="B62" t="s">
-        <v>25</v>
-      </c>
-      <c r="C62" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>94</v>
-      </c>
-      <c r="B63" t="s">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>142</v>
-      </c>
-      <c r="B64" t="s">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>72</v>
-      </c>
-      <c r="B65" t="s">
-        <v>633</v>
-      </c>
-      <c r="C65" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>105</v>
-      </c>
-      <c r="B66" t="s">
-        <v>633</v>
-      </c>
-      <c r="C66" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>116</v>
-      </c>
-      <c r="B67" t="s">
-        <v>25</v>
-      </c>
-      <c r="C67" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>117</v>
-      </c>
-      <c r="B68" t="s">
-        <v>25</v>
-      </c>
-      <c r="C68" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>111</v>
-      </c>
-      <c r="B69" t="s">
-        <v>25</v>
-      </c>
-      <c r="C69" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>112</v>
-      </c>
-      <c r="B70" t="s">
-        <v>25</v>
-      </c>
-      <c r="C70" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>110</v>
-      </c>
-      <c r="B71" t="s">
-        <v>25</v>
-      </c>
-      <c r="C71" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>114</v>
-      </c>
-      <c r="B72" t="s">
-        <v>25</v>
-      </c>
-      <c r="C72" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>119</v>
-      </c>
-      <c r="B73" t="s">
-        <v>25</v>
-      </c>
-      <c r="C73" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>113</v>
-      </c>
-      <c r="B74" t="s">
-        <v>25</v>
-      </c>
-      <c r="C74" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
-        <v>155</v>
-      </c>
-      <c r="B75" t="s">
-        <v>633</v>
-      </c>
-      <c r="C75" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
-        <v>168</v>
-      </c>
-      <c r="B76" t="s">
-        <v>25</v>
-      </c>
-      <c r="C76" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
-        <v>167</v>
-      </c>
-      <c r="B77" t="s">
-        <v>634</v>
-      </c>
-      <c r="C77" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
-        <v>133</v>
-      </c>
-      <c r="B78" t="s">
-        <v>634</v>
-      </c>
-      <c r="C78" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
-        <v>118</v>
-      </c>
-      <c r="B79" t="s">
-        <v>25</v>
-      </c>
-      <c r="C79" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
-        <v>616</v>
-      </c>
-      <c r="B80" t="s">
-        <v>617</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
-        <v>138</v>
-      </c>
-      <c r="B81" t="s">
-        <v>634</v>
-      </c>
-      <c r="C81" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
-        <v>605</v>
-      </c>
-      <c r="B82" t="s">
-        <v>634</v>
-      </c>
-      <c r="C82" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
-        <v>141</v>
-      </c>
-      <c r="B83" t="s">
-        <v>32</v>
-      </c>
-      <c r="C83" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
-        <v>173</v>
-      </c>
-      <c r="B84" t="s">
-        <v>27</v>
-      </c>
-      <c r="C84" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
-        <v>618</v>
-      </c>
-      <c r="B85" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
-        <v>176</v>
-      </c>
-      <c r="B86" t="s">
-        <v>27</v>
-      </c>
-      <c r="C86" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B87" t="s">
-        <v>26</v>
-      </c>
-      <c r="C87" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B88" t="s">
-        <v>32</v>
-      </c>
-      <c r="C88" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B89" t="s">
-        <v>635</v>
-      </c>
-      <c r="C89" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
-        <v>622</v>
-      </c>
-      <c r="B90" t="s">
-        <v>617</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
-        <v>624</v>
-      </c>
-      <c r="B91" t="s">
-        <v>634</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
-        <v>636</v>
-      </c>
-      <c r="B92" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
-        <v>643</v>
-      </c>
-      <c r="B93" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
-        <v>646</v>
-      </c>
-      <c r="B94" t="s">
-        <v>25</v>
-      </c>
-      <c r="C94" t="s">
-        <v>25</v>
-      </c>
-    </row>
-  </sheetData>
-  <autoFilter ref="A1:C1" xr:uid="{00000000-0009-0000-0000-000003000000}">
-    <sortState ref="A2:C89">
-      <sortCondition ref="A1"/>
-    </sortState>
-  </autoFilter>
-  <conditionalFormatting sqref="A93:A1048576 A1:A8 A10:A12 A14:A43 A45:A86">
-    <cfRule type="duplicateValues" dxfId="16" priority="11"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A9">
-    <cfRule type="duplicateValues" dxfId="15" priority="10"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A13">
-    <cfRule type="duplicateValues" dxfId="14" priority="8"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A87">
-    <cfRule type="duplicateValues" dxfId="13" priority="7"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A88">
-    <cfRule type="duplicateValues" dxfId="12" priority="6"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A89">
-    <cfRule type="duplicateValues" dxfId="11" priority="5"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A44">
-    <cfRule type="duplicateValues" dxfId="10" priority="4"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A90">
-    <cfRule type="duplicateValues" dxfId="9" priority="3"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A91">
-    <cfRule type="duplicateValues" dxfId="8" priority="2"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A92">
-    <cfRule type="duplicateValues" dxfId="7" priority="1"/>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B233"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A91" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="J95" sqref="J95"/>
     </sheetView>
@@ -4201,1858 +2719,1858 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>281</v>
+        <v>191</v>
       </c>
       <c r="B2" t="s">
-        <v>469</v>
+        <v>379</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>275</v>
+        <v>185</v>
       </c>
       <c r="B3" t="s">
-        <v>601</v>
+        <v>511</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>368</v>
+        <v>278</v>
       </c>
       <c r="B4" t="s">
-        <v>601</v>
+        <v>511</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>186</v>
+        <v>96</v>
       </c>
       <c r="B5" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>337</v>
+        <v>247</v>
       </c>
       <c r="B6" t="s">
-        <v>524</v>
+        <v>434</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>375</v>
+        <v>285</v>
       </c>
       <c r="B7" t="s">
-        <v>560</v>
+        <v>470</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>261</v>
+        <v>171</v>
       </c>
       <c r="B8" t="s">
-        <v>450</v>
+        <v>360</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>389</v>
+        <v>299</v>
       </c>
       <c r="B9" t="s">
-        <v>629</v>
+        <v>528</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>257</v>
+        <v>167</v>
       </c>
       <c r="B10" t="s">
-        <v>446</v>
+        <v>356</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>232</v>
+        <v>142</v>
       </c>
       <c r="B11" t="s">
-        <v>421</v>
+        <v>331</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>223</v>
+        <v>133</v>
       </c>
       <c r="B12" t="s">
-        <v>412</v>
+        <v>322</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>373</v>
+        <v>283</v>
       </c>
       <c r="B13" t="s">
-        <v>558</v>
+        <v>468</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>329</v>
+        <v>239</v>
       </c>
       <c r="B14" t="s">
-        <v>516</v>
+        <v>426</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>330</v>
+        <v>240</v>
       </c>
       <c r="B15" t="s">
-        <v>517</v>
+        <v>427</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>225</v>
+        <v>135</v>
       </c>
       <c r="B16" t="s">
-        <v>414</v>
+        <v>324</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>233</v>
+        <v>143</v>
       </c>
       <c r="B17" t="s">
-        <v>422</v>
+        <v>332</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>332</v>
+        <v>242</v>
       </c>
       <c r="B18" t="s">
-        <v>519</v>
+        <v>429</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>216</v>
+        <v>126</v>
       </c>
       <c r="B19" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>260</v>
+        <v>170</v>
       </c>
       <c r="B20" t="s">
-        <v>449</v>
+        <v>359</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>262</v>
+        <v>172</v>
       </c>
       <c r="B21" t="s">
-        <v>451</v>
+        <v>361</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>331</v>
+        <v>241</v>
       </c>
       <c r="B22" t="s">
-        <v>518</v>
+        <v>428</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>224</v>
+        <v>134</v>
       </c>
       <c r="B23" t="s">
-        <v>413</v>
+        <v>323</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>211</v>
+        <v>121</v>
       </c>
       <c r="B24" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>403</v>
+        <v>313</v>
       </c>
       <c r="B25" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>185</v>
+        <v>95</v>
       </c>
       <c r="B26" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>234</v>
+        <v>144</v>
       </c>
       <c r="B27" t="s">
-        <v>423</v>
+        <v>333</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>268</v>
+        <v>178</v>
       </c>
       <c r="B28" t="s">
-        <v>457</v>
+        <v>367</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>286</v>
+        <v>196</v>
       </c>
       <c r="B29" t="s">
-        <v>474</v>
+        <v>384</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>235</v>
+        <v>145</v>
       </c>
       <c r="B30" t="s">
-        <v>424</v>
+        <v>334</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>392</v>
+        <v>302</v>
       </c>
       <c r="B31" t="s">
-        <v>574</v>
+        <v>484</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>602</v>
+        <v>512</v>
       </c>
       <c r="B32" t="s">
-        <v>602</v>
+        <v>512</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>226</v>
+        <v>136</v>
       </c>
       <c r="B33" t="s">
-        <v>415</v>
+        <v>325</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>288</v>
+        <v>198</v>
       </c>
       <c r="B34" t="s">
-        <v>476</v>
+        <v>386</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>280</v>
+        <v>190</v>
       </c>
       <c r="B35" t="s">
-        <v>468</v>
+        <v>378</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>400</v>
+        <v>310</v>
       </c>
       <c r="B36" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>219</v>
+        <v>129</v>
       </c>
       <c r="B37" t="s">
-        <v>408</v>
+        <v>318</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>318</v>
+        <v>228</v>
       </c>
       <c r="B38" t="s">
-        <v>505</v>
+        <v>415</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>333</v>
+        <v>243</v>
       </c>
       <c r="B39" t="s">
-        <v>520</v>
+        <v>430</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>391</v>
+        <v>301</v>
       </c>
       <c r="B40" t="s">
-        <v>573</v>
+        <v>483</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>322</v>
+        <v>232</v>
       </c>
       <c r="B41" t="s">
-        <v>509</v>
+        <v>419</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>267</v>
+        <v>177</v>
       </c>
       <c r="B42" t="s">
-        <v>456</v>
+        <v>366</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>236</v>
+        <v>146</v>
       </c>
       <c r="B43" t="s">
-        <v>425</v>
+        <v>335</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>315</v>
+        <v>225</v>
       </c>
       <c r="B44" t="s">
-        <v>502</v>
+        <v>412</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>237</v>
+        <v>147</v>
       </c>
       <c r="B45" t="s">
-        <v>426</v>
+        <v>336</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>312</v>
+        <v>222</v>
       </c>
       <c r="B46" t="s">
-        <v>499</v>
+        <v>409</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>325</v>
+        <v>235</v>
       </c>
       <c r="B47" t="s">
-        <v>512</v>
+        <v>422</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>311</v>
+        <v>221</v>
       </c>
       <c r="B48" t="s">
-        <v>498</v>
+        <v>408</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>383</v>
+        <v>293</v>
       </c>
       <c r="B49" t="s">
-        <v>630</v>
+        <v>529</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>238</v>
+        <v>148</v>
       </c>
       <c r="B50" t="s">
-        <v>427</v>
+        <v>337</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>405</v>
+        <v>315</v>
       </c>
       <c r="B51" t="s">
-        <v>487</v>
+        <v>397</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
+        <v>307</v>
+      </c>
+      <c r="B52" t="s">
         <v>397</v>
-      </c>
-      <c r="B52" t="s">
-        <v>487</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>300</v>
+        <v>210</v>
       </c>
       <c r="B53" t="s">
-        <v>487</v>
+        <v>397</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>604</v>
+        <v>514</v>
       </c>
       <c r="B54" t="s">
-        <v>487</v>
+        <v>397</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>277</v>
+        <v>187</v>
       </c>
       <c r="B55" t="s">
-        <v>465</v>
+        <v>375</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>371</v>
+        <v>281</v>
       </c>
       <c r="B56" t="s">
-        <v>556</v>
+        <v>466</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>334</v>
+        <v>244</v>
       </c>
       <c r="B57" t="s">
-        <v>521</v>
+        <v>431</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>271</v>
+        <v>181</v>
       </c>
       <c r="B58" t="s">
-        <v>460</v>
+        <v>370</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>336</v>
+        <v>246</v>
       </c>
       <c r="B59" t="s">
-        <v>523</v>
+        <v>433</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>335</v>
+        <v>245</v>
       </c>
       <c r="B60" t="s">
-        <v>522</v>
+        <v>432</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>256</v>
+        <v>166</v>
       </c>
       <c r="B61" t="s">
-        <v>445</v>
+        <v>355</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>239</v>
+        <v>149</v>
       </c>
       <c r="B62" t="s">
-        <v>428</v>
+        <v>338</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>370</v>
+        <v>280</v>
       </c>
       <c r="B63" t="s">
-        <v>555</v>
+        <v>465</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>369</v>
+        <v>279</v>
       </c>
       <c r="B64" t="s">
-        <v>407</v>
+        <v>317</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>240</v>
+        <v>150</v>
       </c>
       <c r="B65" t="s">
-        <v>429</v>
+        <v>339</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>320</v>
+        <v>230</v>
       </c>
       <c r="B66" t="s">
-        <v>507</v>
+        <v>417</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>612</v>
+        <v>519</v>
       </c>
       <c r="B67" t="s">
-        <v>507</v>
+        <v>417</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>250</v>
+        <v>160</v>
       </c>
       <c r="B68" t="s">
-        <v>439</v>
+        <v>349</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>324</v>
+        <v>234</v>
       </c>
       <c r="B69" t="s">
-        <v>511</v>
+        <v>421</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>231</v>
+        <v>141</v>
       </c>
       <c r="B70" t="s">
-        <v>420</v>
+        <v>330</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>276</v>
+        <v>186</v>
       </c>
       <c r="B71" t="s">
-        <v>464</v>
+        <v>374</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>215</v>
+        <v>125</v>
       </c>
       <c r="B72" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>213</v>
+        <v>123</v>
       </c>
       <c r="B73" t="s">
-        <v>407</v>
+        <v>317</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>406</v>
+        <v>316</v>
       </c>
       <c r="B74" t="s">
-        <v>407</v>
+        <v>317</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>228</v>
+        <v>138</v>
       </c>
       <c r="B75" t="s">
-        <v>417</v>
+        <v>327</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>339</v>
+        <v>249</v>
       </c>
       <c r="B76" t="s">
-        <v>526</v>
+        <v>436</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>340</v>
+        <v>250</v>
       </c>
       <c r="B77" t="s">
-        <v>527</v>
+        <v>437</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>341</v>
+        <v>251</v>
       </c>
       <c r="B78" t="s">
-        <v>528</v>
+        <v>438</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>217</v>
+        <v>127</v>
       </c>
       <c r="B79" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>632</v>
+        <v>531</v>
       </c>
       <c r="B80" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>272</v>
+        <v>182</v>
       </c>
       <c r="B81" t="s">
-        <v>461</v>
+        <v>371</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>263</v>
+        <v>173</v>
       </c>
       <c r="B82" t="s">
-        <v>452</v>
+        <v>362</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>218</v>
+        <v>128</v>
       </c>
       <c r="B83" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>376</v>
+        <v>286</v>
       </c>
       <c r="B84" t="s">
-        <v>561</v>
+        <v>471</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>343</v>
+        <v>253</v>
       </c>
       <c r="B85" t="s">
-        <v>530</v>
+        <v>440</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>390</v>
+        <v>300</v>
       </c>
       <c r="B86" t="s">
-        <v>572</v>
+        <v>482</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>402</v>
+        <v>312</v>
       </c>
       <c r="B87" t="s">
-        <v>578</v>
+        <v>488</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>241</v>
+        <v>151</v>
       </c>
       <c r="B88" t="s">
-        <v>430</v>
+        <v>340</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>220</v>
+        <v>130</v>
       </c>
       <c r="B89" t="s">
-        <v>409</v>
+        <v>319</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>372</v>
+        <v>282</v>
       </c>
       <c r="B90" t="s">
-        <v>557</v>
+        <v>467</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>242</v>
+        <v>152</v>
       </c>
       <c r="B91" t="s">
-        <v>431</v>
+        <v>341</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>244</v>
+        <v>154</v>
       </c>
       <c r="B92" t="s">
-        <v>433</v>
+        <v>343</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>243</v>
+        <v>153</v>
       </c>
       <c r="B93" t="s">
-        <v>432</v>
+        <v>342</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>344</v>
+        <v>254</v>
       </c>
       <c r="B94" t="s">
-        <v>531</v>
+        <v>441</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>278</v>
+        <v>188</v>
       </c>
       <c r="B95" t="s">
-        <v>466</v>
+        <v>376</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>377</v>
+        <v>287</v>
       </c>
       <c r="B96" t="s">
-        <v>562</v>
+        <v>472</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>274</v>
+        <v>184</v>
       </c>
       <c r="B97" t="s">
-        <v>463</v>
+        <v>373</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>319</v>
+        <v>229</v>
       </c>
       <c r="B98" t="s">
-        <v>506</v>
+        <v>416</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>321</v>
+        <v>231</v>
       </c>
       <c r="B99" t="s">
-        <v>508</v>
+        <v>418</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>323</v>
+        <v>233</v>
       </c>
       <c r="B100" t="s">
-        <v>510</v>
+        <v>420</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>345</v>
+        <v>255</v>
       </c>
       <c r="B101" t="s">
-        <v>532</v>
+        <v>442</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>346</v>
+        <v>256</v>
       </c>
       <c r="B102" t="s">
-        <v>533</v>
+        <v>443</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>347</v>
+        <v>257</v>
       </c>
       <c r="B103" t="s">
-        <v>534</v>
+        <v>444</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>245</v>
+        <v>155</v>
       </c>
       <c r="B104" t="s">
-        <v>434</v>
+        <v>344</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>348</v>
+        <v>258</v>
       </c>
       <c r="B105" t="s">
-        <v>535</v>
+        <v>445</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>253</v>
+        <v>163</v>
       </c>
       <c r="B106" t="s">
-        <v>442</v>
+        <v>352</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>279</v>
+        <v>189</v>
       </c>
       <c r="B107" t="s">
-        <v>467</v>
+        <v>377</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>221</v>
+        <v>131</v>
       </c>
       <c r="B108" t="s">
-        <v>410</v>
+        <v>320</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>647</v>
+        <v>537</v>
       </c>
       <c r="B109" t="s">
-        <v>644</v>
+        <v>535</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>395</v>
+        <v>305</v>
       </c>
       <c r="B110" t="s">
-        <v>575</v>
+        <v>485</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>349</v>
+        <v>259</v>
       </c>
       <c r="B111" t="s">
-        <v>536</v>
+        <v>446</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>265</v>
+        <v>175</v>
       </c>
       <c r="B112" t="s">
-        <v>454</v>
+        <v>364</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>350</v>
+        <v>260</v>
       </c>
       <c r="B113" t="s">
-        <v>537</v>
+        <v>447</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>264</v>
+        <v>174</v>
       </c>
       <c r="B114" t="s">
-        <v>453</v>
+        <v>363</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>201</v>
+        <v>111</v>
       </c>
       <c r="B115" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>374</v>
+        <v>284</v>
       </c>
       <c r="B116" t="s">
-        <v>559</v>
+        <v>469</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>284</v>
+        <v>194</v>
       </c>
       <c r="B117" t="s">
-        <v>472</v>
+        <v>382</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>351</v>
+        <v>261</v>
       </c>
       <c r="B118" t="s">
-        <v>538</v>
+        <v>448</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>283</v>
+        <v>193</v>
       </c>
       <c r="B119" t="s">
-        <v>471</v>
+        <v>381</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>227</v>
+        <v>137</v>
       </c>
       <c r="B120" t="s">
-        <v>416</v>
+        <v>326</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>382</v>
+        <v>292</v>
       </c>
       <c r="B121" t="s">
-        <v>567</v>
+        <v>477</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>378</v>
+        <v>288</v>
       </c>
       <c r="B122" t="s">
-        <v>563</v>
+        <v>473</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>282</v>
+        <v>192</v>
       </c>
       <c r="B123" t="s">
-        <v>470</v>
+        <v>380</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>352</v>
+        <v>262</v>
       </c>
       <c r="B124" t="s">
-        <v>539</v>
+        <v>449</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>285</v>
+        <v>195</v>
       </c>
       <c r="B125" t="s">
-        <v>473</v>
+        <v>383</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>202</v>
+        <v>112</v>
       </c>
       <c r="B126" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>297</v>
+        <v>207</v>
       </c>
       <c r="B127" t="s">
-        <v>484</v>
+        <v>394</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>316</v>
+        <v>226</v>
       </c>
       <c r="B128" t="s">
-        <v>503</v>
+        <v>413</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>299</v>
+        <v>209</v>
       </c>
       <c r="B129" t="s">
-        <v>486</v>
+        <v>396</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>203</v>
+        <v>113</v>
       </c>
       <c r="B130" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>353</v>
+        <v>263</v>
       </c>
       <c r="B131" t="s">
-        <v>540</v>
+        <v>450</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>309</v>
+        <v>219</v>
       </c>
       <c r="B132" t="s">
-        <v>496</v>
+        <v>406</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>308</v>
+        <v>218</v>
       </c>
       <c r="B133" t="s">
-        <v>495</v>
+        <v>405</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>313</v>
+        <v>223</v>
       </c>
       <c r="B134" t="s">
-        <v>500</v>
+        <v>410</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>246</v>
+        <v>156</v>
       </c>
       <c r="B135" t="s">
-        <v>435</v>
+        <v>345</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>384</v>
+        <v>294</v>
       </c>
       <c r="B136" t="s">
-        <v>568</v>
+        <v>478</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>603</v>
+        <v>513</v>
       </c>
       <c r="B137" t="s">
-        <v>568</v>
+        <v>478</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>269</v>
+        <v>179</v>
       </c>
       <c r="B138" t="s">
-        <v>458</v>
+        <v>368</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>399</v>
+        <v>309</v>
       </c>
       <c r="B139" t="s">
-        <v>576</v>
+        <v>486</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>204</v>
+        <v>114</v>
       </c>
       <c r="B140" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>210</v>
+        <v>120</v>
       </c>
       <c r="B141" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>393</v>
+        <v>303</v>
       </c>
       <c r="B142" t="s">
-        <v>614</v>
+        <v>520</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>310</v>
+        <v>220</v>
       </c>
       <c r="B143" t="s">
-        <v>497</v>
+        <v>407</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>205</v>
+        <v>115</v>
       </c>
       <c r="B144" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>314</v>
+        <v>224</v>
       </c>
       <c r="B145" t="s">
-        <v>501</v>
+        <v>411</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>206</v>
+        <v>116</v>
       </c>
       <c r="B146" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>386</v>
+        <v>296</v>
       </c>
       <c r="B147" t="s">
-        <v>569</v>
+        <v>479</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>230</v>
+        <v>140</v>
       </c>
       <c r="B148" t="s">
-        <v>419</v>
+        <v>329</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>354</v>
+        <v>264</v>
       </c>
       <c r="B149" t="s">
-        <v>541</v>
+        <v>451</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>355</v>
+        <v>265</v>
       </c>
       <c r="B150" t="s">
-        <v>542</v>
+        <v>452</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>247</v>
+        <v>157</v>
       </c>
       <c r="B151" t="s">
-        <v>436</v>
+        <v>346</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>188</v>
+        <v>98</v>
       </c>
       <c r="B152" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>298</v>
+        <v>208</v>
       </c>
       <c r="B153" t="s">
-        <v>485</v>
+        <v>395</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>385</v>
+        <v>295</v>
       </c>
       <c r="B154" t="s">
-        <v>631</v>
+        <v>530</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>379</v>
+        <v>289</v>
       </c>
       <c r="B155" t="s">
-        <v>564</v>
+        <v>474</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>356</v>
+        <v>266</v>
       </c>
       <c r="B156" t="s">
-        <v>543</v>
+        <v>453</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>229</v>
+        <v>139</v>
       </c>
       <c r="B157" t="s">
-        <v>418</v>
+        <v>328</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>387</v>
+        <v>297</v>
       </c>
       <c r="B158" t="s">
-        <v>570</v>
+        <v>480</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>248</v>
+        <v>158</v>
       </c>
       <c r="B159" t="s">
-        <v>437</v>
+        <v>347</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>197</v>
+        <v>107</v>
       </c>
       <c r="B160" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>249</v>
+        <v>159</v>
       </c>
       <c r="B161" t="s">
-        <v>438</v>
+        <v>348</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>196</v>
+        <v>106</v>
       </c>
       <c r="B162" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>287</v>
+        <v>197</v>
       </c>
       <c r="B163" t="s">
-        <v>475</v>
+        <v>385</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>266</v>
+        <v>176</v>
       </c>
       <c r="B164" t="s">
-        <v>455</v>
+        <v>365</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>357</v>
+        <v>267</v>
       </c>
       <c r="B165" t="s">
-        <v>544</v>
+        <v>454</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>401</v>
+        <v>311</v>
       </c>
       <c r="B166" t="s">
-        <v>577</v>
+        <v>487</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>358</v>
+        <v>268</v>
       </c>
       <c r="B167" t="s">
-        <v>545</v>
+        <v>455</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>191</v>
+        <v>101</v>
       </c>
       <c r="B168" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>273</v>
+        <v>183</v>
       </c>
       <c r="B169" t="s">
-        <v>462</v>
+        <v>372</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>294</v>
+        <v>204</v>
       </c>
       <c r="B170" t="s">
-        <v>481</v>
+        <v>391</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>193</v>
+        <v>103</v>
       </c>
       <c r="B171" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>295</v>
+        <v>205</v>
       </c>
       <c r="B172" t="s">
-        <v>482</v>
+        <v>392</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>380</v>
+        <v>290</v>
       </c>
       <c r="B173" t="s">
-        <v>565</v>
+        <v>475</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>396</v>
+        <v>306</v>
       </c>
       <c r="B174" t="s">
-        <v>492</v>
+        <v>402</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>305</v>
+        <v>215</v>
       </c>
       <c r="B175" t="s">
-        <v>492</v>
+        <v>402</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>404</v>
+        <v>314</v>
       </c>
       <c r="B176" t="s">
-        <v>492</v>
+        <v>402</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>359</v>
+        <v>269</v>
       </c>
       <c r="B177" t="s">
-        <v>546</v>
+        <v>456</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>194</v>
+        <v>104</v>
       </c>
       <c r="B178" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>638</v>
+        <v>533</v>
       </c>
       <c r="B179" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>639</v>
+        <v>534</v>
       </c>
       <c r="B180" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>209</v>
+        <v>119</v>
       </c>
       <c r="B181" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>208</v>
+        <v>118</v>
       </c>
       <c r="B182" t="s">
-        <v>579</v>
+        <v>489</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>296</v>
+        <v>206</v>
       </c>
       <c r="B183" t="s">
-        <v>483</v>
+        <v>393</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>190</v>
+        <v>100</v>
       </c>
       <c r="B184" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>360</v>
+        <v>270</v>
       </c>
       <c r="B185" t="s">
-        <v>547</v>
+        <v>457</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>362</v>
+        <v>272</v>
       </c>
       <c r="B186" t="s">
-        <v>549</v>
+        <v>459</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>363</v>
+        <v>273</v>
       </c>
       <c r="B187" t="s">
-        <v>550</v>
+        <v>460</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>306</v>
+        <v>216</v>
       </c>
       <c r="B188" t="s">
-        <v>493</v>
+        <v>403</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>361</v>
+        <v>271</v>
       </c>
       <c r="B189" t="s">
-        <v>548</v>
+        <v>458</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>200</v>
+        <v>110</v>
       </c>
       <c r="B190" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>304</v>
+        <v>214</v>
       </c>
       <c r="B191" t="s">
-        <v>491</v>
+        <v>401</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>338</v>
+        <v>248</v>
       </c>
       <c r="B192" t="s">
-        <v>525</v>
+        <v>435</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>293</v>
+        <v>203</v>
       </c>
       <c r="B193" t="s">
-        <v>480</v>
+        <v>390</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>259</v>
+        <v>169</v>
       </c>
       <c r="B194" t="s">
-        <v>448</v>
+        <v>358</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>255</v>
+        <v>165</v>
       </c>
       <c r="B195" t="s">
-        <v>444</v>
+        <v>354</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>398</v>
+        <v>308</v>
       </c>
       <c r="B196" t="s">
-        <v>447</v>
+        <v>357</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>258</v>
+        <v>168</v>
       </c>
       <c r="B197" t="s">
-        <v>447</v>
+        <v>357</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>292</v>
+        <v>202</v>
       </c>
       <c r="B198" t="s">
-        <v>479</v>
+        <v>389</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>251</v>
+        <v>161</v>
       </c>
       <c r="B199" t="s">
-        <v>440</v>
+        <v>350</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>291</v>
+        <v>201</v>
       </c>
       <c r="B200" t="s">
-        <v>644</v>
+        <v>535</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>364</v>
+        <v>274</v>
       </c>
       <c r="B201" t="s">
-        <v>551</v>
+        <v>461</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>381</v>
+        <v>291</v>
       </c>
       <c r="B202" t="s">
-        <v>566</v>
+        <v>476</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>365</v>
+        <v>275</v>
       </c>
       <c r="B203" t="s">
-        <v>552</v>
+        <v>462</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>645</v>
+        <v>536</v>
       </c>
       <c r="B204" t="s">
-        <v>553</v>
+        <v>463</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>366</v>
+        <v>276</v>
       </c>
       <c r="B205" t="s">
-        <v>553</v>
+        <v>463</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>198</v>
+        <v>108</v>
       </c>
       <c r="B206" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>187</v>
+        <v>97</v>
       </c>
       <c r="B207" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>222</v>
+        <v>132</v>
       </c>
       <c r="B208" t="s">
-        <v>411</v>
+        <v>321</v>
       </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>326</v>
+        <v>236</v>
       </c>
       <c r="B209" t="s">
-        <v>513</v>
+        <v>423</v>
       </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>302</v>
+        <v>212</v>
       </c>
       <c r="B210" t="s">
-        <v>489</v>
+        <v>399</v>
       </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>290</v>
+        <v>200</v>
       </c>
       <c r="B211" t="s">
-        <v>478</v>
+        <v>388</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>254</v>
+        <v>164</v>
       </c>
       <c r="B212" t="s">
-        <v>443</v>
+        <v>353</v>
       </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>317</v>
+        <v>227</v>
       </c>
       <c r="B213" t="s">
-        <v>504</v>
+        <v>414</v>
       </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>307</v>
+        <v>217</v>
       </c>
       <c r="B214" t="s">
-        <v>494</v>
+        <v>404</v>
       </c>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>301</v>
+        <v>211</v>
       </c>
       <c r="B215" t="s">
-        <v>488</v>
+        <v>398</v>
       </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>388</v>
+        <v>298</v>
       </c>
       <c r="B216" t="s">
-        <v>571</v>
+        <v>481</v>
       </c>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>189</v>
+        <v>99</v>
       </c>
       <c r="B217" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>270</v>
+        <v>180</v>
       </c>
       <c r="B218" t="s">
-        <v>459</v>
+        <v>369</v>
       </c>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>328</v>
+        <v>238</v>
       </c>
       <c r="B219" t="s">
-        <v>515</v>
+        <v>425</v>
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>342</v>
+        <v>252</v>
       </c>
       <c r="B220" t="s">
-        <v>529</v>
+        <v>439</v>
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
-        <v>367</v>
+        <v>277</v>
       </c>
       <c r="B221" t="s">
-        <v>554</v>
+        <v>464</v>
       </c>
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>252</v>
+        <v>162</v>
       </c>
       <c r="B222" t="s">
-        <v>441</v>
+        <v>351</v>
       </c>
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>327</v>
+        <v>237</v>
       </c>
       <c r="B223" t="s">
-        <v>514</v>
+        <v>424</v>
       </c>
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>192</v>
+        <v>102</v>
       </c>
       <c r="B224" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>394</v>
+        <v>304</v>
       </c>
       <c r="B225" t="s">
-        <v>610</v>
+        <v>517</v>
       </c>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>195</v>
+        <v>105</v>
       </c>
       <c r="B226" t="s">
-        <v>610</v>
+        <v>517</v>
       </c>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>609</v>
+        <v>516</v>
       </c>
       <c r="B227" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
-        <v>199</v>
+        <v>109</v>
       </c>
       <c r="B228" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
-        <v>289</v>
+        <v>199</v>
       </c>
       <c r="B229" t="s">
-        <v>477</v>
+        <v>387</v>
       </c>
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
-        <v>214</v>
+        <v>124</v>
       </c>
       <c r="B230" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
-        <v>212</v>
+        <v>122</v>
       </c>
       <c r="B231" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
-        <v>207</v>
+        <v>117</v>
       </c>
       <c r="B232" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
-        <v>303</v>
+        <v>213</v>
       </c>
       <c r="B233" t="s">
-        <v>490</v>
+        <v>400</v>
       </c>
     </row>
   </sheetData>
@@ -6090,11 +4608,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
@@ -6114,90 +4632,90 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>623</v>
+        <v>523</v>
       </c>
       <c r="B2" t="s">
-        <v>619</v>
+        <v>522</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>591</v>
+        <v>501</v>
       </c>
       <c r="B3" t="s">
-        <v>582</v>
+        <v>492</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>592</v>
+        <v>502</v>
       </c>
       <c r="B4" t="s">
-        <v>582</v>
+        <v>492</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>583</v>
+        <v>493</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>584</v>
+        <v>494</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>585</v>
+        <v>495</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>586</v>
+        <v>496</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>587</v>
+        <v>497</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>588</v>
+        <v>498</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>589</v>
+        <v>499</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>590</v>
+        <v>500</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>594</v>
+        <v>504</v>
       </c>
       <c r="B13" t="s">
-        <v>619</v>
+        <v>522</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>615</v>
+        <v>521</v>
       </c>
       <c r="B14" t="s">
-        <v>619</v>
+        <v>522</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>593</v>
+        <v>503</v>
       </c>
       <c r="B15" t="s">
-        <v>619</v>
+        <v>522</v>
       </c>
     </row>
   </sheetData>
@@ -6206,7 +4724,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:B10"/>
   <sheetViews>
@@ -6230,18 +4748,18 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>596</v>
+        <v>506</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>625</v>
+        <v>524</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>597</v>
+        <v>507</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>626</v>
+        <v>525</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -6249,36 +4767,36 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>626</v>
+        <v>525</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>598</v>
+        <v>508</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>626</v>
+        <v>525</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>600</v>
+        <v>510</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>628</v>
+        <v>527</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>595</v>
+        <v>505</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>627</v>
+        <v>526</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>599</v>
+        <v>509</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
fixed lookup and add_internal_data
</commit_message>
<xml_diff>
--- a/data-raw/control_vocab_mapping.xlsx
+++ b/data-raw/control_vocab_mapping.xlsx
@@ -8,21 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WB525812\cmder\Git Repos\mdlibtoddh\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{590854F0-2327-499D-AAAC-0BE2BF1FD823}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{700C2F1C-0A8E-46E5-9CC9-C33220A58566}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="10770" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="10770" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dataClassification" sheetId="1" r:id="rId1"/>
     <sheet name="termsofUse" sheetId="2" r:id="rId2"/>
-    <sheet name="kindData" sheetId="3" r:id="rId3"/>
-    <sheet name="geographicalCoverage" sheetId="5" r:id="rId4"/>
-    <sheet name="source" sheetId="7" r:id="rId5"/>
-    <sheet name="license" sheetId="8" r:id="rId6"/>
+    <sheet name="geographicalCoverage" sheetId="5" r:id="rId3"/>
+    <sheet name="source" sheetId="7" r:id="rId4"/>
+    <sheet name="license" sheetId="8" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">geographicalCoverage!$A$1:$B$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">kindData!$A$1:$B$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">geographicalCoverage!$A$1:$B$1</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -34,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="650" uniqueCount="538">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="484">
   <si>
     <t>microdata_category</t>
   </si>
@@ -78,39 +76,6 @@
     <t>Esri Credits</t>
   </si>
   <si>
-    <t>Sample survey data</t>
-  </si>
-  <si>
-    <t>Census/enumeration data</t>
-  </si>
-  <si>
-    <t>Administrative records data</t>
-  </si>
-  <si>
-    <t>Aggregate data</t>
-  </si>
-  <si>
-    <t>Clinical data</t>
-  </si>
-  <si>
-    <t>Event/transaction data</t>
-  </si>
-  <si>
-    <t>Observation data/ratings</t>
-  </si>
-  <si>
-    <t>Process-produced data</t>
-  </si>
-  <si>
-    <t>Time budget diaries</t>
-  </si>
-  <si>
-    <t>Time series data</t>
-  </si>
-  <si>
-    <t>Geo-Spatial data</t>
-  </si>
-  <si>
     <t>Bhutan</t>
   </si>
   <si>
@@ -204,123 +169,6 @@
     <t>Cabo Verde</t>
   </si>
   <si>
-    <t>--</t>
-  </si>
-  <si>
-    <t>sample survey data [ssd]</t>
-  </si>
-  <si>
-    <t>sample survey data</t>
-  </si>
-  <si>
-    <t>census/enumeration data [cen]</t>
-  </si>
-  <si>
-    <t>aggregate data [agg]</t>
-  </si>
-  <si>
-    <t>clinical data [cli]</t>
-  </si>
-  <si>
-    <t>process-produced data [pro]</t>
-  </si>
-  <si>
-    <t>observation data/ratings [obs]</t>
-  </si>
-  <si>
-    <t>other</t>
-  </si>
-  <si>
-    <t>administrative records (customs)</t>
-  </si>
-  <si>
-    <t>administrative records data [adm]</t>
-  </si>
-  <si>
-    <t>censos (cen)</t>
-  </si>
-  <si>
-    <t>census/enumeration data</t>
-  </si>
-  <si>
-    <t>dados de inquérito por amostragem [ssd]</t>
-  </si>
-  <si>
-    <t>datos obtenidos por un proceso (pro)</t>
-  </si>
-  <si>
-    <t>données échantillonées [ssd]</t>
-  </si>
-  <si>
-    <t>encuesta  por muestreo (ssd)</t>
-  </si>
-  <si>
-    <t>encuesta por muestreo</t>
-  </si>
-  <si>
-    <t>encuesta por muestreo (no probabilístico)</t>
-  </si>
-  <si>
-    <t>encuesta por muestreo (ssd)</t>
-  </si>
-  <si>
-    <t>encuesta por muestreo (ssd)/datos de una encuesta</t>
-  </si>
-  <si>
-    <t>encuesta probabilística en hogares</t>
-  </si>
-  <si>
-    <t>encuestador muestreo (ssd)</t>
-  </si>
-  <si>
-    <t>encuestapor muestreo (ssd)</t>
-  </si>
-  <si>
-    <t>encuestas por muestreo (ssd)</t>
-  </si>
-  <si>
-    <t>estadística basada en registros administrativos</t>
-  </si>
-  <si>
-    <t>event history data</t>
-  </si>
-  <si>
-    <t>event/transaction data [evn]</t>
-  </si>
-  <si>
-    <t>modelo probabilístico, trietápico de conglomerados; el diseño muestral incluye en las etapas de seleccion aplicadas, las ciudades del área urbana, los sectores urbanos que las conforman y las viviendas existentes en ellos</t>
-  </si>
-  <si>
-    <t>muestreo probabilístico, trietápico de conglomerados, donde las (i) upm corresponden a las ciudades (autorepresentadas y correpresentadas), (ii) usm a los sectores censales, y (iii) utm a las viviendas</t>
-  </si>
-  <si>
-    <t>NA</t>
-  </si>
-  <si>
-    <t>nationally and regionally representative sample survey data (ssd)</t>
-  </si>
-  <si>
-    <t>operación estadística basada en registros administrativos (adm)</t>
-  </si>
-  <si>
-    <t>registros administrativos (adm)</t>
-  </si>
-  <si>
-    <t>sample survey data [ssd], administrative records data [adm], other</t>
-  </si>
-  <si>
-    <t>sample survey data [ssd], air quality measurements</t>
-  </si>
-  <si>
-    <t>survey data</t>
-  </si>
-  <si>
-    <t>verbal autopsy-based cause of death data</t>
-  </si>
-  <si>
-    <t>Sample survey data;Administrative records data</t>
-  </si>
-  <si>
     <t>bhutan</t>
   </si>
   <si>
@@ -1509,9 +1357,6 @@
     <t>Official Use Only</t>
   </si>
   <si>
-    <t>ddh_category_multiple</t>
-  </si>
-  <si>
     <t>Other International Organization</t>
   </si>
   <si>
@@ -1581,18 +1426,12 @@
     <t>Cote d’Ivoire</t>
   </si>
   <si>
-    <t>encuesta probabilística en establecimientos</t>
-  </si>
-  <si>
     <t>viet nam</t>
   </si>
   <si>
     <t>Venezuela, RB</t>
   </si>
   <si>
-    <t>Kind of Data not specified</t>
-  </si>
-  <si>
     <t>egypt</t>
   </si>
   <si>
@@ -1630,9 +1469,6 @@
   </si>
   <si>
     <t>gambia</t>
-  </si>
-  <si>
-    <t>Sample survey data[ssd]</t>
   </si>
   <si>
     <t>Sénégal</t>
@@ -2080,7 +1916,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
@@ -2103,7 +1939,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>490</v>
+        <v>440</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -2143,7 +1979,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>506</v>
+        <v>455</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>5</v>
@@ -2151,7 +1987,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>507</v>
+        <v>456</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>6</v>
@@ -2167,7 +2003,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>508</v>
+        <v>457</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>8</v>
@@ -2175,7 +2011,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>510</v>
+        <v>459</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>9</v>
@@ -2183,7 +2019,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>505</v>
+        <v>454</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>10</v>
@@ -2191,7 +2027,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>509</v>
+        <v>458</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>11</v>
@@ -2216,489 +2052,10 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C44"/>
-  <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="53" customWidth="1"/>
-    <col min="2" max="2" width="32" customWidth="1"/>
-    <col min="3" max="18" width="35" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>59</v>
-      </c>
-      <c r="B4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>60</v>
-      </c>
-      <c r="B5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>63</v>
-      </c>
-      <c r="B6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>64</v>
-      </c>
-      <c r="B10" t="s">
-        <v>518</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>56</v>
-      </c>
-      <c r="B11" t="s">
-        <v>518</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>65</v>
-      </c>
-      <c r="B12" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>66</v>
-      </c>
-      <c r="B13" t="s">
-        <v>16</v>
-      </c>
-      <c r="C13" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>67</v>
-      </c>
-      <c r="B14" t="s">
-        <v>15</v>
-      </c>
-      <c r="C14" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>68</v>
-      </c>
-      <c r="B15" t="s">
-        <v>15</v>
-      </c>
-      <c r="C15" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>61</v>
-      </c>
-      <c r="B16" t="s">
-        <v>18</v>
-      </c>
-      <c r="C16" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>69</v>
-      </c>
-      <c r="B17" t="s">
-        <v>14</v>
-      </c>
-      <c r="C17" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>70</v>
-      </c>
-      <c r="B18" t="s">
-        <v>21</v>
-      </c>
-      <c r="C18" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>71</v>
-      </c>
-      <c r="B19" t="s">
-        <v>14</v>
-      </c>
-      <c r="C19" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>72</v>
-      </c>
-      <c r="B20" t="s">
-        <v>14</v>
-      </c>
-      <c r="C20" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>73</v>
-      </c>
-      <c r="B21" t="s">
-        <v>14</v>
-      </c>
-      <c r="C21" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>74</v>
-      </c>
-      <c r="B22" t="s">
-        <v>14</v>
-      </c>
-      <c r="C22" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>75</v>
-      </c>
-      <c r="B23" t="s">
-        <v>14</v>
-      </c>
-      <c r="C23" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>76</v>
-      </c>
-      <c r="B24" t="s">
-        <v>14</v>
-      </c>
-      <c r="C24" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>77</v>
-      </c>
-      <c r="B25" t="s">
-        <v>14</v>
-      </c>
-      <c r="C25" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>78</v>
-      </c>
-      <c r="B26" t="s">
-        <v>14</v>
-      </c>
-      <c r="C26" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>79</v>
-      </c>
-      <c r="B27" t="s">
-        <v>14</v>
-      </c>
-      <c r="C27" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>80</v>
-      </c>
-      <c r="B28" t="s">
-        <v>14</v>
-      </c>
-      <c r="C28" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>81</v>
-      </c>
-      <c r="B29" t="s">
-        <v>16</v>
-      </c>
-      <c r="C29" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>82</v>
-      </c>
-      <c r="B30" t="s">
-        <v>19</v>
-      </c>
-      <c r="C30" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>83</v>
-      </c>
-      <c r="B31" t="s">
-        <v>19</v>
-      </c>
-      <c r="C31" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>84</v>
-      </c>
-      <c r="B32" t="s">
-        <v>14</v>
-      </c>
-      <c r="C32" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>85</v>
-      </c>
-      <c r="B33" t="s">
-        <v>14</v>
-      </c>
-      <c r="C33" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>86</v>
-      </c>
-      <c r="B34" t="s">
-        <v>518</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>87</v>
-      </c>
-      <c r="B35" t="s">
-        <v>14</v>
-      </c>
-      <c r="C35" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>88</v>
-      </c>
-      <c r="B36" t="s">
-        <v>16</v>
-      </c>
-      <c r="C36" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>62</v>
-      </c>
-      <c r="B37" t="s">
-        <v>21</v>
-      </c>
-      <c r="C37" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>89</v>
-      </c>
-      <c r="B38" t="s">
-        <v>16</v>
-      </c>
-      <c r="C38" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>90</v>
-      </c>
-      <c r="B39" t="s">
-        <v>14</v>
-      </c>
-      <c r="C39" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>91</v>
-      </c>
-      <c r="B40" t="s">
-        <v>14</v>
-      </c>
-      <c r="C40" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>92</v>
-      </c>
-      <c r="B41" t="s">
-        <v>14</v>
-      </c>
-      <c r="C41" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>93</v>
-      </c>
-      <c r="B42" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>515</v>
-      </c>
-      <c r="B43" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>532</v>
-      </c>
-      <c r="B44" t="s">
-        <v>14</v>
-      </c>
-    </row>
-  </sheetData>
-  <autoFilter ref="A1:B1" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B233"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A91" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="J95" sqref="J95"/>
     </sheetView>
@@ -2719,1858 +2076,1858 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>191</v>
+        <v>141</v>
       </c>
       <c r="B2" t="s">
-        <v>379</v>
+        <v>329</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>185</v>
+        <v>135</v>
       </c>
       <c r="B3" t="s">
-        <v>511</v>
+        <v>460</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>278</v>
+        <v>228</v>
       </c>
       <c r="B4" t="s">
-        <v>511</v>
+        <v>460</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>96</v>
+        <v>46</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>247</v>
+        <v>197</v>
       </c>
       <c r="B6" t="s">
-        <v>434</v>
+        <v>384</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>285</v>
+        <v>235</v>
       </c>
       <c r="B7" t="s">
-        <v>470</v>
+        <v>420</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>171</v>
+        <v>121</v>
       </c>
       <c r="B8" t="s">
-        <v>360</v>
+        <v>310</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>299</v>
+        <v>249</v>
       </c>
       <c r="B9" t="s">
-        <v>528</v>
+        <v>475</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>167</v>
+        <v>117</v>
       </c>
       <c r="B10" t="s">
-        <v>356</v>
+        <v>306</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>142</v>
+        <v>92</v>
       </c>
       <c r="B11" t="s">
-        <v>331</v>
+        <v>281</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>133</v>
+        <v>83</v>
       </c>
       <c r="B12" t="s">
-        <v>322</v>
+        <v>272</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>283</v>
+        <v>233</v>
       </c>
       <c r="B13" t="s">
-        <v>468</v>
+        <v>418</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>239</v>
+        <v>189</v>
       </c>
       <c r="B14" t="s">
-        <v>426</v>
+        <v>376</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>240</v>
+        <v>190</v>
       </c>
       <c r="B15" t="s">
-        <v>427</v>
+        <v>377</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>135</v>
+        <v>85</v>
       </c>
       <c r="B16" t="s">
-        <v>324</v>
+        <v>274</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>143</v>
+        <v>93</v>
       </c>
       <c r="B17" t="s">
-        <v>332</v>
+        <v>282</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>242</v>
+        <v>192</v>
       </c>
       <c r="B18" t="s">
-        <v>429</v>
+        <v>379</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>126</v>
+        <v>76</v>
       </c>
       <c r="B19" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>170</v>
+        <v>120</v>
       </c>
       <c r="B20" t="s">
-        <v>359</v>
+        <v>309</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>172</v>
+        <v>122</v>
       </c>
       <c r="B21" t="s">
-        <v>361</v>
+        <v>311</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>241</v>
+        <v>191</v>
       </c>
       <c r="B22" t="s">
-        <v>428</v>
+        <v>378</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>134</v>
+        <v>84</v>
       </c>
       <c r="B23" t="s">
-        <v>323</v>
+        <v>273</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>121</v>
+        <v>71</v>
       </c>
       <c r="B24" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>313</v>
+        <v>263</v>
       </c>
       <c r="B25" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>95</v>
+        <v>45</v>
       </c>
       <c r="B26" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>144</v>
+        <v>94</v>
       </c>
       <c r="B27" t="s">
-        <v>333</v>
+        <v>283</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>178</v>
+        <v>128</v>
       </c>
       <c r="B28" t="s">
-        <v>367</v>
+        <v>317</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>196</v>
+        <v>146</v>
       </c>
       <c r="B29" t="s">
-        <v>384</v>
+        <v>334</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>145</v>
+        <v>95</v>
       </c>
       <c r="B30" t="s">
-        <v>334</v>
+        <v>284</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>302</v>
+        <v>252</v>
       </c>
       <c r="B31" t="s">
-        <v>484</v>
+        <v>434</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>512</v>
+        <v>461</v>
       </c>
       <c r="B32" t="s">
-        <v>512</v>
+        <v>461</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>136</v>
+        <v>86</v>
       </c>
       <c r="B33" t="s">
-        <v>325</v>
+        <v>275</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>198</v>
+        <v>148</v>
       </c>
       <c r="B34" t="s">
-        <v>386</v>
+        <v>336</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>190</v>
+        <v>140</v>
       </c>
       <c r="B35" t="s">
-        <v>378</v>
+        <v>328</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>310</v>
+        <v>260</v>
       </c>
       <c r="B36" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>129</v>
+        <v>79</v>
       </c>
       <c r="B37" t="s">
-        <v>318</v>
+        <v>268</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>228</v>
+        <v>178</v>
       </c>
       <c r="B38" t="s">
-        <v>415</v>
+        <v>365</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>243</v>
+        <v>193</v>
       </c>
       <c r="B39" t="s">
-        <v>430</v>
+        <v>380</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>301</v>
+        <v>251</v>
       </c>
       <c r="B40" t="s">
-        <v>483</v>
+        <v>433</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>232</v>
+        <v>182</v>
       </c>
       <c r="B41" t="s">
-        <v>419</v>
+        <v>369</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>177</v>
+        <v>127</v>
       </c>
       <c r="B42" t="s">
-        <v>366</v>
+        <v>316</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>146</v>
+        <v>96</v>
       </c>
       <c r="B43" t="s">
-        <v>335</v>
+        <v>285</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>225</v>
+        <v>175</v>
       </c>
       <c r="B44" t="s">
-        <v>412</v>
+        <v>362</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>147</v>
+        <v>97</v>
       </c>
       <c r="B45" t="s">
-        <v>336</v>
+        <v>286</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>222</v>
+        <v>172</v>
       </c>
       <c r="B46" t="s">
-        <v>409</v>
+        <v>359</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>235</v>
+        <v>185</v>
       </c>
       <c r="B47" t="s">
-        <v>422</v>
+        <v>372</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>221</v>
+        <v>171</v>
       </c>
       <c r="B48" t="s">
-        <v>408</v>
+        <v>358</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>293</v>
+        <v>243</v>
       </c>
       <c r="B49" t="s">
-        <v>529</v>
+        <v>476</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>148</v>
+        <v>98</v>
       </c>
       <c r="B50" t="s">
-        <v>337</v>
+        <v>287</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>315</v>
+        <v>265</v>
       </c>
       <c r="B51" t="s">
-        <v>397</v>
+        <v>347</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>307</v>
+        <v>257</v>
       </c>
       <c r="B52" t="s">
-        <v>397</v>
+        <v>347</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>210</v>
+        <v>160</v>
       </c>
       <c r="B53" t="s">
-        <v>397</v>
+        <v>347</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>514</v>
+        <v>463</v>
       </c>
       <c r="B54" t="s">
-        <v>397</v>
+        <v>347</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>187</v>
+        <v>137</v>
       </c>
       <c r="B55" t="s">
-        <v>375</v>
+        <v>325</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>281</v>
+        <v>231</v>
       </c>
       <c r="B56" t="s">
-        <v>466</v>
+        <v>416</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>244</v>
+        <v>194</v>
       </c>
       <c r="B57" t="s">
-        <v>431</v>
+        <v>381</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>181</v>
+        <v>131</v>
       </c>
       <c r="B58" t="s">
-        <v>370</v>
+        <v>320</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>246</v>
+        <v>196</v>
       </c>
       <c r="B59" t="s">
-        <v>433</v>
+        <v>383</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>245</v>
+        <v>195</v>
       </c>
       <c r="B60" t="s">
-        <v>432</v>
+        <v>382</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>166</v>
+        <v>116</v>
       </c>
       <c r="B61" t="s">
-        <v>355</v>
+        <v>305</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>149</v>
+        <v>99</v>
       </c>
       <c r="B62" t="s">
-        <v>338</v>
+        <v>288</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>280</v>
+        <v>230</v>
       </c>
       <c r="B63" t="s">
-        <v>465</v>
+        <v>415</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>279</v>
+        <v>229</v>
       </c>
       <c r="B64" t="s">
-        <v>317</v>
+        <v>267</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="B65" t="s">
-        <v>339</v>
+        <v>289</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>230</v>
+        <v>180</v>
       </c>
       <c r="B66" t="s">
-        <v>417</v>
+        <v>367</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>519</v>
+        <v>466</v>
       </c>
       <c r="B67" t="s">
-        <v>417</v>
+        <v>367</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>160</v>
+        <v>110</v>
       </c>
       <c r="B68" t="s">
-        <v>349</v>
+        <v>299</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>234</v>
+        <v>184</v>
       </c>
       <c r="B69" t="s">
-        <v>421</v>
+        <v>371</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>141</v>
+        <v>91</v>
       </c>
       <c r="B70" t="s">
-        <v>330</v>
+        <v>280</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>186</v>
+        <v>136</v>
       </c>
       <c r="B71" t="s">
-        <v>374</v>
+        <v>324</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>125</v>
+        <v>75</v>
       </c>
       <c r="B72" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>123</v>
+        <v>73</v>
       </c>
       <c r="B73" t="s">
-        <v>317</v>
+        <v>267</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>316</v>
+        <v>266</v>
       </c>
       <c r="B74" t="s">
-        <v>317</v>
+        <v>267</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>138</v>
+        <v>88</v>
       </c>
       <c r="B75" t="s">
-        <v>327</v>
+        <v>277</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>249</v>
+        <v>199</v>
       </c>
       <c r="B76" t="s">
-        <v>436</v>
+        <v>386</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>250</v>
+        <v>200</v>
       </c>
       <c r="B77" t="s">
-        <v>437</v>
+        <v>387</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>251</v>
+        <v>201</v>
       </c>
       <c r="B78" t="s">
-        <v>438</v>
+        <v>388</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>127</v>
+        <v>77</v>
       </c>
       <c r="B79" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>531</v>
+        <v>478</v>
       </c>
       <c r="B80" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>182</v>
+        <v>132</v>
       </c>
       <c r="B81" t="s">
-        <v>371</v>
+        <v>321</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>173</v>
+        <v>123</v>
       </c>
       <c r="B82" t="s">
-        <v>362</v>
+        <v>312</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>128</v>
+        <v>78</v>
       </c>
       <c r="B83" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>286</v>
+        <v>236</v>
       </c>
       <c r="B84" t="s">
-        <v>471</v>
+        <v>421</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>253</v>
+        <v>203</v>
       </c>
       <c r="B85" t="s">
-        <v>440</v>
+        <v>390</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>300</v>
+        <v>250</v>
       </c>
       <c r="B86" t="s">
-        <v>482</v>
+        <v>432</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>312</v>
+        <v>262</v>
       </c>
       <c r="B87" t="s">
-        <v>488</v>
+        <v>438</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>151</v>
+        <v>101</v>
       </c>
       <c r="B88" t="s">
-        <v>340</v>
+        <v>290</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>130</v>
+        <v>80</v>
       </c>
       <c r="B89" t="s">
-        <v>319</v>
+        <v>269</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>282</v>
+        <v>232</v>
       </c>
       <c r="B90" t="s">
-        <v>467</v>
+        <v>417</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>152</v>
+        <v>102</v>
       </c>
       <c r="B91" t="s">
-        <v>341</v>
+        <v>291</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>154</v>
+        <v>104</v>
       </c>
       <c r="B92" t="s">
-        <v>343</v>
+        <v>293</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>153</v>
+        <v>103</v>
       </c>
       <c r="B93" t="s">
-        <v>342</v>
+        <v>292</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>254</v>
+        <v>204</v>
       </c>
       <c r="B94" t="s">
-        <v>441</v>
+        <v>391</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>188</v>
+        <v>138</v>
       </c>
       <c r="B95" t="s">
-        <v>376</v>
+        <v>326</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>287</v>
+        <v>237</v>
       </c>
       <c r="B96" t="s">
-        <v>472</v>
+        <v>422</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>184</v>
+        <v>134</v>
       </c>
       <c r="B97" t="s">
-        <v>373</v>
+        <v>323</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>229</v>
+        <v>179</v>
       </c>
       <c r="B98" t="s">
-        <v>416</v>
+        <v>366</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>231</v>
+        <v>181</v>
       </c>
       <c r="B99" t="s">
-        <v>418</v>
+        <v>368</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>233</v>
+        <v>183</v>
       </c>
       <c r="B100" t="s">
-        <v>420</v>
+        <v>370</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>255</v>
+        <v>205</v>
       </c>
       <c r="B101" t="s">
-        <v>442</v>
+        <v>392</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>256</v>
+        <v>206</v>
       </c>
       <c r="B102" t="s">
-        <v>443</v>
+        <v>393</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>257</v>
+        <v>207</v>
       </c>
       <c r="B103" t="s">
-        <v>444</v>
+        <v>394</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>155</v>
+        <v>105</v>
       </c>
       <c r="B104" t="s">
-        <v>344</v>
+        <v>294</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>258</v>
+        <v>208</v>
       </c>
       <c r="B105" t="s">
-        <v>445</v>
+        <v>395</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>163</v>
+        <v>113</v>
       </c>
       <c r="B106" t="s">
-        <v>352</v>
+        <v>302</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>189</v>
+        <v>139</v>
       </c>
       <c r="B107" t="s">
-        <v>377</v>
+        <v>327</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>131</v>
+        <v>81</v>
       </c>
       <c r="B108" t="s">
-        <v>320</v>
+        <v>270</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>537</v>
+        <v>483</v>
       </c>
       <c r="B109" t="s">
-        <v>535</v>
+        <v>481</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>305</v>
+        <v>255</v>
       </c>
       <c r="B110" t="s">
-        <v>485</v>
+        <v>435</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>259</v>
+        <v>209</v>
       </c>
       <c r="B111" t="s">
-        <v>446</v>
+        <v>396</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>175</v>
+        <v>125</v>
       </c>
       <c r="B112" t="s">
-        <v>364</v>
+        <v>314</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>260</v>
+        <v>210</v>
       </c>
       <c r="B113" t="s">
-        <v>447</v>
+        <v>397</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>174</v>
+        <v>124</v>
       </c>
       <c r="B114" t="s">
-        <v>363</v>
+        <v>313</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>111</v>
+        <v>61</v>
       </c>
       <c r="B115" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>284</v>
+        <v>234</v>
       </c>
       <c r="B116" t="s">
-        <v>469</v>
+        <v>419</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>194</v>
+        <v>144</v>
       </c>
       <c r="B117" t="s">
-        <v>382</v>
+        <v>332</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>261</v>
+        <v>211</v>
       </c>
       <c r="B118" t="s">
-        <v>448</v>
+        <v>398</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>193</v>
+        <v>143</v>
       </c>
       <c r="B119" t="s">
-        <v>381</v>
+        <v>331</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>137</v>
+        <v>87</v>
       </c>
       <c r="B120" t="s">
-        <v>326</v>
+        <v>276</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>292</v>
+        <v>242</v>
       </c>
       <c r="B121" t="s">
-        <v>477</v>
+        <v>427</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>288</v>
+        <v>238</v>
       </c>
       <c r="B122" t="s">
-        <v>473</v>
+        <v>423</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>192</v>
+        <v>142</v>
       </c>
       <c r="B123" t="s">
-        <v>380</v>
+        <v>330</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>262</v>
+        <v>212</v>
       </c>
       <c r="B124" t="s">
-        <v>449</v>
+        <v>399</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>195</v>
+        <v>145</v>
       </c>
       <c r="B125" t="s">
-        <v>383</v>
+        <v>333</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>112</v>
+        <v>62</v>
       </c>
       <c r="B126" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>207</v>
+        <v>157</v>
       </c>
       <c r="B127" t="s">
-        <v>394</v>
+        <v>344</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>226</v>
+        <v>176</v>
       </c>
       <c r="B128" t="s">
-        <v>413</v>
+        <v>363</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>209</v>
+        <v>159</v>
       </c>
       <c r="B129" t="s">
-        <v>396</v>
+        <v>346</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>113</v>
+        <v>63</v>
       </c>
       <c r="B130" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>263</v>
+        <v>213</v>
       </c>
       <c r="B131" t="s">
-        <v>450</v>
+        <v>400</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>219</v>
+        <v>169</v>
       </c>
       <c r="B132" t="s">
-        <v>406</v>
+        <v>356</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>218</v>
+        <v>168</v>
       </c>
       <c r="B133" t="s">
-        <v>405</v>
+        <v>355</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>223</v>
+        <v>173</v>
       </c>
       <c r="B134" t="s">
-        <v>410</v>
+        <v>360</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>156</v>
+        <v>106</v>
       </c>
       <c r="B135" t="s">
-        <v>345</v>
+        <v>295</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>294</v>
+        <v>244</v>
       </c>
       <c r="B136" t="s">
-        <v>478</v>
+        <v>428</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>513</v>
+        <v>462</v>
       </c>
       <c r="B137" t="s">
-        <v>478</v>
+        <v>428</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>179</v>
+        <v>129</v>
       </c>
       <c r="B138" t="s">
-        <v>368</v>
+        <v>318</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>309</v>
+        <v>259</v>
       </c>
       <c r="B139" t="s">
-        <v>486</v>
+        <v>436</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>114</v>
+        <v>64</v>
       </c>
       <c r="B140" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>120</v>
+        <v>70</v>
       </c>
       <c r="B141" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>303</v>
+        <v>253</v>
       </c>
       <c r="B142" t="s">
-        <v>520</v>
+        <v>467</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>220</v>
+        <v>170</v>
       </c>
       <c r="B143" t="s">
-        <v>407</v>
+        <v>357</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>115</v>
+        <v>65</v>
       </c>
       <c r="B144" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>224</v>
+        <v>174</v>
       </c>
       <c r="B145" t="s">
-        <v>411</v>
+        <v>361</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>116</v>
+        <v>66</v>
       </c>
       <c r="B146" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>296</v>
+        <v>246</v>
       </c>
       <c r="B147" t="s">
-        <v>479</v>
+        <v>429</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>140</v>
+        <v>90</v>
       </c>
       <c r="B148" t="s">
-        <v>329</v>
+        <v>279</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>264</v>
+        <v>214</v>
       </c>
       <c r="B149" t="s">
-        <v>451</v>
+        <v>401</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>265</v>
+        <v>215</v>
       </c>
       <c r="B150" t="s">
-        <v>452</v>
+        <v>402</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>157</v>
+        <v>107</v>
       </c>
       <c r="B151" t="s">
-        <v>346</v>
+        <v>296</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>98</v>
+        <v>48</v>
       </c>
       <c r="B152" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>208</v>
+        <v>158</v>
       </c>
       <c r="B153" t="s">
-        <v>395</v>
+        <v>345</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>295</v>
+        <v>245</v>
       </c>
       <c r="B154" t="s">
-        <v>530</v>
+        <v>477</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>289</v>
+        <v>239</v>
       </c>
       <c r="B155" t="s">
-        <v>474</v>
+        <v>424</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>266</v>
+        <v>216</v>
       </c>
       <c r="B156" t="s">
-        <v>453</v>
+        <v>403</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>139</v>
+        <v>89</v>
       </c>
       <c r="B157" t="s">
-        <v>328</v>
+        <v>278</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>297</v>
+        <v>247</v>
       </c>
       <c r="B158" t="s">
-        <v>480</v>
+        <v>430</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>158</v>
+        <v>108</v>
       </c>
       <c r="B159" t="s">
-        <v>347</v>
+        <v>297</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>107</v>
+        <v>57</v>
       </c>
       <c r="B160" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>159</v>
+        <v>109</v>
       </c>
       <c r="B161" t="s">
-        <v>348</v>
+        <v>298</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>106</v>
+        <v>56</v>
       </c>
       <c r="B162" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>197</v>
+        <v>147</v>
       </c>
       <c r="B163" t="s">
-        <v>385</v>
+        <v>335</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>176</v>
+        <v>126</v>
       </c>
       <c r="B164" t="s">
-        <v>365</v>
+        <v>315</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>267</v>
+        <v>217</v>
       </c>
       <c r="B165" t="s">
-        <v>454</v>
+        <v>404</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>311</v>
+        <v>261</v>
       </c>
       <c r="B166" t="s">
-        <v>487</v>
+        <v>437</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>268</v>
+        <v>218</v>
       </c>
       <c r="B167" t="s">
-        <v>455</v>
+        <v>405</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>101</v>
+        <v>51</v>
       </c>
       <c r="B168" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>183</v>
+        <v>133</v>
       </c>
       <c r="B169" t="s">
-        <v>372</v>
+        <v>322</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>204</v>
+        <v>154</v>
       </c>
       <c r="B170" t="s">
-        <v>391</v>
+        <v>341</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>103</v>
+        <v>53</v>
       </c>
       <c r="B171" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>205</v>
+        <v>155</v>
       </c>
       <c r="B172" t="s">
-        <v>392</v>
+        <v>342</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>290</v>
+        <v>240</v>
       </c>
       <c r="B173" t="s">
-        <v>475</v>
+        <v>425</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>306</v>
+        <v>256</v>
       </c>
       <c r="B174" t="s">
-        <v>402</v>
+        <v>352</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>215</v>
+        <v>165</v>
       </c>
       <c r="B175" t="s">
-        <v>402</v>
+        <v>352</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>314</v>
+        <v>264</v>
       </c>
       <c r="B176" t="s">
-        <v>402</v>
+        <v>352</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>269</v>
+        <v>219</v>
       </c>
       <c r="B177" t="s">
-        <v>456</v>
+        <v>406</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>104</v>
+        <v>54</v>
       </c>
       <c r="B178" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>533</v>
+        <v>479</v>
       </c>
       <c r="B179" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>534</v>
+        <v>480</v>
       </c>
       <c r="B180" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>119</v>
+        <v>69</v>
       </c>
       <c r="B181" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>118</v>
+        <v>68</v>
       </c>
       <c r="B182" t="s">
-        <v>489</v>
+        <v>439</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>206</v>
+        <v>156</v>
       </c>
       <c r="B183" t="s">
-        <v>393</v>
+        <v>343</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="B184" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>270</v>
+        <v>220</v>
       </c>
       <c r="B185" t="s">
-        <v>457</v>
+        <v>407</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>272</v>
+        <v>222</v>
       </c>
       <c r="B186" t="s">
-        <v>459</v>
+        <v>409</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>273</v>
+        <v>223</v>
       </c>
       <c r="B187" t="s">
-        <v>460</v>
+        <v>410</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>216</v>
+        <v>166</v>
       </c>
       <c r="B188" t="s">
-        <v>403</v>
+        <v>353</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>271</v>
+        <v>221</v>
       </c>
       <c r="B189" t="s">
-        <v>458</v>
+        <v>408</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>110</v>
+        <v>60</v>
       </c>
       <c r="B190" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>214</v>
+        <v>164</v>
       </c>
       <c r="B191" t="s">
-        <v>401</v>
+        <v>351</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>248</v>
+        <v>198</v>
       </c>
       <c r="B192" t="s">
-        <v>435</v>
+        <v>385</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>203</v>
+        <v>153</v>
       </c>
       <c r="B193" t="s">
-        <v>390</v>
+        <v>340</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>169</v>
+        <v>119</v>
       </c>
       <c r="B194" t="s">
-        <v>358</v>
+        <v>308</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>165</v>
+        <v>115</v>
       </c>
       <c r="B195" t="s">
-        <v>354</v>
+        <v>304</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>308</v>
+        <v>258</v>
       </c>
       <c r="B196" t="s">
-        <v>357</v>
+        <v>307</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>168</v>
+        <v>118</v>
       </c>
       <c r="B197" t="s">
-        <v>357</v>
+        <v>307</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>202</v>
+        <v>152</v>
       </c>
       <c r="B198" t="s">
-        <v>389</v>
+        <v>339</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>161</v>
+        <v>111</v>
       </c>
       <c r="B199" t="s">
-        <v>350</v>
+        <v>300</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>201</v>
+        <v>151</v>
       </c>
       <c r="B200" t="s">
-        <v>535</v>
+        <v>481</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>274</v>
+        <v>224</v>
       </c>
       <c r="B201" t="s">
-        <v>461</v>
+        <v>411</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>291</v>
+        <v>241</v>
       </c>
       <c r="B202" t="s">
-        <v>476</v>
+        <v>426</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>275</v>
+        <v>225</v>
       </c>
       <c r="B203" t="s">
-        <v>462</v>
+        <v>412</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>536</v>
+        <v>482</v>
       </c>
       <c r="B204" t="s">
-        <v>463</v>
+        <v>413</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>276</v>
+        <v>226</v>
       </c>
       <c r="B205" t="s">
-        <v>463</v>
+        <v>413</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>108</v>
+        <v>58</v>
       </c>
       <c r="B206" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>97</v>
+        <v>47</v>
       </c>
       <c r="B207" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>132</v>
+        <v>82</v>
       </c>
       <c r="B208" t="s">
-        <v>321</v>
+        <v>271</v>
       </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>236</v>
+        <v>186</v>
       </c>
       <c r="B209" t="s">
-        <v>423</v>
+        <v>373</v>
       </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>212</v>
+        <v>162</v>
       </c>
       <c r="B210" t="s">
-        <v>399</v>
+        <v>349</v>
       </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>200</v>
+        <v>150</v>
       </c>
       <c r="B211" t="s">
-        <v>388</v>
+        <v>338</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>164</v>
+        <v>114</v>
       </c>
       <c r="B212" t="s">
-        <v>353</v>
+        <v>303</v>
       </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>227</v>
+        <v>177</v>
       </c>
       <c r="B213" t="s">
-        <v>414</v>
+        <v>364</v>
       </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>217</v>
+        <v>167</v>
       </c>
       <c r="B214" t="s">
-        <v>404</v>
+        <v>354</v>
       </c>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>211</v>
+        <v>161</v>
       </c>
       <c r="B215" t="s">
-        <v>398</v>
+        <v>348</v>
       </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>298</v>
+        <v>248</v>
       </c>
       <c r="B216" t="s">
-        <v>481</v>
+        <v>431</v>
       </c>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>99</v>
+        <v>49</v>
       </c>
       <c r="B217" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>180</v>
+        <v>130</v>
       </c>
       <c r="B218" t="s">
-        <v>369</v>
+        <v>319</v>
       </c>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>238</v>
+        <v>188</v>
       </c>
       <c r="B219" t="s">
-        <v>425</v>
+        <v>375</v>
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>252</v>
+        <v>202</v>
       </c>
       <c r="B220" t="s">
-        <v>439</v>
+        <v>389</v>
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
-        <v>277</v>
+        <v>227</v>
       </c>
       <c r="B221" t="s">
-        <v>464</v>
+        <v>414</v>
       </c>
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>162</v>
+        <v>112</v>
       </c>
       <c r="B222" t="s">
-        <v>351</v>
+        <v>301</v>
       </c>
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>237</v>
+        <v>187</v>
       </c>
       <c r="B223" t="s">
-        <v>424</v>
+        <v>374</v>
       </c>
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>102</v>
+        <v>52</v>
       </c>
       <c r="B224" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>304</v>
+        <v>254</v>
       </c>
       <c r="B225" t="s">
-        <v>517</v>
+        <v>465</v>
       </c>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>105</v>
+        <v>55</v>
       </c>
       <c r="B226" t="s">
-        <v>517</v>
+        <v>465</v>
       </c>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>516</v>
+        <v>464</v>
       </c>
       <c r="B227" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
-        <v>109</v>
+        <v>59</v>
       </c>
       <c r="B228" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
-        <v>199</v>
+        <v>149</v>
       </c>
       <c r="B229" t="s">
-        <v>387</v>
+        <v>337</v>
       </c>
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
-        <v>124</v>
+        <v>74</v>
       </c>
       <c r="B230" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
-        <v>122</v>
+        <v>72</v>
       </c>
       <c r="B231" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
-        <v>117</v>
+        <v>67</v>
       </c>
       <c r="B232" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
-        <v>213</v>
+        <v>163</v>
       </c>
       <c r="B233" t="s">
-        <v>400</v>
+        <v>350</v>
       </c>
     </row>
   </sheetData>
@@ -4608,7 +3965,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:B15"/>
   <sheetViews>
@@ -4632,90 +3989,90 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>523</v>
+        <v>470</v>
       </c>
       <c r="B2" t="s">
-        <v>522</v>
+        <v>469</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>501</v>
+        <v>450</v>
       </c>
       <c r="B3" t="s">
-        <v>492</v>
+        <v>441</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>502</v>
+        <v>451</v>
       </c>
       <c r="B4" t="s">
-        <v>492</v>
+        <v>441</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>493</v>
+        <v>442</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>494</v>
+        <v>443</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>495</v>
+        <v>444</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>496</v>
+        <v>445</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>497</v>
+        <v>446</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>498</v>
+        <v>447</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>499</v>
+        <v>448</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>500</v>
+        <v>449</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>504</v>
+        <v>453</v>
       </c>
       <c r="B13" t="s">
-        <v>522</v>
+        <v>469</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>521</v>
+        <v>468</v>
       </c>
       <c r="B14" t="s">
-        <v>522</v>
+        <v>469</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>503</v>
+        <v>452</v>
       </c>
       <c r="B15" t="s">
-        <v>522</v>
+        <v>469</v>
       </c>
     </row>
   </sheetData>
@@ -4724,7 +4081,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:B10"/>
   <sheetViews>
@@ -4748,18 +4105,18 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>506</v>
+        <v>455</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>524</v>
+        <v>471</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>507</v>
+        <v>456</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>525</v>
+        <v>472</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -4767,36 +4124,36 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>525</v>
+        <v>472</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>508</v>
+        <v>457</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>525</v>
+        <v>472</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>510</v>
+        <v>459</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>527</v>
+        <v>474</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>505</v>
+        <v>454</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>526</v>
+        <v>473</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>509</v>
+        <v>458</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added North Macedonia to lookup
</commit_message>
<xml_diff>
--- a/data-raw/control_vocab_mapping.xlsx
+++ b/data-raw/control_vocab_mapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WB525812\cmder\Git Repos\mdlibtoddh\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{700C2F1C-0A8E-46E5-9CC9-C33220A58566}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61F794A3-61CD-4459-AD2D-43494CB2CDAA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="10770" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="10770" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dataClassification" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="484">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="485">
   <si>
     <t>microdata_category</t>
   </si>
@@ -1484,6 +1484,9 @@
   </si>
   <si>
     <t>Kingdom of Eswatini</t>
+  </si>
+  <si>
+    <t>North Macedonia</t>
   </si>
 </sst>
 </file>
@@ -1916,7 +1919,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
@@ -2053,17 +2056,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:B233"/>
+  <dimension ref="A1:B234"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A91" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J95" sqref="J95"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A108" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G127" sqref="G127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.5703125" customWidth="1"/>
     <col min="2" max="2" width="41.85546875" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -3060,7 +3064,7 @@
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>145</v>
+        <v>484</v>
       </c>
       <c r="B125" t="s">
         <v>333</v>
@@ -3068,95 +3072,95 @@
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>62</v>
+        <v>145</v>
       </c>
       <c r="B126" t="s">
-        <v>29</v>
+        <v>333</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>157</v>
+        <v>62</v>
       </c>
       <c r="B127" t="s">
-        <v>344</v>
+        <v>29</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>176</v>
+        <v>157</v>
       </c>
       <c r="B128" t="s">
-        <v>363</v>
+        <v>344</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>159</v>
+        <v>176</v>
       </c>
       <c r="B129" t="s">
-        <v>346</v>
+        <v>363</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>63</v>
+        <v>159</v>
       </c>
       <c r="B130" t="s">
-        <v>30</v>
+        <v>346</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>213</v>
+        <v>63</v>
       </c>
       <c r="B131" t="s">
-        <v>400</v>
+        <v>30</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>169</v>
+        <v>213</v>
       </c>
       <c r="B132" t="s">
-        <v>356</v>
+        <v>400</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B133" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="B134" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>106</v>
+        <v>173</v>
       </c>
       <c r="B135" t="s">
-        <v>295</v>
+        <v>360</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>244</v>
+        <v>106</v>
       </c>
       <c r="B136" t="s">
-        <v>428</v>
+        <v>295</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>462</v>
+        <v>244</v>
       </c>
       <c r="B137" t="s">
         <v>428</v>
@@ -3164,303 +3168,303 @@
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>129</v>
+        <v>462</v>
       </c>
       <c r="B138" t="s">
-        <v>318</v>
+        <v>428</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>259</v>
+        <v>129</v>
       </c>
       <c r="B139" t="s">
-        <v>436</v>
+        <v>318</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>64</v>
+        <v>259</v>
       </c>
       <c r="B140" t="s">
-        <v>31</v>
+        <v>436</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B141" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>253</v>
+        <v>70</v>
       </c>
       <c r="B142" t="s">
-        <v>467</v>
+        <v>36</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>170</v>
+        <v>253</v>
       </c>
       <c r="B143" t="s">
-        <v>357</v>
+        <v>467</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>65</v>
+        <v>170</v>
       </c>
       <c r="B144" t="s">
-        <v>32</v>
+        <v>357</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>174</v>
+        <v>65</v>
       </c>
       <c r="B145" t="s">
-        <v>361</v>
+        <v>32</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>66</v>
+        <v>174</v>
       </c>
       <c r="B146" t="s">
-        <v>33</v>
+        <v>361</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>246</v>
+        <v>66</v>
       </c>
       <c r="B147" t="s">
-        <v>429</v>
+        <v>33</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>90</v>
+        <v>246</v>
       </c>
       <c r="B148" t="s">
-        <v>279</v>
+        <v>429</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>214</v>
+        <v>90</v>
       </c>
       <c r="B149" t="s">
-        <v>401</v>
+        <v>279</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B150" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>107</v>
+        <v>215</v>
       </c>
       <c r="B151" t="s">
-        <v>296</v>
+        <v>402</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>48</v>
+        <v>107</v>
       </c>
       <c r="B152" t="s">
-        <v>17</v>
+        <v>296</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>158</v>
+        <v>48</v>
       </c>
       <c r="B153" t="s">
-        <v>345</v>
+        <v>17</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>245</v>
+        <v>158</v>
       </c>
       <c r="B154" t="s">
-        <v>477</v>
+        <v>345</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
       <c r="B155" t="s">
-        <v>424</v>
+        <v>477</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>216</v>
+        <v>239</v>
       </c>
       <c r="B156" t="s">
-        <v>403</v>
+        <v>424</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>89</v>
+        <v>216</v>
       </c>
       <c r="B157" t="s">
-        <v>278</v>
+        <v>403</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>247</v>
+        <v>89</v>
       </c>
       <c r="B158" t="s">
-        <v>430</v>
+        <v>278</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>108</v>
+        <v>247</v>
       </c>
       <c r="B159" t="s">
-        <v>297</v>
+        <v>430</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>57</v>
+        <v>108</v>
       </c>
       <c r="B160" t="s">
-        <v>24</v>
+        <v>297</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>109</v>
+        <v>57</v>
       </c>
       <c r="B161" t="s">
-        <v>298</v>
+        <v>24</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>56</v>
+        <v>109</v>
       </c>
       <c r="B162" t="s">
-        <v>23</v>
+        <v>298</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>147</v>
+        <v>56</v>
       </c>
       <c r="B163" t="s">
-        <v>335</v>
+        <v>23</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>126</v>
+        <v>147</v>
       </c>
       <c r="B164" t="s">
-        <v>315</v>
+        <v>335</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>217</v>
+        <v>126</v>
       </c>
       <c r="B165" t="s">
-        <v>404</v>
+        <v>315</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>261</v>
+        <v>217</v>
       </c>
       <c r="B166" t="s">
-        <v>437</v>
+        <v>404</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>218</v>
+        <v>261</v>
       </c>
       <c r="B167" t="s">
-        <v>405</v>
+        <v>437</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>51</v>
+        <v>218</v>
       </c>
       <c r="B168" t="s">
-        <v>44</v>
+        <v>405</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>133</v>
+        <v>51</v>
       </c>
       <c r="B169" t="s">
-        <v>322</v>
+        <v>44</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>154</v>
+        <v>133</v>
       </c>
       <c r="B170" t="s">
-        <v>341</v>
+        <v>322</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>53</v>
+        <v>154</v>
       </c>
       <c r="B171" t="s">
-        <v>21</v>
+        <v>341</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>155</v>
+        <v>53</v>
       </c>
       <c r="B172" t="s">
-        <v>342</v>
+        <v>21</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>240</v>
+        <v>155</v>
       </c>
       <c r="B173" t="s">
-        <v>425</v>
+        <v>342</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>256</v>
+        <v>240</v>
       </c>
       <c r="B174" t="s">
-        <v>352</v>
+        <v>425</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>165</v>
+        <v>256</v>
       </c>
       <c r="B175" t="s">
         <v>352</v>
@@ -3468,7 +3472,7 @@
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>264</v>
+        <v>165</v>
       </c>
       <c r="B176" t="s">
         <v>352</v>
@@ -3476,23 +3480,23 @@
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>219</v>
+        <v>264</v>
       </c>
       <c r="B177" t="s">
-        <v>406</v>
+        <v>352</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>54</v>
+        <v>219</v>
       </c>
       <c r="B178" t="s">
-        <v>22</v>
+        <v>406</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>479</v>
+        <v>54</v>
       </c>
       <c r="B179" t="s">
         <v>22</v>
@@ -3500,7 +3504,7 @@
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B180" t="s">
         <v>22</v>
@@ -3508,135 +3512,135 @@
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>69</v>
+        <v>480</v>
       </c>
       <c r="B181" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B182" t="s">
-        <v>439</v>
+        <v>35</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>156</v>
+        <v>68</v>
       </c>
       <c r="B183" t="s">
-        <v>343</v>
+        <v>439</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>50</v>
+        <v>156</v>
       </c>
       <c r="B184" t="s">
-        <v>19</v>
+        <v>343</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>220</v>
+        <v>50</v>
       </c>
       <c r="B185" t="s">
-        <v>407</v>
+        <v>19</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B186" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B187" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>166</v>
+        <v>223</v>
       </c>
       <c r="B188" t="s">
-        <v>353</v>
+        <v>410</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>221</v>
+        <v>166</v>
       </c>
       <c r="B189" t="s">
-        <v>408</v>
+        <v>353</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>60</v>
+        <v>221</v>
       </c>
       <c r="B190" t="s">
-        <v>27</v>
+        <v>408</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>164</v>
+        <v>60</v>
       </c>
       <c r="B191" t="s">
-        <v>351</v>
+        <v>27</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>198</v>
+        <v>164</v>
       </c>
       <c r="B192" t="s">
-        <v>385</v>
+        <v>351</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>153</v>
+        <v>198</v>
       </c>
       <c r="B193" t="s">
-        <v>340</v>
+        <v>385</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>119</v>
+        <v>153</v>
       </c>
       <c r="B194" t="s">
-        <v>308</v>
+        <v>340</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="B195" t="s">
-        <v>304</v>
+        <v>308</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>258</v>
+        <v>115</v>
       </c>
       <c r="B196" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>118</v>
+        <v>258</v>
       </c>
       <c r="B197" t="s">
         <v>307</v>
@@ -3644,63 +3648,63 @@
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>152</v>
+        <v>118</v>
       </c>
       <c r="B198" t="s">
-        <v>339</v>
+        <v>307</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>111</v>
+        <v>152</v>
       </c>
       <c r="B199" t="s">
-        <v>300</v>
+        <v>339</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>151</v>
+        <v>111</v>
       </c>
       <c r="B200" t="s">
-        <v>481</v>
+        <v>300</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>224</v>
+        <v>151</v>
       </c>
       <c r="B201" t="s">
-        <v>411</v>
+        <v>481</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>241</v>
+        <v>224</v>
       </c>
       <c r="B202" t="s">
-        <v>426</v>
+        <v>411</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>225</v>
+        <v>241</v>
       </c>
       <c r="B203" t="s">
-        <v>412</v>
+        <v>426</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>482</v>
+        <v>225</v>
       </c>
       <c r="B204" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>226</v>
+        <v>482</v>
       </c>
       <c r="B205" t="s">
         <v>413</v>
@@ -3708,167 +3712,167 @@
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>58</v>
+        <v>226</v>
       </c>
       <c r="B206" t="s">
-        <v>25</v>
+        <v>413</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="B207" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>82</v>
+        <v>47</v>
       </c>
       <c r="B208" t="s">
-        <v>271</v>
+        <v>16</v>
       </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>186</v>
+        <v>82</v>
       </c>
       <c r="B209" t="s">
-        <v>373</v>
+        <v>271</v>
       </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>162</v>
+        <v>186</v>
       </c>
       <c r="B210" t="s">
-        <v>349</v>
+        <v>373</v>
       </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>150</v>
+        <v>162</v>
       </c>
       <c r="B211" t="s">
-        <v>338</v>
+        <v>349</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>114</v>
+        <v>150</v>
       </c>
       <c r="B212" t="s">
-        <v>303</v>
+        <v>338</v>
       </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>177</v>
+        <v>114</v>
       </c>
       <c r="B213" t="s">
-        <v>364</v>
+        <v>303</v>
       </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>167</v>
+        <v>177</v>
       </c>
       <c r="B214" t="s">
-        <v>354</v>
+        <v>364</v>
       </c>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="B215" t="s">
-        <v>348</v>
+        <v>354</v>
       </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>248</v>
+        <v>161</v>
       </c>
       <c r="B216" t="s">
-        <v>431</v>
+        <v>348</v>
       </c>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>49</v>
+        <v>248</v>
       </c>
       <c r="B217" t="s">
-        <v>18</v>
+        <v>431</v>
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>130</v>
+        <v>49</v>
       </c>
       <c r="B218" t="s">
-        <v>319</v>
+        <v>18</v>
       </c>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>188</v>
+        <v>130</v>
       </c>
       <c r="B219" t="s">
-        <v>375</v>
+        <v>319</v>
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>202</v>
+        <v>188</v>
       </c>
       <c r="B220" t="s">
-        <v>389</v>
+        <v>375</v>
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
-        <v>227</v>
+        <v>202</v>
       </c>
       <c r="B221" t="s">
-        <v>414</v>
+        <v>389</v>
       </c>
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>112</v>
+        <v>227</v>
       </c>
       <c r="B222" t="s">
-        <v>301</v>
+        <v>414</v>
       </c>
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>187</v>
+        <v>112</v>
       </c>
       <c r="B223" t="s">
-        <v>374</v>
+        <v>301</v>
       </c>
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>52</v>
+        <v>187</v>
       </c>
       <c r="B224" t="s">
-        <v>20</v>
+        <v>374</v>
       </c>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>254</v>
+        <v>52</v>
       </c>
       <c r="B225" t="s">
-        <v>465</v>
+        <v>20</v>
       </c>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>55</v>
+        <v>254</v>
       </c>
       <c r="B226" t="s">
         <v>465</v>
@@ -3876,15 +3880,15 @@
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>464</v>
+        <v>55</v>
       </c>
       <c r="B227" t="s">
-        <v>26</v>
+        <v>465</v>
       </c>
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
-        <v>59</v>
+        <v>464</v>
       </c>
       <c r="B228" t="s">
         <v>26</v>
@@ -3892,72 +3896,80 @@
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
-        <v>149</v>
+        <v>59</v>
       </c>
       <c r="B229" t="s">
-        <v>337</v>
+        <v>26</v>
       </c>
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
-        <v>74</v>
+        <v>149</v>
       </c>
       <c r="B230" t="s">
-        <v>39</v>
+        <v>337</v>
       </c>
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B231" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="B232" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
+        <v>67</v>
+      </c>
+      <c r="B233" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="234" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A234" t="s">
         <v>163</v>
       </c>
-      <c r="B233" t="s">
+      <c r="B234" t="s">
         <v>350</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:B1" xr:uid="{00000000-0009-0000-0000-000004000000}">
-    <sortState ref="A2:B230">
+    <sortState ref="A2:B231">
       <sortCondition ref="A1"/>
     </sortState>
   </autoFilter>
   <sortState ref="A2:B35">
     <sortCondition ref="A2:A35"/>
   </sortState>
-  <conditionalFormatting sqref="A234:A1048576 A1:A53 A138:A179 A228:A232 A55:A136 A181:A226">
+  <conditionalFormatting sqref="A235:A1048576 A1:A53 A139:A180 A229:A233 A55:A124 A182:A227 A126:A137">
     <cfRule type="duplicateValues" dxfId="6" priority="8"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B233">
+  <conditionalFormatting sqref="B234">
     <cfRule type="duplicateValues" dxfId="5" priority="7"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A233">
+  <conditionalFormatting sqref="A234">
     <cfRule type="duplicateValues" dxfId="4" priority="6"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A137">
+  <conditionalFormatting sqref="A138">
     <cfRule type="duplicateValues" dxfId="3" priority="5"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A227">
+  <conditionalFormatting sqref="A228">
     <cfRule type="duplicateValues" dxfId="2" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A54">
     <cfRule type="duplicateValues" dxfId="1" priority="13"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A180">
+  <conditionalFormatting sqref="A181">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updated lookup for Congo Rep. and Dem Congo Rep.
</commit_message>
<xml_diff>
--- a/data-raw/control_vocab_mapping.xlsx
+++ b/data-raw/control_vocab_mapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WB525812\cmder\Git Repos\mdlibtoddh\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61F794A3-61CD-4459-AD2D-43494CB2CDAA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B021BA4-C867-47A4-9A01-32AA044EB968}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="10770" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="485">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="487">
   <si>
     <t>microdata_category</t>
   </si>
@@ -1487,6 +1487,12 @@
   </si>
   <si>
     <t>North Macedonia</t>
+  </si>
+  <si>
+    <t>Republic of the Congo</t>
+  </si>
+  <si>
+    <t>Democratic Republic of the Congo</t>
   </si>
 </sst>
 </file>
@@ -2056,16 +2062,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:B234"/>
+  <dimension ref="A1:B236"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A108" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G127" sqref="G127"/>
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A48" sqref="A48:XFD48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.5703125" customWidth="1"/>
+    <col min="1" max="1" width="59" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="41.85546875" customWidth="1"/>
     <col min="4" max="4" width="16.42578125" bestFit="1" customWidth="1"/>
   </cols>
@@ -2440,55 +2446,55 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>185</v>
+        <v>485</v>
       </c>
       <c r="B47" t="s">
-        <v>372</v>
+        <v>358</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>171</v>
+        <v>486</v>
       </c>
       <c r="B48" t="s">
-        <v>358</v>
+        <v>372</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>243</v>
+        <v>185</v>
       </c>
       <c r="B49" t="s">
-        <v>476</v>
+        <v>372</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>98</v>
+        <v>171</v>
       </c>
       <c r="B50" t="s">
-        <v>287</v>
+        <v>358</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>265</v>
+        <v>243</v>
       </c>
       <c r="B51" t="s">
-        <v>347</v>
+        <v>476</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>257</v>
+        <v>98</v>
       </c>
       <c r="B52" t="s">
-        <v>347</v>
+        <v>287</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>160</v>
+        <v>265</v>
       </c>
       <c r="B53" t="s">
         <v>347</v>
@@ -2496,7 +2502,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>463</v>
+        <v>257</v>
       </c>
       <c r="B54" t="s">
         <v>347</v>
@@ -2504,983 +2510,983 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>137</v>
+        <v>160</v>
       </c>
       <c r="B55" t="s">
-        <v>325</v>
+        <v>347</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>231</v>
+        <v>463</v>
       </c>
       <c r="B56" t="s">
-        <v>416</v>
+        <v>347</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>194</v>
+        <v>137</v>
       </c>
       <c r="B57" t="s">
-        <v>381</v>
+        <v>325</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>131</v>
+        <v>231</v>
       </c>
       <c r="B58" t="s">
-        <v>320</v>
+        <v>416</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B59" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>195</v>
+        <v>131</v>
       </c>
       <c r="B60" t="s">
-        <v>382</v>
+        <v>320</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>116</v>
+        <v>196</v>
       </c>
       <c r="B61" t="s">
-        <v>305</v>
+        <v>383</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>99</v>
+        <v>195</v>
       </c>
       <c r="B62" t="s">
-        <v>288</v>
+        <v>382</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>230</v>
+        <v>116</v>
       </c>
       <c r="B63" t="s">
-        <v>415</v>
+        <v>305</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>229</v>
+        <v>99</v>
       </c>
       <c r="B64" t="s">
-        <v>267</v>
+        <v>288</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>100</v>
+        <v>230</v>
       </c>
       <c r="B65" t="s">
-        <v>289</v>
+        <v>415</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>180</v>
+        <v>229</v>
       </c>
       <c r="B66" t="s">
-        <v>367</v>
+        <v>267</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>466</v>
+        <v>100</v>
       </c>
       <c r="B67" t="s">
-        <v>367</v>
+        <v>289</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>110</v>
+        <v>180</v>
       </c>
       <c r="B68" t="s">
-        <v>299</v>
+        <v>367</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>184</v>
+        <v>466</v>
       </c>
       <c r="B69" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>91</v>
+        <v>110</v>
       </c>
       <c r="B70" t="s">
-        <v>280</v>
+        <v>299</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>136</v>
+        <v>184</v>
       </c>
       <c r="B71" t="s">
-        <v>324</v>
+        <v>371</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>75</v>
+        <v>91</v>
       </c>
       <c r="B72" t="s">
-        <v>40</v>
+        <v>280</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>73</v>
+        <v>136</v>
       </c>
       <c r="B73" t="s">
-        <v>267</v>
+        <v>324</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>266</v>
+        <v>75</v>
       </c>
       <c r="B74" t="s">
-        <v>267</v>
+        <v>40</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>88</v>
+        <v>73</v>
       </c>
       <c r="B75" t="s">
-        <v>277</v>
+        <v>267</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>199</v>
+        <v>266</v>
       </c>
       <c r="B76" t="s">
-        <v>386</v>
+        <v>267</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>200</v>
+        <v>88</v>
       </c>
       <c r="B77" t="s">
-        <v>387</v>
+        <v>277</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B78" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>77</v>
+        <v>200</v>
       </c>
       <c r="B79" t="s">
-        <v>42</v>
+        <v>387</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>478</v>
+        <v>201</v>
       </c>
       <c r="B80" t="s">
-        <v>42</v>
+        <v>388</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>132</v>
+        <v>77</v>
       </c>
       <c r="B81" t="s">
-        <v>321</v>
+        <v>42</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>123</v>
+        <v>478</v>
       </c>
       <c r="B82" t="s">
-        <v>312</v>
+        <v>42</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>78</v>
+        <v>132</v>
       </c>
       <c r="B83" t="s">
-        <v>43</v>
+        <v>321</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>236</v>
+        <v>123</v>
       </c>
       <c r="B84" t="s">
-        <v>421</v>
+        <v>312</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>203</v>
+        <v>78</v>
       </c>
       <c r="B85" t="s">
-        <v>390</v>
+        <v>43</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>250</v>
+        <v>236</v>
       </c>
       <c r="B86" t="s">
-        <v>432</v>
+        <v>421</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>262</v>
+        <v>203</v>
       </c>
       <c r="B87" t="s">
-        <v>438</v>
+        <v>390</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>101</v>
+        <v>250</v>
       </c>
       <c r="B88" t="s">
-        <v>290</v>
+        <v>432</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>80</v>
+        <v>262</v>
       </c>
       <c r="B89" t="s">
-        <v>269</v>
+        <v>438</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>232</v>
+        <v>101</v>
       </c>
       <c r="B90" t="s">
-        <v>417</v>
+        <v>290</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>102</v>
+        <v>80</v>
       </c>
       <c r="B91" t="s">
-        <v>291</v>
+        <v>269</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>104</v>
+        <v>232</v>
       </c>
       <c r="B92" t="s">
-        <v>293</v>
+        <v>417</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B93" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>204</v>
+        <v>104</v>
       </c>
       <c r="B94" t="s">
-        <v>391</v>
+        <v>293</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>138</v>
+        <v>103</v>
       </c>
       <c r="B95" t="s">
-        <v>326</v>
+        <v>292</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>237</v>
+        <v>204</v>
       </c>
       <c r="B96" t="s">
-        <v>422</v>
+        <v>391</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="B97" t="s">
-        <v>323</v>
+        <v>326</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>179</v>
+        <v>237</v>
       </c>
       <c r="B98" t="s">
-        <v>366</v>
+        <v>422</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>181</v>
+        <v>134</v>
       </c>
       <c r="B99" t="s">
-        <v>368</v>
+        <v>323</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="B100" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>205</v>
+        <v>181</v>
       </c>
       <c r="B101" t="s">
-        <v>392</v>
+        <v>368</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>206</v>
+        <v>183</v>
       </c>
       <c r="B102" t="s">
-        <v>393</v>
+        <v>370</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B103" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>105</v>
+        <v>206</v>
       </c>
       <c r="B104" t="s">
-        <v>294</v>
+        <v>393</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B105" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="B106" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>139</v>
+        <v>208</v>
       </c>
       <c r="B107" t="s">
-        <v>327</v>
+        <v>395</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>81</v>
+        <v>113</v>
       </c>
       <c r="B108" t="s">
-        <v>270</v>
+        <v>302</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>483</v>
+        <v>139</v>
       </c>
       <c r="B109" t="s">
-        <v>481</v>
+        <v>327</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>255</v>
+        <v>81</v>
       </c>
       <c r="B110" t="s">
-        <v>435</v>
+        <v>270</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>209</v>
+        <v>483</v>
       </c>
       <c r="B111" t="s">
-        <v>396</v>
+        <v>481</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>125</v>
+        <v>255</v>
       </c>
       <c r="B112" t="s">
-        <v>314</v>
+        <v>435</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B113" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B114" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>61</v>
+        <v>210</v>
       </c>
       <c r="B115" t="s">
-        <v>28</v>
+        <v>397</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>234</v>
+        <v>124</v>
       </c>
       <c r="B116" t="s">
-        <v>419</v>
+        <v>313</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>144</v>
+        <v>61</v>
       </c>
       <c r="B117" t="s">
-        <v>332</v>
+        <v>28</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>211</v>
+        <v>234</v>
       </c>
       <c r="B118" t="s">
-        <v>398</v>
+        <v>419</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B119" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>87</v>
+        <v>211</v>
       </c>
       <c r="B120" t="s">
-        <v>276</v>
+        <v>398</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>242</v>
+        <v>143</v>
       </c>
       <c r="B121" t="s">
-        <v>427</v>
+        <v>331</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>238</v>
+        <v>87</v>
       </c>
       <c r="B122" t="s">
-        <v>423</v>
+        <v>276</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>142</v>
+        <v>242</v>
       </c>
       <c r="B123" t="s">
-        <v>330</v>
+        <v>427</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>212</v>
+        <v>238</v>
       </c>
       <c r="B124" t="s">
-        <v>399</v>
+        <v>423</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>484</v>
+        <v>142</v>
       </c>
       <c r="B125" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>145</v>
+        <v>212</v>
       </c>
       <c r="B126" t="s">
-        <v>333</v>
+        <v>399</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>62</v>
+        <v>484</v>
       </c>
       <c r="B127" t="s">
-        <v>29</v>
+        <v>333</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="B128" t="s">
-        <v>344</v>
+        <v>333</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>176</v>
+        <v>62</v>
       </c>
       <c r="B129" t="s">
-        <v>363</v>
+        <v>29</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B130" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>63</v>
+        <v>176</v>
       </c>
       <c r="B131" t="s">
-        <v>30</v>
+        <v>363</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>213</v>
+        <v>159</v>
       </c>
       <c r="B132" t="s">
-        <v>400</v>
+        <v>346</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>169</v>
+        <v>63</v>
       </c>
       <c r="B133" t="s">
-        <v>356</v>
+        <v>30</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>168</v>
+        <v>213</v>
       </c>
       <c r="B134" t="s">
-        <v>355</v>
+        <v>400</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="B135" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>106</v>
+        <v>168</v>
       </c>
       <c r="B136" t="s">
-        <v>295</v>
+        <v>355</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>244</v>
+        <v>173</v>
       </c>
       <c r="B137" t="s">
-        <v>428</v>
+        <v>360</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>462</v>
+        <v>106</v>
       </c>
       <c r="B138" t="s">
-        <v>428</v>
+        <v>295</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>129</v>
+        <v>244</v>
       </c>
       <c r="B139" t="s">
-        <v>318</v>
+        <v>428</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>259</v>
+        <v>462</v>
       </c>
       <c r="B140" t="s">
-        <v>436</v>
+        <v>428</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>64</v>
+        <v>129</v>
       </c>
       <c r="B141" t="s">
-        <v>31</v>
+        <v>318</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>70</v>
+        <v>259</v>
       </c>
       <c r="B142" t="s">
-        <v>36</v>
+        <v>436</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>253</v>
+        <v>64</v>
       </c>
       <c r="B143" t="s">
-        <v>467</v>
+        <v>31</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>170</v>
+        <v>70</v>
       </c>
       <c r="B144" t="s">
-        <v>357</v>
+        <v>36</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>65</v>
+        <v>253</v>
       </c>
       <c r="B145" t="s">
-        <v>32</v>
+        <v>467</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="B146" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B147" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>246</v>
+        <v>174</v>
       </c>
       <c r="B148" t="s">
-        <v>429</v>
+        <v>361</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>90</v>
+        <v>66</v>
       </c>
       <c r="B149" t="s">
-        <v>279</v>
+        <v>33</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>214</v>
+        <v>246</v>
       </c>
       <c r="B150" t="s">
-        <v>401</v>
+        <v>429</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>215</v>
+        <v>90</v>
       </c>
       <c r="B151" t="s">
-        <v>402</v>
+        <v>279</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>107</v>
+        <v>214</v>
       </c>
       <c r="B152" t="s">
-        <v>296</v>
+        <v>401</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>48</v>
+        <v>215</v>
       </c>
       <c r="B153" t="s">
-        <v>17</v>
+        <v>402</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>158</v>
+        <v>107</v>
       </c>
       <c r="B154" t="s">
-        <v>345</v>
+        <v>296</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>245</v>
+        <v>48</v>
       </c>
       <c r="B155" t="s">
-        <v>477</v>
+        <v>17</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>239</v>
+        <v>158</v>
       </c>
       <c r="B156" t="s">
-        <v>424</v>
+        <v>345</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>216</v>
+        <v>245</v>
       </c>
       <c r="B157" t="s">
-        <v>403</v>
+        <v>477</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>89</v>
+        <v>239</v>
       </c>
       <c r="B158" t="s">
-        <v>278</v>
+        <v>424</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>247</v>
+        <v>216</v>
       </c>
       <c r="B159" t="s">
-        <v>430</v>
+        <v>403</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>108</v>
+        <v>89</v>
       </c>
       <c r="B160" t="s">
-        <v>297</v>
+        <v>278</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>57</v>
+        <v>247</v>
       </c>
       <c r="B161" t="s">
-        <v>24</v>
+        <v>430</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B162" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B163" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>147</v>
+        <v>109</v>
       </c>
       <c r="B164" t="s">
-        <v>335</v>
+        <v>298</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>126</v>
+        <v>56</v>
       </c>
       <c r="B165" t="s">
-        <v>315</v>
+        <v>23</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>217</v>
+        <v>147</v>
       </c>
       <c r="B166" t="s">
-        <v>404</v>
+        <v>335</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>261</v>
+        <v>126</v>
       </c>
       <c r="B167" t="s">
-        <v>437</v>
+        <v>315</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B168" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>51</v>
+        <v>261</v>
       </c>
       <c r="B169" t="s">
-        <v>44</v>
+        <v>437</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>133</v>
+        <v>218</v>
       </c>
       <c r="B170" t="s">
-        <v>322</v>
+        <v>405</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>154</v>
+        <v>51</v>
       </c>
       <c r="B171" t="s">
-        <v>341</v>
+        <v>44</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>53</v>
+        <v>133</v>
       </c>
       <c r="B172" t="s">
-        <v>21</v>
+        <v>322</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B173" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>240</v>
+        <v>53</v>
       </c>
       <c r="B174" t="s">
-        <v>425</v>
+        <v>21</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>256</v>
+        <v>155</v>
       </c>
       <c r="B175" t="s">
-        <v>352</v>
+        <v>342</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>165</v>
+        <v>240</v>
       </c>
       <c r="B176" t="s">
-        <v>352</v>
+        <v>425</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="B177" t="s">
         <v>352</v>
@@ -3488,31 +3494,31 @@
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>219</v>
+        <v>165</v>
       </c>
       <c r="B178" t="s">
-        <v>406</v>
+        <v>352</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>54</v>
+        <v>264</v>
       </c>
       <c r="B179" t="s">
-        <v>22</v>
+        <v>352</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>479</v>
+        <v>219</v>
       </c>
       <c r="B180" t="s">
-        <v>22</v>
+        <v>406</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>480</v>
+        <v>54</v>
       </c>
       <c r="B181" t="s">
         <v>22</v>
@@ -3520,456 +3526,472 @@
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>69</v>
+        <v>479</v>
       </c>
       <c r="B182" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>68</v>
+        <v>480</v>
       </c>
       <c r="B183" t="s">
-        <v>439</v>
+        <v>22</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>156</v>
+        <v>69</v>
       </c>
       <c r="B184" t="s">
-        <v>343</v>
+        <v>35</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>50</v>
+        <v>68</v>
       </c>
       <c r="B185" t="s">
-        <v>19</v>
+        <v>439</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>220</v>
+        <v>156</v>
       </c>
       <c r="B186" t="s">
-        <v>407</v>
+        <v>343</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>222</v>
+        <v>50</v>
       </c>
       <c r="B187" t="s">
-        <v>409</v>
+        <v>19</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="B188" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>166</v>
+        <v>222</v>
       </c>
       <c r="B189" t="s">
-        <v>353</v>
+        <v>409</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="B190" t="s">
-        <v>408</v>
+        <v>410</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>60</v>
+        <v>166</v>
       </c>
       <c r="B191" t="s">
-        <v>27</v>
+        <v>353</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>164</v>
+        <v>221</v>
       </c>
       <c r="B192" t="s">
-        <v>351</v>
+        <v>408</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>198</v>
+        <v>60</v>
       </c>
       <c r="B193" t="s">
-        <v>385</v>
+        <v>27</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>153</v>
+        <v>164</v>
       </c>
       <c r="B194" t="s">
-        <v>340</v>
+        <v>351</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>119</v>
+        <v>198</v>
       </c>
       <c r="B195" t="s">
-        <v>308</v>
+        <v>385</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>115</v>
+        <v>153</v>
       </c>
       <c r="B196" t="s">
-        <v>304</v>
+        <v>340</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>258</v>
+        <v>119</v>
       </c>
       <c r="B197" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B198" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>152</v>
+        <v>258</v>
       </c>
       <c r="B199" t="s">
-        <v>339</v>
+        <v>307</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="B200" t="s">
-        <v>300</v>
+        <v>307</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B201" t="s">
-        <v>481</v>
+        <v>339</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>224</v>
+        <v>111</v>
       </c>
       <c r="B202" t="s">
-        <v>411</v>
+        <v>300</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>241</v>
+        <v>151</v>
       </c>
       <c r="B203" t="s">
-        <v>426</v>
+        <v>481</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B204" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>482</v>
+        <v>241</v>
       </c>
       <c r="B205" t="s">
-        <v>413</v>
+        <v>426</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B206" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>58</v>
+        <v>482</v>
       </c>
       <c r="B207" t="s">
-        <v>25</v>
+        <v>413</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>47</v>
+        <v>226</v>
       </c>
       <c r="B208" t="s">
-        <v>16</v>
+        <v>413</v>
       </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>82</v>
+        <v>58</v>
       </c>
       <c r="B209" t="s">
-        <v>271</v>
+        <v>25</v>
       </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>186</v>
+        <v>47</v>
       </c>
       <c r="B210" t="s">
-        <v>373</v>
+        <v>16</v>
       </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>162</v>
+        <v>82</v>
       </c>
       <c r="B211" t="s">
-        <v>349</v>
+        <v>271</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>150</v>
+        <v>186</v>
       </c>
       <c r="B212" t="s">
-        <v>338</v>
+        <v>373</v>
       </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>114</v>
+        <v>162</v>
       </c>
       <c r="B213" t="s">
-        <v>303</v>
+        <v>349</v>
       </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>177</v>
+        <v>150</v>
       </c>
       <c r="B214" t="s">
-        <v>364</v>
+        <v>338</v>
       </c>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>167</v>
+        <v>114</v>
       </c>
       <c r="B215" t="s">
-        <v>354</v>
+        <v>303</v>
       </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>161</v>
+        <v>177</v>
       </c>
       <c r="B216" t="s">
-        <v>348</v>
+        <v>364</v>
       </c>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>248</v>
+        <v>167</v>
       </c>
       <c r="B217" t="s">
-        <v>431</v>
+        <v>354</v>
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>49</v>
+        <v>161</v>
       </c>
       <c r="B218" t="s">
-        <v>18</v>
+        <v>348</v>
       </c>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>130</v>
+        <v>248</v>
       </c>
       <c r="B219" t="s">
-        <v>319</v>
+        <v>431</v>
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>188</v>
+        <v>49</v>
       </c>
       <c r="B220" t="s">
-        <v>375</v>
+        <v>18</v>
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
-        <v>202</v>
+        <v>130</v>
       </c>
       <c r="B221" t="s">
-        <v>389</v>
+        <v>319</v>
       </c>
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>227</v>
+        <v>188</v>
       </c>
       <c r="B222" t="s">
-        <v>414</v>
+        <v>375</v>
       </c>
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>112</v>
+        <v>202</v>
       </c>
       <c r="B223" t="s">
-        <v>301</v>
+        <v>389</v>
       </c>
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>187</v>
+        <v>227</v>
       </c>
       <c r="B224" t="s">
-        <v>374</v>
+        <v>414</v>
       </c>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>52</v>
+        <v>112</v>
       </c>
       <c r="B225" t="s">
-        <v>20</v>
+        <v>301</v>
       </c>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>254</v>
+        <v>187</v>
       </c>
       <c r="B226" t="s">
-        <v>465</v>
+        <v>374</v>
       </c>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B227" t="s">
-        <v>465</v>
+        <v>20</v>
       </c>
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
-        <v>464</v>
+        <v>254</v>
       </c>
       <c r="B228" t="s">
-        <v>26</v>
+        <v>465</v>
       </c>
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B229" t="s">
-        <v>26</v>
+        <v>465</v>
       </c>
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
-        <v>149</v>
+        <v>464</v>
       </c>
       <c r="B230" t="s">
-        <v>337</v>
+        <v>26</v>
       </c>
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="B231" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
-        <v>72</v>
+        <v>149</v>
       </c>
       <c r="B232" t="s">
-        <v>38</v>
+        <v>337</v>
       </c>
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="B233" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
+        <v>72</v>
+      </c>
+      <c r="B234" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="235" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A235" t="s">
+        <v>67</v>
+      </c>
+      <c r="B235" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="236" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A236" t="s">
         <v>163</v>
       </c>
-      <c r="B234" t="s">
+      <c r="B236" t="s">
         <v>350</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:B1" xr:uid="{00000000-0009-0000-0000-000004000000}">
-    <sortState ref="A2:B231">
+    <sortState ref="A2:B233">
       <sortCondition ref="A1"/>
     </sortState>
   </autoFilter>
   <sortState ref="A2:B35">
     <sortCondition ref="A2:A35"/>
   </sortState>
-  <conditionalFormatting sqref="A235:A1048576 A1:A53 A139:A180 A229:A233 A55:A124 A182:A227 A126:A137">
+  <conditionalFormatting sqref="A237:A1048576 A1:A55 A141:A182 A231:A235 A57:A126 A184:A229 A128:A139">
     <cfRule type="duplicateValues" dxfId="6" priority="8"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B234">
+  <conditionalFormatting sqref="B236">
     <cfRule type="duplicateValues" dxfId="5" priority="7"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A234">
+  <conditionalFormatting sqref="A236">
     <cfRule type="duplicateValues" dxfId="4" priority="6"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A138">
+  <conditionalFormatting sqref="A140">
     <cfRule type="duplicateValues" dxfId="3" priority="5"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A228">
+  <conditionalFormatting sqref="A230">
     <cfRule type="duplicateValues" dxfId="2" priority="3"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A54">
+  <conditionalFormatting sqref="A56">
     <cfRule type="duplicateValues" dxfId="1" priority="13"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A181">
+  <conditionalFormatting sqref="A183">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
removed terms_of_use as controlled vocab
</commit_message>
<xml_diff>
--- a/data-raw/control_vocab_mapping.xlsx
+++ b/data-raw/control_vocab_mapping.xlsx
@@ -8,18 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WB525812\cmder\Git Repos\mdlibtoddh\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84B8B227-A60C-43F4-86E4-4C57DCF5E80B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEF985AE-C95E-41DD-9C0A-FFFB300EE864}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="10770" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="10770" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dataClassification" sheetId="1" r:id="rId1"/>
-    <sheet name="termsofUse" sheetId="2" r:id="rId2"/>
-    <sheet name="geographicalCoverage" sheetId="5" r:id="rId3"/>
-    <sheet name="license" sheetId="8" r:id="rId4"/>
+    <sheet name="geographicalCoverage" sheetId="5" r:id="rId2"/>
+    <sheet name="license" sheetId="8" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">geographicalCoverage!$A$1:$B$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">geographicalCoverage!$A$1:$B$1</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="471">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="462">
   <si>
     <t>microdata_category</t>
   </si>
@@ -46,33 +45,6 @@
   </si>
   <si>
     <t>Public</t>
-  </si>
-  <si>
-    <t>Open Data Access</t>
-  </si>
-  <si>
-    <t>Direct Access</t>
-  </si>
-  <si>
-    <t>Public Use</t>
-  </si>
-  <si>
-    <t>Licensed Data files</t>
-  </si>
-  <si>
-    <t>Data from External repositories</t>
-  </si>
-  <si>
-    <t>No Access</t>
-  </si>
-  <si>
-    <t>Enclave</t>
-  </si>
-  <si>
-    <t>Restricted Data</t>
-  </si>
-  <si>
-    <t>Esri Credits</t>
   </si>
   <si>
     <t>Bhutan</t>
@@ -1899,7 +1871,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>440</v>
+        <v>431</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1916,106 +1888,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="36.28515625" customWidth="1"/>
-    <col min="2" max="2" width="29.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>442</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>443</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>444</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>446</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>441</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>445</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B236"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A48" sqref="A48:XFD48"/>
     </sheetView>
@@ -2037,1882 +1913,1882 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="B2" t="s">
-        <v>329</v>
+        <v>320</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="B3" t="s">
-        <v>447</v>
+        <v>438</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>228</v>
+        <v>219</v>
       </c>
       <c r="B4" t="s">
-        <v>447</v>
+        <v>438</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="B6" t="s">
-        <v>384</v>
+        <v>375</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="B7" t="s">
-        <v>420</v>
+        <v>411</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="B8" t="s">
-        <v>310</v>
+        <v>301</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>249</v>
+        <v>240</v>
       </c>
       <c r="B9" t="s">
-        <v>459</v>
+        <v>450</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="B10" t="s">
-        <v>306</v>
+        <v>297</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="B11" t="s">
-        <v>281</v>
+        <v>272</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="B12" t="s">
-        <v>272</v>
+        <v>263</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="B13" t="s">
-        <v>418</v>
+        <v>409</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="B14" t="s">
-        <v>376</v>
+        <v>367</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="B15" t="s">
-        <v>377</v>
+        <v>368</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="B16" t="s">
-        <v>274</v>
+        <v>265</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="B17" t="s">
-        <v>282</v>
+        <v>273</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="B18" t="s">
-        <v>379</v>
+        <v>370</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="B19" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="B20" t="s">
-        <v>309</v>
+        <v>300</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="B21" t="s">
-        <v>311</v>
+        <v>302</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="B22" t="s">
-        <v>378</v>
+        <v>369</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="B23" t="s">
-        <v>273</v>
+        <v>264</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="B24" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>263</v>
+        <v>254</v>
       </c>
       <c r="B25" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="B26" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="B27" t="s">
-        <v>283</v>
+        <v>274</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="B28" t="s">
-        <v>317</v>
+        <v>308</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="B29" t="s">
-        <v>334</v>
+        <v>325</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="B30" t="s">
-        <v>284</v>
+        <v>275</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>252</v>
+        <v>243</v>
       </c>
       <c r="B31" t="s">
-        <v>434</v>
+        <v>425</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>448</v>
+        <v>439</v>
       </c>
       <c r="B32" t="s">
-        <v>448</v>
+        <v>439</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="B33" t="s">
-        <v>275</v>
+        <v>266</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="B34" t="s">
-        <v>336</v>
+        <v>327</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="B35" t="s">
-        <v>328</v>
+        <v>319</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>260</v>
+        <v>251</v>
       </c>
       <c r="B36" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="B37" t="s">
-        <v>268</v>
+        <v>259</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="B38" t="s">
-        <v>365</v>
+        <v>356</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="B39" t="s">
-        <v>380</v>
+        <v>371</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>251</v>
+        <v>242</v>
       </c>
       <c r="B40" t="s">
-        <v>433</v>
+        <v>424</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="B41" t="s">
-        <v>369</v>
+        <v>360</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="B42" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="B43" t="s">
-        <v>285</v>
+        <v>276</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="B44" t="s">
-        <v>362</v>
+        <v>353</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="B45" t="s">
-        <v>286</v>
+        <v>277</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="B46" t="s">
-        <v>359</v>
+        <v>350</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>469</v>
+        <v>460</v>
       </c>
       <c r="B47" t="s">
-        <v>358</v>
+        <v>349</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>470</v>
+        <v>461</v>
       </c>
       <c r="B48" t="s">
-        <v>372</v>
+        <v>363</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="B49" t="s">
-        <v>372</v>
+        <v>363</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="B50" t="s">
-        <v>358</v>
+        <v>349</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>243</v>
+        <v>234</v>
       </c>
       <c r="B51" t="s">
-        <v>460</v>
+        <v>451</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="B52" t="s">
-        <v>287</v>
+        <v>278</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>265</v>
+        <v>256</v>
       </c>
       <c r="B53" t="s">
-        <v>347</v>
+        <v>338</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>257</v>
+        <v>248</v>
       </c>
       <c r="B54" t="s">
-        <v>347</v>
+        <v>338</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="B55" t="s">
-        <v>347</v>
+        <v>338</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>450</v>
+        <v>441</v>
       </c>
       <c r="B56" t="s">
-        <v>347</v>
+        <v>338</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="B57" t="s">
-        <v>325</v>
+        <v>316</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>231</v>
+        <v>222</v>
       </c>
       <c r="B58" t="s">
-        <v>416</v>
+        <v>407</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="B59" t="s">
-        <v>381</v>
+        <v>372</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="B60" t="s">
-        <v>320</v>
+        <v>311</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="B61" t="s">
-        <v>383</v>
+        <v>374</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="B62" t="s">
-        <v>382</v>
+        <v>373</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="B63" t="s">
-        <v>305</v>
+        <v>296</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="B64" t="s">
-        <v>288</v>
+        <v>279</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>230</v>
+        <v>221</v>
       </c>
       <c r="B65" t="s">
-        <v>415</v>
+        <v>406</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
       <c r="B66" t="s">
-        <v>267</v>
+        <v>258</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="B67" t="s">
-        <v>289</v>
+        <v>280</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
       <c r="B68" t="s">
-        <v>367</v>
+        <v>358</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>453</v>
+        <v>444</v>
       </c>
       <c r="B69" t="s">
-        <v>367</v>
+        <v>358</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="B70" t="s">
-        <v>299</v>
+        <v>290</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="B71" t="s">
-        <v>371</v>
+        <v>362</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="B72" t="s">
-        <v>280</v>
+        <v>271</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="B73" t="s">
-        <v>324</v>
+        <v>315</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="B74" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="B75" t="s">
-        <v>267</v>
+        <v>258</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>266</v>
+        <v>257</v>
       </c>
       <c r="B76" t="s">
-        <v>267</v>
+        <v>258</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="B77" t="s">
-        <v>277</v>
+        <v>268</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="B78" t="s">
-        <v>386</v>
+        <v>377</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="B79" t="s">
-        <v>387</v>
+        <v>378</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="B80" t="s">
-        <v>388</v>
+        <v>379</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="B81" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>462</v>
+        <v>453</v>
       </c>
       <c r="B82" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="B83" t="s">
-        <v>321</v>
+        <v>312</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="B84" t="s">
-        <v>312</v>
+        <v>303</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="B85" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>236</v>
+        <v>227</v>
       </c>
       <c r="B86" t="s">
-        <v>421</v>
+        <v>412</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
       <c r="B87" t="s">
-        <v>390</v>
+        <v>381</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>250</v>
+        <v>241</v>
       </c>
       <c r="B88" t="s">
-        <v>432</v>
+        <v>423</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>262</v>
+        <v>253</v>
       </c>
       <c r="B89" t="s">
-        <v>438</v>
+        <v>429</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="B90" t="s">
-        <v>290</v>
+        <v>281</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="B91" t="s">
-        <v>269</v>
+        <v>260</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>232</v>
+        <v>223</v>
       </c>
       <c r="B92" t="s">
-        <v>417</v>
+        <v>408</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="B93" t="s">
-        <v>291</v>
+        <v>282</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="B94" t="s">
-        <v>293</v>
+        <v>284</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="B95" t="s">
-        <v>292</v>
+        <v>283</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="B96" t="s">
-        <v>391</v>
+        <v>382</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="B97" t="s">
-        <v>326</v>
+        <v>317</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
       <c r="B98" t="s">
-        <v>422</v>
+        <v>413</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="B99" t="s">
-        <v>323</v>
+        <v>314</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="B100" t="s">
-        <v>366</v>
+        <v>357</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="B101" t="s">
-        <v>368</v>
+        <v>359</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="B102" t="s">
-        <v>370</v>
+        <v>361</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
       <c r="B103" t="s">
-        <v>392</v>
+        <v>383</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="B104" t="s">
-        <v>393</v>
+        <v>384</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
       <c r="B105" t="s">
-        <v>394</v>
+        <v>385</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="B106" t="s">
-        <v>294</v>
+        <v>285</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="B107" t="s">
-        <v>395</v>
+        <v>386</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="B108" t="s">
-        <v>302</v>
+        <v>293</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="B109" t="s">
-        <v>327</v>
+        <v>318</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="B110" t="s">
-        <v>270</v>
+        <v>261</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>467</v>
+        <v>458</v>
       </c>
       <c r="B111" t="s">
-        <v>465</v>
+        <v>456</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>255</v>
+        <v>246</v>
       </c>
       <c r="B112" t="s">
-        <v>435</v>
+        <v>426</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="B113" t="s">
-        <v>396</v>
+        <v>387</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="B114" t="s">
-        <v>314</v>
+        <v>305</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
       <c r="B115" t="s">
-        <v>397</v>
+        <v>388</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="B116" t="s">
-        <v>313</v>
+        <v>304</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="B117" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
       <c r="B118" t="s">
-        <v>419</v>
+        <v>410</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="B119" t="s">
-        <v>332</v>
+        <v>323</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="B120" t="s">
-        <v>398</v>
+        <v>389</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="B121" t="s">
-        <v>331</v>
+        <v>322</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="B122" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>242</v>
+        <v>233</v>
       </c>
       <c r="B123" t="s">
-        <v>427</v>
+        <v>418</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>238</v>
+        <v>229</v>
       </c>
       <c r="B124" t="s">
-        <v>423</v>
+        <v>414</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="B125" t="s">
-        <v>330</v>
+        <v>321</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="B126" t="s">
-        <v>399</v>
+        <v>390</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>468</v>
+        <v>459</v>
       </c>
       <c r="B127" t="s">
-        <v>333</v>
+        <v>324</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="B128" t="s">
-        <v>333</v>
+        <v>324</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="B129" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="B130" t="s">
-        <v>344</v>
+        <v>335</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="B131" t="s">
-        <v>363</v>
+        <v>354</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="B132" t="s">
-        <v>346</v>
+        <v>337</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="B133" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
       <c r="B134" t="s">
-        <v>400</v>
+        <v>391</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="B135" t="s">
-        <v>356</v>
+        <v>347</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="B136" t="s">
-        <v>355</v>
+        <v>346</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="B137" t="s">
-        <v>360</v>
+        <v>351</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="B138" t="s">
-        <v>295</v>
+        <v>286</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>244</v>
+        <v>235</v>
       </c>
       <c r="B139" t="s">
-        <v>428</v>
+        <v>419</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>449</v>
+        <v>440</v>
       </c>
       <c r="B140" t="s">
-        <v>428</v>
+        <v>419</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="B141" t="s">
-        <v>318</v>
+        <v>309</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>259</v>
+        <v>250</v>
       </c>
       <c r="B142" t="s">
-        <v>436</v>
+        <v>427</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="B143" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="B144" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>253</v>
+        <v>244</v>
       </c>
       <c r="B145" t="s">
-        <v>454</v>
+        <v>445</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="B146" t="s">
-        <v>357</v>
+        <v>348</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="B147" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="B148" t="s">
-        <v>361</v>
+        <v>352</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="B149" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>246</v>
+        <v>237</v>
       </c>
       <c r="B150" t="s">
-        <v>429</v>
+        <v>420</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="B151" t="s">
-        <v>279</v>
+        <v>270</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="B152" t="s">
-        <v>401</v>
+        <v>392</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="B153" t="s">
-        <v>402</v>
+        <v>393</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="B154" t="s">
-        <v>296</v>
+        <v>287</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="B155" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="B156" t="s">
-        <v>345</v>
+        <v>336</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>245</v>
+        <v>236</v>
       </c>
       <c r="B157" t="s">
-        <v>461</v>
+        <v>452</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>239</v>
+        <v>230</v>
       </c>
       <c r="B158" t="s">
-        <v>424</v>
+        <v>415</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
       <c r="B159" t="s">
-        <v>403</v>
+        <v>394</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="B160" t="s">
-        <v>278</v>
+        <v>269</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>247</v>
+        <v>238</v>
       </c>
       <c r="B161" t="s">
-        <v>430</v>
+        <v>421</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="B162" t="s">
-        <v>297</v>
+        <v>288</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="B163" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="B164" t="s">
-        <v>298</v>
+        <v>289</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="B165" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="B166" t="s">
-        <v>335</v>
+        <v>326</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="B167" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
       <c r="B168" t="s">
-        <v>404</v>
+        <v>395</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>261</v>
+        <v>252</v>
       </c>
       <c r="B169" t="s">
-        <v>437</v>
+        <v>428</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="B170" t="s">
-        <v>405</v>
+        <v>396</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="B171" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="B172" t="s">
-        <v>322</v>
+        <v>313</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="B173" t="s">
-        <v>341</v>
+        <v>332</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="B174" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="B175" t="s">
-        <v>342</v>
+        <v>333</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>240</v>
+        <v>231</v>
       </c>
       <c r="B176" t="s">
-        <v>425</v>
+        <v>416</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>256</v>
+        <v>247</v>
       </c>
       <c r="B177" t="s">
-        <v>352</v>
+        <v>343</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="B178" t="s">
-        <v>352</v>
+        <v>343</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>264</v>
+        <v>255</v>
       </c>
       <c r="B179" t="s">
-        <v>352</v>
+        <v>343</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="B180" t="s">
-        <v>406</v>
+        <v>397</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="B181" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>463</v>
+        <v>454</v>
       </c>
       <c r="B182" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>464</v>
+        <v>455</v>
       </c>
       <c r="B183" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="B184" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="B185" t="s">
-        <v>439</v>
+        <v>430</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="B186" t="s">
-        <v>343</v>
+        <v>334</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="B187" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="B188" t="s">
-        <v>407</v>
+        <v>398</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="B189" t="s">
-        <v>409</v>
+        <v>400</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="B190" t="s">
-        <v>410</v>
+        <v>401</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="B191" t="s">
-        <v>353</v>
+        <v>344</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="B192" t="s">
-        <v>408</v>
+        <v>399</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="B193" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="B194" t="s">
-        <v>351</v>
+        <v>342</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="B195" t="s">
-        <v>385</v>
+        <v>376</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="B196" t="s">
-        <v>340</v>
+        <v>331</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="B197" t="s">
-        <v>308</v>
+        <v>299</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="B198" t="s">
-        <v>304</v>
+        <v>295</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>258</v>
+        <v>249</v>
       </c>
       <c r="B199" t="s">
-        <v>307</v>
+        <v>298</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="B200" t="s">
-        <v>307</v>
+        <v>298</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="B201" t="s">
-        <v>339</v>
+        <v>330</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="B202" t="s">
-        <v>300</v>
+        <v>291</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="B203" t="s">
-        <v>465</v>
+        <v>456</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="B204" t="s">
-        <v>411</v>
+        <v>402</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>241</v>
+        <v>232</v>
       </c>
       <c r="B205" t="s">
-        <v>426</v>
+        <v>417</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="B206" t="s">
-        <v>412</v>
+        <v>403</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>466</v>
+        <v>457</v>
       </c>
       <c r="B207" t="s">
-        <v>413</v>
+        <v>404</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="B208" t="s">
-        <v>413</v>
+        <v>404</v>
       </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="B209" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="B210" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="B211" t="s">
-        <v>271</v>
+        <v>262</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="B212" t="s">
-        <v>373</v>
+        <v>364</v>
       </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="B213" t="s">
-        <v>349</v>
+        <v>340</v>
       </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B214" t="s">
-        <v>338</v>
+        <v>329</v>
       </c>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="B215" t="s">
-        <v>303</v>
+        <v>294</v>
       </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="B216" t="s">
-        <v>364</v>
+        <v>355</v>
       </c>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="B217" t="s">
-        <v>354</v>
+        <v>345</v>
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="B218" t="s">
-        <v>348</v>
+        <v>339</v>
       </c>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
       <c r="B219" t="s">
-        <v>431</v>
+        <v>422</v>
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="B220" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="B221" t="s">
-        <v>319</v>
+        <v>310</v>
       </c>
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="B222" t="s">
-        <v>375</v>
+        <v>366</v>
       </c>
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="B223" t="s">
-        <v>389</v>
+        <v>380</v>
       </c>
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="B224" t="s">
-        <v>414</v>
+        <v>405</v>
       </c>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="B225" t="s">
-        <v>301</v>
+        <v>292</v>
       </c>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="B226" t="s">
-        <v>374</v>
+        <v>365</v>
       </c>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="B227" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
-        <v>254</v>
+        <v>245</v>
       </c>
       <c r="B228" t="s">
-        <v>452</v>
+        <v>443</v>
       </c>
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="B229" t="s">
-        <v>452</v>
+        <v>443</v>
       </c>
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
-        <v>451</v>
+        <v>442</v>
       </c>
       <c r="B230" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="B231" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="B232" t="s">
-        <v>337</v>
+        <v>328</v>
       </c>
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="B233" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="B234" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="B235" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="B236" t="s">
-        <v>350</v>
+        <v>341</v>
       </c>
     </row>
   </sheetData>
@@ -3950,11 +3826,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -3974,18 +3850,18 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>442</v>
+        <v>433</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>455</v>
+        <v>446</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>443</v>
+        <v>434</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>456</v>
+        <v>447</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -3993,36 +3869,36 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>456</v>
+        <v>447</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>444</v>
+        <v>435</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>456</v>
+        <v>447</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>446</v>
+        <v>437</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>458</v>
+        <v>449</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>441</v>
+        <v>432</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>457</v>
+        <v>448</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>445</v>
+        <v>436</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>